<commit_message>
Ajustar planilhas - BASIS-246701
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/reports/planilhas/modelo3-anac.xlsx
+++ b/backend/src/main/resources/reports/planilhas/modelo3-anac.xlsx
@@ -683,7 +683,7 @@
     <numFmt numFmtId="171" formatCode="0.00"/>
     <numFmt numFmtId="172" formatCode="0"/>
   </numFmts>
-  <fonts count="54">
+  <fonts count="53">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1052,12 +1052,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1224,7 +1218,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="173">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1917,14 +1911,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="53" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="53" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1935,7 +1921,37 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="265">
+  <dxfs count="269">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -3512,16 +3528,6 @@
         <color rgb="FF0066FF"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -3587,6 +3593,56 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304560</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>6120</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="0" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7999920" cy="6355800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
@@ -3601,15 +3657,15 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="9.09"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3624,7 +3680,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3639,7 +3695,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="17.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -3654,7 +3710,7 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
@@ -3688,7 +3744,7 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
@@ -3701,7 +3757,7 @@
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
@@ -3714,7 +3770,7 @@
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="11"/>
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
@@ -3727,7 +3783,7 @@
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="11"/>
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
@@ -3740,7 +3796,7 @@
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
       <c r="D10" s="11"/>
@@ -3753,7 +3809,7 @@
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -3766,7 +3822,7 @@
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="13"/>
@@ -3779,7 +3835,7 @@
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="13"/>
@@ -3792,7 +3848,7 @@
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="13"/>
@@ -3805,7 +3861,7 @@
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="D15" s="13"/>
@@ -3818,7 +3874,7 @@
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="13"/>
@@ -3831,7 +3887,7 @@
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="14" t="s">
         <v>7</v>
       </c>
@@ -3904,22 +3960,22 @@
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="15" width="1.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="15" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="15" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="15" width="1.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="6.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="20.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="9.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="15" width="3.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="15" width="6.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="15" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="15" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="15" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="15" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="15" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="15" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="15" width="10.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="15" width="9.09"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3973,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="21" t="str">
         <f aca="false">IF(OR(ISBLANK(D13),D13=0),"Aguardando Aferição da Fábrica de Software",IF(OR(ISBLANK(D20),D20=0),"Aguardando Aferição da Fábrica de Métricas",IF(OR(AND(D24&gt;=0,D24&lt;=H3),AND(D24&lt;=0,D24&gt;=H4)),"Contagem Aprovada","Contagem em Divergência")))</f>
         <v>Aguardando Aferição da Fábrica de Software</v>
@@ -3987,7 +4043,7 @@
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="22" t="s">
         <v>12</v>
       </c>
@@ -4117,7 +4173,7 @@
       <c r="I14" s="32"/>
       <c r="J14" s="33"/>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="34"/>
@@ -4128,7 +4184,7 @@
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
         <v>23</v>
       </c>
@@ -4217,7 +4273,7 @@
       <c r="I21" s="32"/>
       <c r="J21" s="30"/>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
@@ -4228,7 +4284,7 @@
       <c r="I22" s="34"/>
       <c r="J22" s="34"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
         <v>25</v>
       </c>
@@ -4463,7 +4519,7 @@
       <c r="I36" s="47"/>
       <c r="J36" s="47"/>
     </row>
-    <row r="37" s="53" customFormat="true" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="53" customFormat="true" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="54" t="str">
         <f aca="false">CONCATENATE(B16," = ",D20," PF")</f>
         <v>Contagem Fábrica de Métricas = 0 PF</v>
@@ -4477,7 +4533,7 @@
       <c r="I37" s="54"/>
       <c r="J37" s="54"/>
     </row>
-    <row r="38" s="53" customFormat="true" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" s="53" customFormat="true" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="54" t="str">
         <f aca="false">CONCATENATE(E20,":",H20," PF")</f>
         <v>:0 PF</v>
@@ -4491,10 +4547,10 @@
       <c r="I38" s="54"/>
       <c r="J38" s="54"/>
     </row>
-    <row r="39" s="53" customFormat="true" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" s="53" customFormat="true" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="54" t="str">
         <f aca="false">CONCATENATE(B24,":",D24*100,"%")</f>
-        <v>% de Divergência:0%</v>
+        <v>    % de Divergência:0%</v>
       </c>
       <c r="C39" s="54"/>
       <c r="D39" s="54"/>
@@ -4505,7 +4561,7 @@
       <c r="I39" s="54"/>
       <c r="J39" s="54"/>
     </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="55"/>
       <c r="C40" s="55"/>
       <c r="D40" s="55"/>
@@ -4516,7 +4572,7 @@
       <c r="I40" s="55"/>
       <c r="J40" s="56"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="22" t="s">
         <v>51</v>
       </c>
@@ -4540,7 +4596,7 @@
       <c r="I42" s="57"/>
       <c r="J42" s="58"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
         <v>52</v>
       </c>
@@ -4564,7 +4620,7 @@
       <c r="I44" s="57"/>
       <c r="J44" s="59"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="22" t="s">
         <v>53</v>
       </c>
@@ -4588,7 +4644,7 @@
       <c r="I46" s="57"/>
       <c r="J46" s="58"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="22" t="s">
         <v>54</v>
       </c>
@@ -4612,7 +4668,7 @@
       <c r="I48" s="57"/>
       <c r="J48" s="58"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
         <v>55</v>
       </c>
@@ -4664,7 +4720,7 @@
       <c r="I52" s="62"/>
       <c r="J52" s="62"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
         <v>59</v>
       </c>
@@ -4688,7 +4744,7 @@
       <c r="I54" s="57"/>
       <c r="J54" s="58"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="22" t="s">
         <v>60</v>
       </c>
@@ -4823,26 +4879,26 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="64" width="16.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="64" width="16.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="65" width="59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="66" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="67" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="66" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="68" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="68" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="8" style="64" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="69" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="70" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="71" width="135.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="71" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="69" width="12.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="69" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="248" min="15" style="64" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="250" min="249" style="64" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="251" min="251" style="64" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1025" min="252" style="64" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="66" width="5.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="67" width="5.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="66" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="68" width="9.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="68" width="17.45"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="8" style="64" width="16.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="69" width="10.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="70" width="13.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="71" width="135.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="71" width="12.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="69" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="69" width="9.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="248" min="15" style="64" width="9.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="250" min="249" style="64" width="7.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="251" min="251" style="64" width="15.09"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1025" min="252" style="64" width="9.09"/>
   </cols>
   <sheetData>
     <row r="1" s="78" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4895,7 +4951,7 @@
       <c r="M2" s="87"/>
       <c r="N2" s="87"/>
     </row>
-    <row r="3" s="101" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="101" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="89"/>
       <c r="B3" s="90" t="str">
         <f aca="false">IF(A3="","",IF(Resumo!$D$7="CAST",VLOOKUP(A3,lista!#ref!,2,0),VLOOKUP(A3,lista!#ref!,2,0)))</f>
@@ -4925,7 +4981,7 @@
       <c r="M3" s="100"/>
       <c r="N3" s="69"/>
     </row>
-    <row r="4" s="101" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="101" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="89"/>
       <c r="B4" s="90" t="str">
         <f aca="false">IF(A4="","",IF(Resumo!$D$7="CAST",VLOOKUP(A4,lista!#ref!,2,0),VLOOKUP(A4,lista!#ref!,2,0)))</f>
@@ -4955,7 +5011,7 @@
       <c r="M4" s="100"/>
       <c r="N4" s="69"/>
     </row>
-    <row r="5" s="101" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="101" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="89"/>
       <c r="B5" s="90" t="str">
         <f aca="false">IF(A5="","",IF(Resumo!$D$7="CAST",VLOOKUP(A5,lista!#ref!,2,0),VLOOKUP(A5,lista!#ref!,2,0)))</f>
@@ -4985,7 +5041,7 @@
       <c r="M5" s="100"/>
       <c r="N5" s="69"/>
     </row>
-    <row r="6" s="101" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="101" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="89"/>
       <c r="B6" s="90" t="str">
         <f aca="false">IF(A6="","",IF(Resumo!$D$7="CAST",VLOOKUP(A6,lista!#ref!,2,0),VLOOKUP(A6,lista!#ref!,2,0)))</f>
@@ -5015,7 +5071,7 @@
       <c r="M6" s="100"/>
       <c r="N6" s="69"/>
     </row>
-    <row r="7" s="101" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="101" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="89"/>
       <c r="B7" s="90" t="str">
         <f aca="false">IF(A7="","",IF(Resumo!$D$7="CAST",VLOOKUP(A7,lista!#ref!,2,0),VLOOKUP(A7,lista!#ref!,2,0)))</f>
@@ -5045,7 +5101,7 @@
       <c r="M7" s="69"/>
       <c r="N7" s="69"/>
     </row>
-    <row r="8" s="101" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="101" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="89"/>
       <c r="B8" s="90" t="str">
         <f aca="false">IF(A8="","",IF(Resumo!$D$7="CAST",VLOOKUP(A8,lista!#ref!,2,0),VLOOKUP(A8,lista!#ref!,2,0)))</f>
@@ -5075,7 +5131,7 @@
       <c r="M8" s="69"/>
       <c r="N8" s="69"/>
     </row>
-    <row r="9" s="101" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="101" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="89"/>
       <c r="B9" s="90" t="str">
         <f aca="false">IF(A9="","",IF(Resumo!$D$7="CAST",VLOOKUP(A9,lista!#ref!,2,0),VLOOKUP(A9,lista!#ref!,2,0)))</f>
@@ -5105,7 +5161,7 @@
       <c r="M9" s="69"/>
       <c r="N9" s="69"/>
     </row>
-    <row r="10" s="101" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="101" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="89"/>
       <c r="B10" s="90" t="str">
         <f aca="false">IF(A10="","",IF(Resumo!$D$7="CAST",VLOOKUP(A10,lista!#ref!,2,0),VLOOKUP(A10,lista!#ref!,2,0)))</f>
@@ -5135,7 +5191,7 @@
       <c r="M10" s="100"/>
       <c r="N10" s="69"/>
     </row>
-    <row r="11" s="101" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="101" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="89"/>
       <c r="B11" s="90" t="str">
         <f aca="false">IF(A11="","",IF(Resumo!$D$7="CAST",VLOOKUP(A11,lista!#ref!,2,0),VLOOKUP(A11,lista!#ref!,2,0)))</f>
@@ -5165,7 +5221,7 @@
       <c r="M11" s="100"/>
       <c r="N11" s="69"/>
     </row>
-    <row r="12" s="101" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="101" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="89"/>
       <c r="B12" s="90" t="str">
         <f aca="false">IF(A12="","",IF(Resumo!$D$7="CAST",VLOOKUP(A12,lista!#ref!,2,0),VLOOKUP(A12,lista!#ref!,2,0)))</f>
@@ -5195,7 +5251,7 @@
       <c r="M12" s="69"/>
       <c r="N12" s="69"/>
     </row>
-    <row r="13" s="101" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="101" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="89"/>
       <c r="B13" s="90" t="str">
         <f aca="false">IF(A13="","",IF(Resumo!$D$7="CAST",VLOOKUP(A13,lista!#ref!,2,0),VLOOKUP(A13,lista!#ref!,2,0)))</f>
@@ -5225,7 +5281,7 @@
       <c r="M13" s="69"/>
       <c r="N13" s="69"/>
     </row>
-    <row r="14" s="101" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="101" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="89"/>
       <c r="B14" s="90" t="str">
         <f aca="false">IF(A14="","",IF(Resumo!$D$7="CAST",VLOOKUP(A14,lista!#ref!,2,0),VLOOKUP(A14,lista!#ref!,2,0)))</f>
@@ -5255,7 +5311,7 @@
       <c r="M14" s="69"/>
       <c r="N14" s="69"/>
     </row>
-    <row r="15" s="101" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="101" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="89"/>
       <c r="B15" s="90" t="str">
         <f aca="false">IF(A15="","",IF(Resumo!$D$7="CAST",VLOOKUP(A15,lista!#ref!,2,0),VLOOKUP(A15,lista!#ref!,2,0)))</f>
@@ -5285,7 +5341,7 @@
       <c r="M15" s="69"/>
       <c r="N15" s="69"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="105" t="s">
         <v>67</v>
       </c>
@@ -5294,43 +5350,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="107"/>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="108" t="str">
         <f aca="false">Resumo!D27</f>
         <v>Philipe Dias de Alencar</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="109" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="107"/>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="108" t="n">
         <f aca="false">Resumo!D28</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="109" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="110"/>
     </row>
-    <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="111" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="109" t="s">
         <v>70</v>
       </c>
@@ -5356,7 +5412,8 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -5375,40 +5432,40 @@
       <selection pane="bottomRight" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="112" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="112" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="112" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="112" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="112" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="112" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="112" width="12.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="112" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="112" width="30.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="112" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="112" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="112" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="112" width="12.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="112" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="112" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="112" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="113" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="113" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="113" width="7.28"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="113" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="14" style="113" width="9.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="114" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="115" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="116" width="1.43"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="113" width="10.09"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="113" width="7.27"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="113" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="14" style="113" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="114" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="115" width="30.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="116" width="1.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="117" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="112" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="112" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="112" width="4.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="112" width="4.85"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="26" min="26" style="113" width="8.28"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="27" style="113" width="9.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="112" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="112" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="112" width="4.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="112" width="4.82"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="26" min="26" style="113" width="8.27"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="27" style="113" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="28" style="113" width="4"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="113" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="113" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="31" style="118" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="113" width="5.27"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="113" width="4.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="31" style="118" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="119" width="34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="116" width="1.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="116" width="1.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="119" width="34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="38" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="38" style="0" width="9.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5457,7 +5514,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" s="127" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="127" customFormat="true" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="124" t="s">
         <v>75</v>
       </c>
@@ -23762,7 +23819,7 @@
       <c r="AJ202" s="139"/>
       <c r="AK202" s="139"/>
     </row>
-    <row r="203" s="146" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" s="146" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B203" s="128"/>
       <c r="C203" s="147"/>
       <c r="D203" s="147"/>
@@ -23817,975 +23874,975 @@
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3:Y4">
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:X3 U6:X6 X7 U9:X12 W8:X8">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A9">
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B106:B202 B4:B88 B92:B102">
-    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>ISBLANK($T4)</formula>
     </cfRule>
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>$T4="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
       <formula>$K4&lt;&gt;$AA4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R88 R92:R97">
-    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
+    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
       <formula>ISBLANK($R3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
+    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
       <formula>$R3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
       <formula>$I3&lt;&gt;$Y3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH3:AH98">
-    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
+    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
       <formula>ISBLANK($R3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
+    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
       <formula>$R3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
       <formula>$I3&lt;&gt;$Y3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3:AJ97">
-    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
       <formula>ISBLANK($R3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
       <formula>$R3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
       <formula>$I3&lt;&gt;$Y3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK23 AK25 AK5 AK28:AK91">
-    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
+    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
       <formula>ISBLANK($R5)</formula>
     </cfRule>
-    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
+    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
       <formula>$R5="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
+    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
       <formula>$I5&lt;&gt;$Y5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98 G98 E98">
-    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
+    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
+    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98">
-    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
+    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
+    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H98">
-    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
+    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98 D100:D101">
-    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
+    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:E99 G99">
-    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
+    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
+    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
+    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B99">
-    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
+    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
+    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H99">
-    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
+    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
+    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R98">
-    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
+    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57">
       <formula>ISBLANK($R98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58">
       <formula>$R98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
       <formula>$I98&lt;&gt;$Y98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F92:F101">
-    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
       <formula>ISBLANK($T92)</formula>
     </cfRule>
-    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57">
+    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
       <formula>$T92="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58">
+    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
       <formula>$K92&lt;&gt;$AA92</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105 E105 G105:H105">
-    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
+    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
       <formula>ISBLANK($T105)</formula>
     </cfRule>
-    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
+    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
       <formula>$T105="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
+    <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
       <formula>$K105&lt;&gt;$AA105</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B105">
-    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
+    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
       <formula>ISBLANK($T105)</formula>
     </cfRule>
-    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
+    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
       <formula>$T105="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
       <formula>$K105&lt;&gt;$AA105</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103 G103 E103">
-    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
+    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B103">
-    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
+    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
+    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H103">
-    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71">
+    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
+    <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
+    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103 D105">
-    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
+    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
+    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
+    <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104:E104 G104">
-    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
+    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
       <formula>ISBLANK($T104)</formula>
     </cfRule>
-    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
+    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
       <formula>$T104="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
+    <cfRule type="expression" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
       <formula>$K104&lt;&gt;$AA104</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B104">
-    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
+    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84">
       <formula>ISBLANK($T104)</formula>
     </cfRule>
-    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
+    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
       <formula>$T104="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
+    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86">
       <formula>$K104&lt;&gt;$AA104</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H104">
-    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
+    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
       <formula>ISBLANK($T104)</formula>
     </cfRule>
-    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84">
+    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
       <formula>$T104="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
+    <cfRule type="expression" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
       <formula>$K104&lt;&gt;$AA104</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F103:F105">
-    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86">
+    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
+    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
+    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R105">
-    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
+    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93">
       <formula>ISBLANK($T105)</formula>
     </cfRule>
-    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
+    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
       <formula>$T105="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91">
+    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95">
       <formula>$K105&lt;&gt;$AA105</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R103">
-    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92">
+    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
       <formula>ISBLANK($R103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93">
+    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97">
       <formula>$R103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
+    <cfRule type="expression" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98">
       <formula>$I103&lt;&gt;$Y103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R104">
-    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95">
+    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
       <formula>ISBLANK($R104)</formula>
     </cfRule>
-    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
+    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100">
       <formula>$R104="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="103" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97">
+    <cfRule type="expression" priority="103" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101">
       <formula>$I104&lt;&gt;$Y104</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R99:R101">
-    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98">
+    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
       <formula>ISBLANK($R99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
+    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103">
       <formula>$R99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100">
+    <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104">
       <formula>$I99&lt;&gt;$Y99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91 E91 G91:H91">
-    <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101">
+    <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
+    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103">
+    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104">
+    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105">
+    <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106">
+    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89 G89 E89">
-    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
+    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108">
+    <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109">
+    <cfRule type="expression" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89">
-    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110">
+    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111">
+    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="118" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112">
+    <cfRule type="expression" priority="118" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89">
-    <cfRule type="expression" priority="119" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113">
+    <cfRule type="expression" priority="119" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114">
+    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115">
+    <cfRule type="expression" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D89 D91">
-    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116">
+    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117">
+    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118">
+    <cfRule type="expression" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90:E90 G90">
-    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119">
+    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120">
+    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121">
+    <cfRule type="expression" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90">
-    <cfRule type="expression" priority="128" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122">
+    <cfRule type="expression" priority="128" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123">
+    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124">
+    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H90">
-    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125">
+    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126">
+    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127">
+    <cfRule type="expression" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F89:F91">
-    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128">
+    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129">
+    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130">
+    <cfRule type="expression" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R91">
-    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131">
+    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="138" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132">
+    <cfRule type="expression" priority="138" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="139" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133">
+    <cfRule type="expression" priority="139" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R89">
-    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134">
+    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138">
       <formula>ISBLANK($R89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135">
+    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139">
       <formula>$R89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136">
+    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140">
       <formula>$I89&lt;&gt;$Y89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R90">
-    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137">
+    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141">
       <formula>ISBLANK($R90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138">
+    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142">
       <formula>$R90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139">
+    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143">
       <formula>$I90&lt;&gt;$Y90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4">
-    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140">
+    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144">
       <formula>ISBLANK($T4)</formula>
     </cfRule>
-    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141">
+    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="145">
       <formula>$T4="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142">
+    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146">
       <formula>$K4&lt;&gt;$AA4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U4:X4">
-    <cfRule type="expression" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143">
+    <cfRule type="expression" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="147">
       <formula>ISBLANK($T4)</formula>
     </cfRule>
-    <cfRule type="expression" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144">
+    <cfRule type="expression" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148">
       <formula>$T4="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="145">
+    <cfRule type="expression" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="149">
       <formula>$K4&lt;&gt;$AA4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5">
-    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146">
+    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150">
       <formula>ISBLANK($T5)</formula>
     </cfRule>
-    <cfRule type="expression" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="147">
+    <cfRule type="expression" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="151">
       <formula>$T5="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="154" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148">
+    <cfRule type="expression" priority="154" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="152">
       <formula>$K5&lt;&gt;$AA5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5:X5">
-    <cfRule type="expression" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="149">
+    <cfRule type="expression" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="153">
       <formula>ISBLANK($T5)</formula>
     </cfRule>
-    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150">
+    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154">
       <formula>$T5="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="151">
+    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155">
       <formula>$K5&lt;&gt;$AA5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH103">
-    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="152">
+    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156">
       <formula>ISBLANK($R103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="153">
+    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157">
       <formula>$R103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154">
+    <cfRule type="expression" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158">
       <formula>$I103&lt;&gt;$Y103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:W7">
-    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155">
+    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159">
       <formula>ISBLANK($T7)</formula>
     </cfRule>
-    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156">
+    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160">
       <formula>$T7="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157">
+    <cfRule type="expression" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161">
       <formula>$K7&lt;&gt;$AA7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T13">
-    <cfRule type="expression" priority="164" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158">
+    <cfRule type="expression" priority="164" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162">
       <formula>ISBLANK($T13)</formula>
     </cfRule>
-    <cfRule type="expression" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159">
+    <cfRule type="expression" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163">
       <formula>$T13="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160">
+    <cfRule type="expression" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164">
       <formula>$K13&lt;&gt;$AA13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U13:X13">
-    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161">
+    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165">
       <formula>ISBLANK($T13)</formula>
     </cfRule>
-    <cfRule type="expression" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162">
+    <cfRule type="expression" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166">
       <formula>$T13="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="169" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163">
+    <cfRule type="expression" priority="169" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167">
       <formula>$K13&lt;&gt;$AA13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T14">
-    <cfRule type="expression" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164">
+    <cfRule type="expression" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168">
       <formula>ISBLANK($T14)</formula>
     </cfRule>
-    <cfRule type="expression" priority="171" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165">
+    <cfRule type="expression" priority="171" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169">
       <formula>$T14="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166">
+    <cfRule type="expression" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170">
       <formula>$K14&lt;&gt;$AA14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U14:X14">
-    <cfRule type="expression" priority="173" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167">
+    <cfRule type="expression" priority="173" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171">
       <formula>ISBLANK($T14)</formula>
     </cfRule>
-    <cfRule type="expression" priority="174" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168">
+    <cfRule type="expression" priority="174" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="172">
       <formula>$T14="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169">
+    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173">
       <formula>$K14&lt;&gt;$AA14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15">
-    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170">
+    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174">
       <formula>ISBLANK($T15)</formula>
     </cfRule>
-    <cfRule type="expression" priority="177" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171">
+    <cfRule type="expression" priority="177" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175">
       <formula>$T15="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="172">
+    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176">
       <formula>$K15&lt;&gt;$AA15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U15:X15">
-    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173">
+    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177">
       <formula>ISBLANK($T15)</formula>
     </cfRule>
-    <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174">
+    <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178">
       <formula>$T15="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="181" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175">
+    <cfRule type="expression" priority="181" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179">
       <formula>$K15&lt;&gt;$AA15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16">
-    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176">
+    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180">
       <formula>ISBLANK($T16)</formula>
     </cfRule>
-    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177">
+    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181">
       <formula>$T16="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178">
+    <cfRule type="expression" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182">
       <formula>$K16&lt;&gt;$AA16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16:X16">
-    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179">
+    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183">
       <formula>ISBLANK($T16)</formula>
     </cfRule>
-    <cfRule type="expression" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180">
+    <cfRule type="expression" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184">
       <formula>$T16="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="187" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181">
+    <cfRule type="expression" priority="187" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185">
       <formula>$K16&lt;&gt;$AA16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U92:W101 U30:W39 U41:W88 W40">
-    <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182">
+    <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186">
       <formula>ISBLANK($T30)</formula>
     </cfRule>
-    <cfRule type="expression" priority="189" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183">
+    <cfRule type="expression" priority="189" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187">
       <formula>$T30="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184">
+    <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188">
       <formula>$K30&lt;&gt;$AA30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U98 W98">
-    <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185">
+    <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186">
+    <cfRule type="expression" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="193" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187">
+    <cfRule type="expression" priority="193" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V98 V100:V101">
-    <cfRule type="expression" priority="194" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188">
+    <cfRule type="expression" priority="194" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="192">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="195" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189">
+    <cfRule type="expression" priority="195" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="193">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190">
+    <cfRule type="expression" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="194">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U99:W99">
-    <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191">
+    <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="195">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="198" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="192">
+    <cfRule type="expression" priority="198" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="196">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="199" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="193">
+    <cfRule type="expression" priority="199" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="197">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W91">
-    <cfRule type="expression" priority="200" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="194">
+    <cfRule type="expression" priority="200" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="198">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="201" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="195">
+    <cfRule type="expression" priority="201" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="199">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="202" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="196">
+    <cfRule type="expression" priority="202" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W89">
-    <cfRule type="expression" priority="203" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="197">
+    <cfRule type="expression" priority="203" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="201">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="204" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="198">
+    <cfRule type="expression" priority="204" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="202">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="205" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="199">
+    <cfRule type="expression" priority="205" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="203">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W90">
-    <cfRule type="expression" priority="206" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200">
+    <cfRule type="expression" priority="206" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="204">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="207" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="201">
+    <cfRule type="expression" priority="207" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="205">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="208" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="202">
+    <cfRule type="expression" priority="208" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="206">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X30:X88 X92:X101">
-    <cfRule type="expression" priority="209" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="203">
+    <cfRule type="expression" priority="209" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="207">
       <formula>ISBLANK($T30)</formula>
     </cfRule>
-    <cfRule type="expression" priority="210" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="204">
+    <cfRule type="expression" priority="210" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="208">
       <formula>$T30="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="211" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="205">
+    <cfRule type="expression" priority="211" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="209">
       <formula>$K30&lt;&gt;$AA30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X98">
-    <cfRule type="expression" priority="212" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="206">
+    <cfRule type="expression" priority="212" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="213" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="207">
+    <cfRule type="expression" priority="213" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="211">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="208">
+    <cfRule type="expression" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="212">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X99">
-    <cfRule type="expression" priority="215" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="209">
+    <cfRule type="expression" priority="215" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="213">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="216" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210">
+    <cfRule type="expression" priority="216" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="217" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="211">
+    <cfRule type="expression" priority="217" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X91">
-    <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="212">
+    <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="213">
+    <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="220" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214">
+    <cfRule type="expression" priority="220" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X89">
-    <cfRule type="expression" priority="221" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215">
+    <cfRule type="expression" priority="221" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216">
+    <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217">
+    <cfRule type="expression" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X90">
-    <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218">
+    <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219">
+    <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="226" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220">
+    <cfRule type="expression" priority="226" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH99:AH101">
-    <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221">
+    <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225">
       <formula>ISBLANK($R99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="228" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222">
+    <cfRule type="expression" priority="228" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226">
       <formula>$R99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="229" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223">
+    <cfRule type="expression" priority="229" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227">
       <formula>$I99&lt;&gt;$Y99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK6">
-    <cfRule type="expression" priority="230" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224">
+    <cfRule type="expression" priority="230" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228">
       <formula>ISBLANK($R6)</formula>
     </cfRule>
-    <cfRule type="expression" priority="231" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225">
+    <cfRule type="expression" priority="231" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229">
       <formula>$R6="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="232" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226">
+    <cfRule type="expression" priority="232" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230">
       <formula>$I6&lt;&gt;$Y6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T89:T91">
-    <cfRule type="expression" priority="233" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227">
+    <cfRule type="expression" priority="233" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="231">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="234" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228">
+    <cfRule type="expression" priority="234" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="232">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="235" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229">
+    <cfRule type="expression" priority="235" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="233">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U89:V91">
-    <cfRule type="expression" priority="236" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230">
+    <cfRule type="expression" priority="236" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="234">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="237" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="231">
+    <cfRule type="expression" priority="237" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="235">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="238" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="232">
+    <cfRule type="expression" priority="238" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK26:AK27">
-    <cfRule type="expression" priority="239" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="233">
+    <cfRule type="expression" priority="239" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237">
       <formula>ISBLANK($R26)</formula>
     </cfRule>
-    <cfRule type="expression" priority="240" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="234">
+    <cfRule type="expression" priority="240" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238">
       <formula>$R26="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="241" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="235">
+    <cfRule type="expression" priority="241" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239">
       <formula>$I26&lt;&gt;$Y26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK24">
-    <cfRule type="expression" priority="242" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236">
+    <cfRule type="expression" priority="242" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240">
       <formula>ISBLANK($R24)</formula>
     </cfRule>
-    <cfRule type="expression" priority="243" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237">
+    <cfRule type="expression" priority="243" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241">
       <formula>$R24="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="244" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238">
+    <cfRule type="expression" priority="244" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242">
       <formula>$I24&lt;&gt;$Y24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK22">
-    <cfRule type="expression" priority="245" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239">
+    <cfRule type="expression" priority="245" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="243">
       <formula>ISBLANK($R9)</formula>
     </cfRule>
-    <cfRule type="expression" priority="246" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240">
+    <cfRule type="expression" priority="246" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="244">
       <formula>$R9="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="247" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241">
+    <cfRule type="expression" priority="247" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="245">
       <formula>$I9&lt;&gt;$Y9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK7">
-    <cfRule type="expression" priority="248" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242">
+    <cfRule type="expression" priority="248" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="246">
       <formula>ISBLANK($R7)</formula>
     </cfRule>
-    <cfRule type="expression" priority="249" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="243">
+    <cfRule type="expression" priority="249" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="247">
       <formula>$R7="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="250" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="244">
+    <cfRule type="expression" priority="250" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="248">
       <formula>$I7&lt;&gt;$Y7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4">
-    <cfRule type="expression" priority="251" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="245">
+    <cfRule type="expression" priority="251" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="249">
       <formula>ISBLANK($R4)</formula>
     </cfRule>
-    <cfRule type="expression" priority="252" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="246">
+    <cfRule type="expression" priority="252" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250">
       <formula>$R4="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="253" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="247">
+    <cfRule type="expression" priority="253" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="251">
       <formula>$I4&lt;&gt;$Y4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK3">
-    <cfRule type="expression" priority="254" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="248">
+    <cfRule type="expression" priority="254" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="252">
       <formula>ISBLANK($R3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="255" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="249">
+    <cfRule type="expression" priority="255" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="253">
       <formula>$R3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="256" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250">
+    <cfRule type="expression" priority="256" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="254">
       <formula>$I3&lt;&gt;$Y3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK92:AK101">
-    <cfRule type="expression" priority="257" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="251">
+    <cfRule type="expression" priority="257" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="255">
       <formula>ISBLANK($R92)</formula>
     </cfRule>
-    <cfRule type="expression" priority="258" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="252">
+    <cfRule type="expression" priority="258" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="256">
       <formula>$R92="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="259" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="253">
+    <cfRule type="expression" priority="259" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="257">
       <formula>$I92&lt;&gt;$Y92</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK8">
-    <cfRule type="expression" priority="260" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="254">
+    <cfRule type="expression" priority="260" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="258">
       <formula>ISBLANK($R8)</formula>
     </cfRule>
-    <cfRule type="expression" priority="261" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="255">
+    <cfRule type="expression" priority="261" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="259">
       <formula>$R8="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="262" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="256">
+    <cfRule type="expression" priority="262" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260">
       <formula>$I8&lt;&gt;$Y8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U40:V40">
-    <cfRule type="expression" priority="263" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="257">
+    <cfRule type="expression" priority="263" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="261">
       <formula>ISBLANK($T40)</formula>
     </cfRule>
-    <cfRule type="expression" priority="264" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="258">
+    <cfRule type="expression" priority="264" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="262">
       <formula>$T40="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="265" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="259">
+    <cfRule type="expression" priority="265" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="263">
       <formula>$K40&lt;&gt;$AA40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U8:V8">
-    <cfRule type="expression" priority="266" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260">
+    <cfRule type="expression" priority="266" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="264">
       <formula>ISBLANK($T8)</formula>
     </cfRule>
-    <cfRule type="expression" priority="267" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="261">
+    <cfRule type="expression" priority="267" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="265">
       <formula>$T8="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="268" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="262">
+    <cfRule type="expression" priority="268" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="266">
       <formula>$K8&lt;&gt;$AA8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24832,12 +24889,12 @@
       <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="9.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="9.09"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24851,7 +24908,7 @@
       <c r="G2" s="123"/>
       <c r="H2" s="123"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="153"/>
       <c r="C3" s="154" t="s">
         <v>39</v>
@@ -24874,7 +24931,7 @@
       <c r="I3" s="155"/>
       <c r="J3" s="156"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="154" t="s">
         <v>99</v>
       </c>
@@ -24910,7 +24967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="154" t="s">
         <v>100</v>
       </c>
@@ -24946,7 +25003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="154" t="s">
         <v>101</v>
       </c>
@@ -24982,7 +25039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="154" t="s">
         <v>102</v>
       </c>
@@ -25018,7 +25075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="154" t="s">
         <v>103</v>
       </c>
@@ -25049,7 +25106,7 @@
       <c r="I8" s="158"/>
       <c r="J8" s="156"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="154" t="s">
         <v>104</v>
       </c>
@@ -25068,7 +25125,7 @@
       <c r="I9" s="158"/>
       <c r="J9" s="156"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="154" t="s">
         <v>105</v>
       </c>
@@ -25099,7 +25156,7 @@
       <c r="I10" s="155"/>
       <c r="J10" s="156"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I11" s="156"/>
       <c r="J11" s="156"/>
     </row>
@@ -25116,7 +25173,7 @@
       <c r="I12" s="156"/>
       <c r="J12" s="156"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="153"/>
       <c r="C13" s="154" t="s">
         <v>39</v>
@@ -25139,7 +25196,7 @@
       <c r="I13" s="155"/>
       <c r="J13" s="156"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="159" t="s">
         <v>99</v>
       </c>
@@ -25175,7 +25232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="159" t="s">
         <v>100</v>
       </c>
@@ -25211,7 +25268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="159" t="s">
         <v>101</v>
       </c>
@@ -25247,7 +25304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="159" t="s">
         <v>102</v>
       </c>
@@ -25283,7 +25340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="159" t="s">
         <v>103</v>
       </c>
@@ -25314,7 +25371,7 @@
       <c r="I18" s="158"/>
       <c r="J18" s="156"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="159" t="s">
         <v>104</v>
       </c>
@@ -25333,7 +25390,7 @@
       <c r="I19" s="158"/>
       <c r="J19" s="156"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="159" t="s">
         <v>105</v>
       </c>
@@ -25391,17 +25448,17 @@
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="160" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="160" width="14.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="156" width="61.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="160" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="161" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="160" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="156" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="160" width="12.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="161" width="18.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="160" width="11.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="156" width="9.09"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="162" t="s">
         <v>107</v>
       </c>
@@ -25464,7 +25521,7 @@
       </c>
       <c r="F4" s="164"/>
     </row>
-    <row r="5" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="165" t="s">
         <v>118</v>
       </c>
@@ -25482,7 +25539,7 @@
       </c>
       <c r="F5" s="164"/>
     </row>
-    <row r="6" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="165" t="s">
         <v>120</v>
       </c>
@@ -25500,7 +25557,7 @@
       </c>
       <c r="F6" s="164"/>
     </row>
-    <row r="7" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="165" t="s">
         <v>122</v>
       </c>
@@ -25518,7 +25575,7 @@
       </c>
       <c r="F7" s="164"/>
     </row>
-    <row r="8" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="165" t="s">
         <v>124</v>
       </c>
@@ -25536,7 +25593,7 @@
       </c>
       <c r="F8" s="164"/>
     </row>
-    <row r="9" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="165" t="s">
         <v>126</v>
       </c>
@@ -25554,7 +25611,7 @@
       </c>
       <c r="F9" s="164"/>
     </row>
-    <row r="10" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="165" t="s">
         <v>129</v>
       </c>
@@ -25572,7 +25629,7 @@
       </c>
       <c r="F10" s="164"/>
     </row>
-    <row r="11" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="165" t="s">
         <v>131</v>
       </c>
@@ -25590,7 +25647,7 @@
       </c>
       <c r="F11" s="164"/>
     </row>
-    <row r="12" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="165" t="s">
         <v>134</v>
       </c>
@@ -25608,7 +25665,7 @@
       </c>
       <c r="F12" s="164"/>
     </row>
-    <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="165" t="s">
         <v>137</v>
       </c>
@@ -25626,7 +25683,7 @@
       </c>
       <c r="F13" s="164"/>
     </row>
-    <row r="14" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="165" t="s">
         <v>140</v>
       </c>
@@ -25644,7 +25701,7 @@
       </c>
       <c r="F14" s="164"/>
     </row>
-    <row r="15" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="165" t="s">
         <v>143</v>
       </c>
@@ -25662,7 +25719,7 @@
       </c>
       <c r="F15" s="164"/>
     </row>
-    <row r="16" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="165" t="s">
         <v>146</v>
       </c>
@@ -25680,7 +25737,7 @@
       </c>
       <c r="F16" s="164"/>
     </row>
-    <row r="17" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="165" t="s">
         <v>149</v>
       </c>
@@ -25698,7 +25755,7 @@
       </c>
       <c r="F17" s="164"/>
     </row>
-    <row r="18" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="165" t="s">
         <v>152</v>
       </c>
@@ -25716,7 +25773,7 @@
       </c>
       <c r="F18" s="164"/>
     </row>
-    <row r="19" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="165" t="s">
         <v>154</v>
       </c>
@@ -25734,7 +25791,7 @@
       </c>
       <c r="F19" s="164"/>
     </row>
-    <row r="20" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="165" t="s">
         <v>157</v>
       </c>
@@ -25752,7 +25809,7 @@
       </c>
       <c r="F20" s="164"/>
     </row>
-    <row r="21" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="165" t="s">
         <v>159</v>
       </c>
@@ -25770,7 +25827,7 @@
       </c>
       <c r="F21" s="164"/>
     </row>
-    <row r="22" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="165" t="s">
         <v>161</v>
       </c>
@@ -25788,7 +25845,7 @@
       </c>
       <c r="F22" s="164"/>
     </row>
-    <row r="23" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="165" t="s">
         <v>164</v>
       </c>
@@ -25806,7 +25863,7 @@
       </c>
       <c r="F23" s="164"/>
     </row>
-    <row r="24" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="165" t="s">
         <v>167</v>
       </c>
@@ -25824,7 +25881,7 @@
       </c>
       <c r="F24" s="164"/>
     </row>
-    <row r="25" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="165" t="s">
         <v>170</v>
       </c>
@@ -25842,7 +25899,7 @@
       </c>
       <c r="F25" s="164"/>
     </row>
-    <row r="26" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="165" t="s">
         <v>173</v>
       </c>
@@ -25860,7 +25917,7 @@
       </c>
       <c r="F26" s="164"/>
     </row>
-    <row r="27" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="165" t="s">
         <v>176</v>
       </c>
@@ -25878,7 +25935,7 @@
       </c>
       <c r="F27" s="164"/>
     </row>
-    <row r="28" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="165" t="s">
         <v>176</v>
       </c>
@@ -25896,7 +25953,7 @@
       </c>
       <c r="F28" s="164"/>
     </row>
-    <row r="29" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="165" t="s">
         <v>180</v>
       </c>
@@ -25914,7 +25971,7 @@
       </c>
       <c r="F29" s="164"/>
     </row>
-    <row r="30" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="165" t="s">
         <v>183</v>
       </c>
@@ -25932,7 +25989,7 @@
       </c>
       <c r="F30" s="164"/>
     </row>
-    <row r="31" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="165" t="s">
         <v>186</v>
       </c>
@@ -25950,7 +26007,7 @@
       </c>
       <c r="F31" s="164"/>
     </row>
-    <row r="32" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="165" t="s">
         <v>188</v>
       </c>
@@ -25968,7 +26025,7 @@
       </c>
       <c r="F32" s="164"/>
     </row>
-    <row r="33" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="165" t="s">
         <v>191</v>
       </c>
@@ -26020,15 +26077,15 @@
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.54"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="163" t="s">
         <v>193</v>
       </c>
@@ -26036,679 +26093,679 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="170"/>
       <c r="C3" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B3,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="170"/>
       <c r="C4" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B4,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="170"/>
       <c r="C5" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B5,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="170"/>
       <c r="C6" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B6,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="170"/>
       <c r="C7" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B7,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="170"/>
       <c r="C8" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B8,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="170"/>
       <c r="C9" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B9,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="170"/>
       <c r="C10" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B10,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="170"/>
       <c r="C11" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B11,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="170"/>
       <c r="C12" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B12,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="170"/>
       <c r="C13" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B13,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="170"/>
       <c r="C14" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B14,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="170"/>
       <c r="C15" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B15,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="170"/>
       <c r="C16" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B16,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="170"/>
       <c r="C17" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B17,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="170"/>
       <c r="C18" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B18,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="170"/>
       <c r="C19" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B19,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="170"/>
       <c r="C20" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B20,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="170"/>
       <c r="C21" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B21,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="170"/>
       <c r="C22" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B22,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="170"/>
       <c r="C23" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B23,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="170"/>
       <c r="C24" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B24,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="170"/>
       <c r="C25" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B25,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="170"/>
       <c r="C26" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B26,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="170"/>
       <c r="C27" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B27,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="170"/>
       <c r="C28" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B28,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="170"/>
       <c r="C29" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B29,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="170"/>
       <c r="C30" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B30,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="170"/>
       <c r="C31" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B31,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="170"/>
       <c r="C32" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B32,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="170"/>
       <c r="C33" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B33,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="170"/>
       <c r="C34" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B34,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="170"/>
       <c r="C35" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B35,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="170"/>
       <c r="C36" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B36,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="170"/>
       <c r="C37" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B37,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="170"/>
       <c r="C38" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B38,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="170"/>
       <c r="C39" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B39,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="170"/>
       <c r="C40" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B40,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="170"/>
       <c r="C41" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B41,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="170"/>
       <c r="C42" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B42,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="170"/>
       <c r="C43" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B43,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="170"/>
       <c r="C44" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B44,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="170"/>
       <c r="C45" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B45,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="170"/>
       <c r="C46" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B46,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="170"/>
       <c r="C47" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B47,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="170"/>
       <c r="C48" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B48,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="170"/>
       <c r="C49" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B49,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="170"/>
       <c r="C50" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B50,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="170"/>
       <c r="C51" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B51,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="170"/>
       <c r="C52" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B52,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="170"/>
       <c r="C53" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B53,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="170"/>
       <c r="C54" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B54,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="170"/>
       <c r="C55" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B55,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="170"/>
       <c r="C56" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B56,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="170"/>
       <c r="C57" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B57,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="170"/>
       <c r="C58" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B58,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="170"/>
       <c r="C59" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B59,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="170"/>
       <c r="C60" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B60,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="170"/>
       <c r="C61" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B61,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="170"/>
       <c r="C62" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B62,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="170"/>
       <c r="C63" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B63,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="170"/>
       <c r="C64" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B64,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="170"/>
       <c r="C65" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B65,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="170"/>
       <c r="C66" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B66,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="170"/>
       <c r="C67" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B67,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="170"/>
       <c r="C68" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B68,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="170"/>
       <c r="C69" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B69,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="170"/>
       <c r="C70" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B70,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="170"/>
       <c r="C71" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B71,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="170"/>
       <c r="C72" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B72,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="170"/>
       <c r="C73" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B73,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="170"/>
       <c r="C74" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B74,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="170"/>
       <c r="C75" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B75,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="170"/>
       <c r="C76" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B76,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="170"/>
       <c r="C77" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B77,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="170"/>
       <c r="C78" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B78,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="170"/>
       <c r="C79" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B79,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="170"/>
       <c r="C80" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B80,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="170"/>
       <c r="C81" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B81,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="170"/>
       <c r="C82" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B82,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="170"/>
       <c r="C83" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B83,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="170"/>
       <c r="C84" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B84,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="170"/>
       <c r="C85" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B85,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="170"/>
       <c r="C86" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B86,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="170"/>
       <c r="C87" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B87,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="170"/>
       <c r="C88" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B88,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="170"/>
       <c r="C89" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B89,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="170"/>
       <c r="C90" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B90,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="170"/>
       <c r="C91" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B91,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="170"/>
       <c r="C92" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B92,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="170"/>
       <c r="C93" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B93,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="170"/>
       <c r="C94" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B94,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="170"/>
       <c r="C95" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B95,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="170"/>
       <c r="C96" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B96,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="170"/>
       <c r="C97" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B97,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="170"/>
       <c r="C98" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B98,Funções!$AG$3:$AG$202)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="170"/>
       <c r="C99" s="168" t="n">
         <f aca="false">SUMIF(Funções!$A$3:$A$202,B99,Funções!$AG$3:$AG$202)</f>
@@ -26738,15 +26795,15 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="171" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.54"/>
   </cols>
   <sheetData>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>195</v>
       </c>
@@ -26776,21 +26833,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="9.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="172" t="s">
         <v>198</v>
       </c>
@@ -26801,186 +26859,305 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="173"/>
-      <c r="B2" s="174"/>
-      <c r="C2" s="174"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="173"/>
-      <c r="B3" s="174"/>
-      <c r="C3" s="174"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="174"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="173"/>
-      <c r="B5" s="174"/>
-      <c r="C5" s="174"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="173"/>
-      <c r="B6" s="174"/>
-      <c r="C6" s="174"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="173"/>
-      <c r="B7" s="174"/>
-      <c r="C7" s="174"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="173"/>
-      <c r="B8" s="174"/>
-      <c r="C8" s="174"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="173"/>
-      <c r="B9" s="174"/>
-      <c r="C9" s="174"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="173"/>
-      <c r="B10" s="174"/>
-      <c r="C10" s="174"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="173"/>
-      <c r="B11" s="174"/>
-      <c r="C11" s="174"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
-      <c r="C12" s="174"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="173"/>
-      <c r="B13" s="174"/>
-      <c r="C13" s="174"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="173"/>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="173"/>
-      <c r="B15" s="174"/>
-      <c r="C15" s="174"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="173"/>
-      <c r="B16" s="174"/>
-      <c r="C16" s="174"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="173"/>
-      <c r="B17" s="174"/>
-      <c r="C17" s="174"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="173"/>
-      <c r="B18" s="174"/>
-      <c r="C18" s="174"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="173"/>
-      <c r="B19" s="174"/>
-      <c r="C19" s="174"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="173"/>
-      <c r="B20" s="174"/>
-      <c r="C20" s="174"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="173"/>
-      <c r="B21" s="174"/>
-      <c r="C21" s="174"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="173"/>
-      <c r="B22" s="174"/>
-      <c r="C22" s="174"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="173"/>
-      <c r="B23" s="174"/>
-      <c r="C23" s="174"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="173"/>
-      <c r="B24" s="174"/>
-      <c r="C24" s="174"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="173"/>
-      <c r="B25" s="174"/>
-      <c r="C25" s="174"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="173"/>
-      <c r="B26" s="174"/>
-      <c r="C26" s="174"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="173"/>
-      <c r="B27" s="174"/>
-      <c r="C27" s="174"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="173"/>
-      <c r="B28" s="174"/>
-      <c r="C28" s="174"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="173"/>
-      <c r="B29" s="174"/>
-      <c r="C29" s="174"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="173"/>
-      <c r="B30" s="174"/>
-      <c r="C30" s="174"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="173"/>
-      <c r="B31" s="174"/>
-      <c r="C31" s="174"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="173"/>
-      <c r="B32" s="174"/>
-      <c r="C32" s="174"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="173"/>
-      <c r="B33" s="174"/>
-      <c r="C33" s="174"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="173"/>
-      <c r="B34" s="174"/>
-      <c r="C34" s="174"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="173"/>
-      <c r="B35" s="174"/>
-      <c r="C35" s="174"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="173"/>
-      <c r="B36" s="174"/>
-      <c r="C36" s="174"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="173"/>
-      <c r="B37" s="174"/>
-      <c r="C37" s="174"/>
-    </row>
+    <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="188" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="189" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="225" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="239" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="241" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="242" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="243" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="244" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="245" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="246" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="247" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="248" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="249" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="250" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="251" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="252" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="253" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="254" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="255" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="256" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="257" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="258" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="259" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="260" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="261" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="262" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="263" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="264" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="265" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="266" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="267" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="268" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="269" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="270" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="271" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="272" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="273" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="274" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="275" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="276" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="277" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="278" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="279" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="280" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="281" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="282" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="283" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="284" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="285" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="286" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="287" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="288" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="289" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="290" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="291" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="292" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="293" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="294" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="295" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="296" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="297" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="298" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="299" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="300" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Ajustar equipe em funções - BASIS-241480
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/reports/planilhas/modelo3-anac.xlsx
+++ b/backend/src/main/resources/reports/planilhas/modelo3-anac.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psantos8\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EF4AE5-3261-4127-87EC-DFE4D067750C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302B3E89-D576-4506-B314-53E411635972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1662,29 +1662,6 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1699,15 +1676,83 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1717,54 +1762,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1780,10 +1784,6 @@
     </xf>
     <xf numFmtId="0" fontId="47" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3759,49 +3759,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="20" x14ac:dyDescent="0.35">
-      <c r="B1" s="150" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
-      <c r="G1" s="150"/>
-      <c r="H1" s="150"/>
-      <c r="I1" s="150"/>
-      <c r="J1" s="150"/>
-      <c r="K1" s="150"/>
-      <c r="L1" s="150"/>
+      <c r="B1" s="144" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="144"/>
+      <c r="J1" s="144"/>
+      <c r="K1" s="144"/>
+      <c r="L1" s="144"/>
     </row>
     <row r="2" spans="2:12" ht="20" x14ac:dyDescent="0.4">
-      <c r="B2" s="151" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="151"/>
-      <c r="K2" s="151"/>
-      <c r="L2" s="151"/>
+      <c r="B2" s="145" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="145"/>
+      <c r="K2" s="145"/>
+      <c r="L2" s="145"/>
     </row>
     <row r="3" spans="2:12" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="152" t="s">
+      <c r="B3" s="146" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="152"/>
-      <c r="K3" s="152"/>
-      <c r="L3" s="152"/>
+      <c r="C3" s="146"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="146"/>
+      <c r="F3" s="146"/>
+      <c r="G3" s="146"/>
+      <c r="H3" s="146"/>
+      <c r="I3" s="146"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="146"/>
+      <c r="L3" s="146"/>
     </row>
     <row r="4" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
@@ -3810,190 +3810,190 @@
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="153" t="s">
+      <c r="D4" s="147" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="153"/>
-      <c r="F4" s="153"/>
-      <c r="G4" s="153" t="s">
+      <c r="E4" s="147"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="147" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
-      <c r="J4" s="153"/>
-      <c r="K4" s="153"/>
-      <c r="L4" s="153"/>
+      <c r="H4" s="147"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="147"/>
+      <c r="K4" s="147"/>
+      <c r="L4" s="147"/>
     </row>
     <row r="5" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="149"/>
-      <c r="E5" s="149"/>
-      <c r="F5" s="149"/>
-      <c r="G5" s="149"/>
-      <c r="H5" s="149"/>
-      <c r="I5" s="149"/>
-      <c r="J5" s="149"/>
-      <c r="K5" s="149"/>
-      <c r="L5" s="149"/>
+      <c r="D5" s="148"/>
+      <c r="E5" s="148"/>
+      <c r="F5" s="148"/>
+      <c r="G5" s="148"/>
+      <c r="H5" s="148"/>
+      <c r="I5" s="148"/>
+      <c r="J5" s="148"/>
+      <c r="K5" s="148"/>
+      <c r="L5" s="148"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="147"/>
-      <c r="E6" s="147"/>
-      <c r="F6" s="147"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="148"/>
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="150"/>
+      <c r="H6" s="150"/>
+      <c r="I6" s="150"/>
+      <c r="J6" s="150"/>
+      <c r="K6" s="150"/>
+      <c r="L6" s="150"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="145"/>
-      <c r="E7" s="145"/>
-      <c r="F7" s="145"/>
-      <c r="G7" s="146"/>
-      <c r="H7" s="146"/>
-      <c r="I7" s="146"/>
-      <c r="J7" s="146"/>
-      <c r="K7" s="146"/>
-      <c r="L7" s="146"/>
+      <c r="D7" s="151"/>
+      <c r="E7" s="151"/>
+      <c r="F7" s="151"/>
+      <c r="G7" s="152"/>
+      <c r="H7" s="152"/>
+      <c r="I7" s="152"/>
+      <c r="J7" s="152"/>
+      <c r="K7" s="152"/>
+      <c r="L7" s="152"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="7"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="147"/>
-      <c r="E8" s="147"/>
-      <c r="F8" s="147"/>
-      <c r="G8" s="148"/>
-      <c r="H8" s="148"/>
-      <c r="I8" s="148"/>
-      <c r="J8" s="148"/>
-      <c r="K8" s="148"/>
-      <c r="L8" s="148"/>
+      <c r="D8" s="149"/>
+      <c r="E8" s="149"/>
+      <c r="F8" s="149"/>
+      <c r="G8" s="150"/>
+      <c r="H8" s="150"/>
+      <c r="I8" s="150"/>
+      <c r="J8" s="150"/>
+      <c r="K8" s="150"/>
+      <c r="L8" s="150"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="7"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="147"/>
-      <c r="E9" s="147"/>
-      <c r="F9" s="147"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="148"/>
-      <c r="I9" s="148"/>
-      <c r="J9" s="148"/>
-      <c r="K9" s="148"/>
-      <c r="L9" s="148"/>
+      <c r="D9" s="149"/>
+      <c r="E9" s="149"/>
+      <c r="F9" s="149"/>
+      <c r="G9" s="150"/>
+      <c r="H9" s="150"/>
+      <c r="I9" s="150"/>
+      <c r="J9" s="150"/>
+      <c r="K9" s="150"/>
+      <c r="L9" s="150"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="146"/>
-      <c r="E10" s="146"/>
-      <c r="F10" s="146"/>
-      <c r="G10" s="146"/>
-      <c r="H10" s="146"/>
-      <c r="I10" s="146"/>
-      <c r="J10" s="146"/>
-      <c r="K10" s="146"/>
-      <c r="L10" s="146"/>
+      <c r="D10" s="152"/>
+      <c r="E10" s="152"/>
+      <c r="F10" s="152"/>
+      <c r="G10" s="152"/>
+      <c r="H10" s="152"/>
+      <c r="I10" s="152"/>
+      <c r="J10" s="152"/>
+      <c r="K10" s="152"/>
+      <c r="L10" s="152"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="146"/>
-      <c r="E11" s="146"/>
-      <c r="F11" s="146"/>
-      <c r="G11" s="146"/>
-      <c r="H11" s="146"/>
-      <c r="I11" s="146"/>
-      <c r="J11" s="146"/>
-      <c r="K11" s="146"/>
-      <c r="L11" s="146"/>
+      <c r="D11" s="152"/>
+      <c r="E11" s="152"/>
+      <c r="F11" s="152"/>
+      <c r="G11" s="152"/>
+      <c r="H11" s="152"/>
+      <c r="I11" s="152"/>
+      <c r="J11" s="152"/>
+      <c r="K11" s="152"/>
+      <c r="L11" s="152"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="145"/>
-      <c r="E12" s="145"/>
-      <c r="F12" s="145"/>
-      <c r="G12" s="146"/>
-      <c r="H12" s="146"/>
-      <c r="I12" s="146"/>
-      <c r="J12" s="146"/>
-      <c r="K12" s="146"/>
-      <c r="L12" s="146"/>
+      <c r="D12" s="151"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="151"/>
+      <c r="G12" s="152"/>
+      <c r="H12" s="152"/>
+      <c r="I12" s="152"/>
+      <c r="J12" s="152"/>
+      <c r="K12" s="152"/>
+      <c r="L12" s="152"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="145"/>
-      <c r="E13" s="145"/>
-      <c r="F13" s="145"/>
-      <c r="G13" s="146"/>
-      <c r="H13" s="146"/>
-      <c r="I13" s="146"/>
-      <c r="J13" s="146"/>
-      <c r="K13" s="146"/>
-      <c r="L13" s="146"/>
+      <c r="D13" s="151"/>
+      <c r="E13" s="151"/>
+      <c r="F13" s="151"/>
+      <c r="G13" s="152"/>
+      <c r="H13" s="152"/>
+      <c r="I13" s="152"/>
+      <c r="J13" s="152"/>
+      <c r="K13" s="152"/>
+      <c r="L13" s="152"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="145"/>
-      <c r="E14" s="145"/>
-      <c r="F14" s="145"/>
-      <c r="G14" s="146"/>
-      <c r="H14" s="146"/>
-      <c r="I14" s="146"/>
-      <c r="J14" s="146"/>
-      <c r="K14" s="146"/>
-      <c r="L14" s="146"/>
+      <c r="D14" s="151"/>
+      <c r="E14" s="151"/>
+      <c r="F14" s="151"/>
+      <c r="G14" s="152"/>
+      <c r="H14" s="152"/>
+      <c r="I14" s="152"/>
+      <c r="J14" s="152"/>
+      <c r="K14" s="152"/>
+      <c r="L14" s="152"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="145"/>
-      <c r="E15" s="145"/>
-      <c r="F15" s="145"/>
-      <c r="G15" s="146"/>
-      <c r="H15" s="146"/>
-      <c r="I15" s="146"/>
-      <c r="J15" s="146"/>
-      <c r="K15" s="146"/>
-      <c r="L15" s="146"/>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="152"/>
+      <c r="H15" s="152"/>
+      <c r="I15" s="152"/>
+      <c r="J15" s="152"/>
+      <c r="K15" s="152"/>
+      <c r="L15" s="152"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="145"/>
-      <c r="E16" s="145"/>
-      <c r="F16" s="145"/>
-      <c r="G16" s="146"/>
-      <c r="H16" s="146"/>
-      <c r="I16" s="146"/>
-      <c r="J16" s="146"/>
-      <c r="K16" s="146"/>
-      <c r="L16" s="146"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="152"/>
+      <c r="H16" s="152"/>
+      <c r="I16" s="152"/>
+      <c r="J16" s="152"/>
+      <c r="K16" s="152"/>
+      <c r="L16" s="152"/>
     </row>
     <row r="17" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B17" s="144" t="s">
+      <c r="B17" s="153" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="144"/>
-      <c r="D17" s="144"/>
-      <c r="E17" s="144"/>
-      <c r="F17" s="144"/>
-      <c r="G17" s="144"/>
-      <c r="H17" s="144"/>
-      <c r="I17" s="144"/>
-      <c r="J17" s="144"/>
-      <c r="K17" s="144"/>
-      <c r="L17" s="144"/>
+      <c r="C17" s="153"/>
+      <c r="D17" s="153"/>
+      <c r="E17" s="153"/>
+      <c r="F17" s="153"/>
+      <c r="G17" s="153"/>
+      <c r="H17" s="153"/>
+      <c r="I17" s="153"/>
+      <c r="J17" s="153"/>
+      <c r="K17" s="153"/>
+      <c r="L17" s="153"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" selectLockedCells="1"/>
@@ -4001,29 +4001,6 @@
     <protectedRange sqref="B1 B2 B5:L16" name="Revisao"/>
   </protectedRanges>
   <mergeCells count="30">
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="G4:L4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:L6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:L8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:L9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:L10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:L12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:L13"/>
     <mergeCell ref="B17:L17"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="G14:L14"/>
@@ -4031,6 +4008,29 @@
     <mergeCell ref="G15:L15"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="G16:L16"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:L12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:L8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:L9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:L10"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:L6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:L4"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4041,7 +4041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="D11" sqref="D11:J11"/>
     </sheetView>
   </sheetViews>
@@ -4064,17 +4064,17 @@
       <c r="J1" s="10"/>
     </row>
     <row r="2" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
-      <c r="I2" s="173"/>
-      <c r="J2" s="173"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
     </row>
     <row r="3" spans="2:10" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11"/>
@@ -4115,126 +4115,126 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="174" t="str">
+      <c r="B5" s="155" t="str">
         <f>IF(OR(ISBLANK(D13),D13=0),"Aguardando Aferição da Fábrica de Software",IF(OR(ISBLANK(D20),D20=0),"Aguardando Aferição da Fábrica de Métricas",IF(OR(AND(D24&gt;=0,D24&lt;=H3),AND(D24&lt;=0,D24&gt;=H4)),"Contagem Aprovada","Contagem em Divergência")))</f>
         <v>Aguardando Aferição da Fábrica de Software</v>
       </c>
-      <c r="C5" s="174"/>
-      <c r="D5" s="174"/>
-      <c r="E5" s="174"/>
-      <c r="F5" s="174"/>
-      <c r="G5" s="174"/>
-      <c r="H5" s="174"/>
-      <c r="I5" s="174"/>
-      <c r="J5" s="174"/>
+      <c r="C5" s="155"/>
+      <c r="D5" s="155"/>
+      <c r="E5" s="155"/>
+      <c r="F5" s="155"/>
+      <c r="G5" s="155"/>
+      <c r="H5" s="155"/>
+      <c r="I5" s="155"/>
+      <c r="J5" s="155"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="155" t="s">
+      <c r="B6" s="156" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="155"/>
-      <c r="D6" s="155"/>
-      <c r="E6" s="155"/>
-      <c r="F6" s="155"/>
-      <c r="G6" s="155"/>
-      <c r="H6" s="155"/>
-      <c r="I6" s="155"/>
-      <c r="J6" s="155"/>
+      <c r="C6" s="156"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="156"/>
+      <c r="G6" s="156"/>
+      <c r="H6" s="156"/>
+      <c r="I6" s="156"/>
+      <c r="J6" s="156"/>
     </row>
     <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="163" t="s">
+      <c r="B7" s="157" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="163"/>
-      <c r="D7" s="171" t="s">
+      <c r="C7" s="157"/>
+      <c r="D7" s="158" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="171"/>
-      <c r="F7" s="171"/>
-      <c r="G7" s="171"/>
-      <c r="H7" s="171"/>
-      <c r="I7" s="171"/>
-      <c r="J7" s="171"/>
+      <c r="E7" s="158"/>
+      <c r="F7" s="158"/>
+      <c r="G7" s="158"/>
+      <c r="H7" s="158"/>
+      <c r="I7" s="158"/>
+      <c r="J7" s="158"/>
     </row>
     <row r="8" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="163" t="s">
+      <c r="B8" s="157" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="163"/>
-      <c r="D8" s="172"/>
-      <c r="E8" s="172"/>
-      <c r="F8" s="172"/>
-      <c r="G8" s="172"/>
-      <c r="H8" s="172"/>
-      <c r="I8" s="172"/>
-      <c r="J8" s="172"/>
+      <c r="C8" s="157"/>
+      <c r="D8" s="159"/>
+      <c r="E8" s="159"/>
+      <c r="F8" s="159"/>
+      <c r="G8" s="159"/>
+      <c r="H8" s="159"/>
+      <c r="I8" s="159"/>
+      <c r="J8" s="159"/>
     </row>
     <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="163" t="s">
+      <c r="B9" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="163"/>
-      <c r="D9" s="171"/>
-      <c r="E9" s="171"/>
-      <c r="F9" s="171"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="171"/>
-      <c r="I9" s="171"/>
-      <c r="J9" s="171"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="158"/>
+      <c r="E9" s="158"/>
+      <c r="F9" s="158"/>
+      <c r="G9" s="158"/>
+      <c r="H9" s="158"/>
+      <c r="I9" s="158"/>
+      <c r="J9" s="158"/>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="163" t="s">
+      <c r="B10" s="157" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="163"/>
-      <c r="D10" s="171"/>
-      <c r="E10" s="171"/>
-      <c r="F10" s="171"/>
-      <c r="G10" s="171"/>
-      <c r="H10" s="171"/>
-      <c r="I10" s="171"/>
-      <c r="J10" s="171"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="158"/>
+      <c r="E10" s="158"/>
+      <c r="F10" s="158"/>
+      <c r="G10" s="158"/>
+      <c r="H10" s="158"/>
+      <c r="I10" s="158"/>
+      <c r="J10" s="158"/>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="163" t="s">
+      <c r="B11" s="157" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="163"/>
-      <c r="D11" s="180"/>
-      <c r="E11" s="180"/>
-      <c r="F11" s="180"/>
-      <c r="G11" s="180"/>
-      <c r="H11" s="180"/>
-      <c r="I11" s="180"/>
-      <c r="J11" s="180"/>
+      <c r="C11" s="157"/>
+      <c r="D11" s="160"/>
+      <c r="E11" s="160"/>
+      <c r="F11" s="160"/>
+      <c r="G11" s="160"/>
+      <c r="H11" s="160"/>
+      <c r="I11" s="160"/>
+      <c r="J11" s="160"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="163" t="s">
+      <c r="B12" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="163"/>
-      <c r="D12" s="171"/>
-      <c r="E12" s="171"/>
-      <c r="F12" s="171"/>
-      <c r="G12" s="171"/>
-      <c r="H12" s="171"/>
-      <c r="I12" s="171"/>
-      <c r="J12" s="171"/>
+      <c r="C12" s="157"/>
+      <c r="D12" s="158"/>
+      <c r="E12" s="158"/>
+      <c r="F12" s="158"/>
+      <c r="G12" s="158"/>
+      <c r="H12" s="158"/>
+      <c r="I12" s="158"/>
+      <c r="J12" s="158"/>
     </row>
     <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="163" t="s">
+      <c r="B13" s="157" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="163"/>
+      <c r="C13" s="157"/>
       <c r="D13" s="15">
         <f>QuadroResumo!G10</f>
         <v>0</v>
       </c>
       <c r="E13" s="16"/>
-      <c r="F13" s="163" t="s">
+      <c r="F13" s="157" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="163"/>
+      <c r="G13" s="157"/>
       <c r="H13" s="15">
         <f>QuadroResumo!H10</f>
         <v>0</v>
@@ -4243,98 +4243,98 @@
       <c r="J13" s="18"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="165" t="s">
+      <c r="B14" s="161" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="165"/>
+      <c r="C14" s="161"/>
       <c r="D14" s="15">
         <f>SUMIF(Funções!D3:D202, "=RT1", Funções!Q3:Q202) + SUMIF(Funções!D3:D202, "=RT2", Funções!Q3:Q202)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="166"/>
-      <c r="F14" s="166"/>
-      <c r="G14" s="166"/>
-      <c r="H14" s="166"/>
-      <c r="I14" s="166"/>
+      <c r="E14" s="162"/>
+      <c r="F14" s="162"/>
+      <c r="G14" s="162"/>
+      <c r="H14" s="162"/>
+      <c r="I14" s="162"/>
       <c r="J14" s="19"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="167"/>
-      <c r="C15" s="167"/>
-      <c r="D15" s="167"/>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="167"/>
-      <c r="J15" s="167"/>
+      <c r="B15" s="163"/>
+      <c r="C15" s="163"/>
+      <c r="D15" s="163"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="163"/>
+      <c r="G15" s="163"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="163"/>
+      <c r="J15" s="163"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="156" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="155"/>
-      <c r="D16" s="155"/>
-      <c r="E16" s="155"/>
-      <c r="F16" s="155"/>
-      <c r="G16" s="155"/>
-      <c r="H16" s="155"/>
-      <c r="I16" s="155"/>
-      <c r="J16" s="155"/>
+      <c r="C16" s="156"/>
+      <c r="D16" s="156"/>
+      <c r="E16" s="156"/>
+      <c r="F16" s="156"/>
+      <c r="G16" s="156"/>
+      <c r="H16" s="156"/>
+      <c r="I16" s="156"/>
+      <c r="J16" s="156"/>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="163" t="s">
+      <c r="B17" s="157" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="163"/>
-      <c r="D17" s="169"/>
-      <c r="E17" s="169"/>
-      <c r="F17" s="169"/>
-      <c r="G17" s="169"/>
-      <c r="H17" s="169"/>
-      <c r="I17" s="169"/>
-      <c r="J17" s="169"/>
+      <c r="C17" s="157"/>
+      <c r="D17" s="164"/>
+      <c r="E17" s="164"/>
+      <c r="F17" s="164"/>
+      <c r="G17" s="164"/>
+      <c r="H17" s="164"/>
+      <c r="I17" s="164"/>
+      <c r="J17" s="164"/>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="163" t="s">
+      <c r="B18" s="157" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="163"/>
-      <c r="D18" s="169"/>
-      <c r="E18" s="169"/>
-      <c r="F18" s="169"/>
-      <c r="G18" s="169"/>
-      <c r="H18" s="169"/>
-      <c r="I18" s="169"/>
-      <c r="J18" s="169"/>
+      <c r="C18" s="157"/>
+      <c r="D18" s="164"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="164"/>
+      <c r="H18" s="164"/>
+      <c r="I18" s="164"/>
+      <c r="J18" s="164"/>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="163" t="s">
+      <c r="B19" s="157" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="163"/>
-      <c r="D19" s="170"/>
-      <c r="E19" s="170"/>
-      <c r="F19" s="170"/>
-      <c r="G19" s="170"/>
-      <c r="H19" s="170"/>
-      <c r="I19" s="170"/>
-      <c r="J19" s="170"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="165"/>
+      <c r="E19" s="165"/>
+      <c r="F19" s="165"/>
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165"/>
+      <c r="J19" s="165"/>
     </row>
     <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="163" t="s">
+      <c r="B20" s="157" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="163"/>
+      <c r="C20" s="157"/>
       <c r="D20" s="15">
         <f>QuadroResumo!G20</f>
         <v>0</v>
       </c>
       <c r="E20" s="16"/>
-      <c r="F20" s="163" t="s">
+      <c r="F20" s="157" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="163"/>
+      <c r="G20" s="157"/>
       <c r="H20" s="15">
         <f>QuadroResumo!H20</f>
         <v>0</v>
@@ -4343,60 +4343,60 @@
       <c r="J20" s="18"/>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="161" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="165"/>
+      <c r="C21" s="161"/>
       <c r="D21" s="15">
         <f>SUMIF(Funções!V3:V202, "=RT1", Funções!AG3:AG202) + SUMIF(Funções!V3:V202, "=RT2", Funções!AG3:AG202)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="166"/>
-      <c r="F21" s="166"/>
-      <c r="G21" s="166"/>
-      <c r="H21" s="166"/>
-      <c r="I21" s="166"/>
+      <c r="E21" s="162"/>
+      <c r="F21" s="162"/>
+      <c r="G21" s="162"/>
+      <c r="H21" s="162"/>
+      <c r="I21" s="162"/>
       <c r="J21" s="18"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="167"/>
-      <c r="C22" s="167"/>
-      <c r="D22" s="167"/>
-      <c r="E22" s="167"/>
-      <c r="F22" s="167"/>
-      <c r="G22" s="167"/>
-      <c r="H22" s="167"/>
-      <c r="I22" s="167"/>
-      <c r="J22" s="167"/>
+      <c r="B22" s="163"/>
+      <c r="C22" s="163"/>
+      <c r="D22" s="163"/>
+      <c r="E22" s="163"/>
+      <c r="F22" s="163"/>
+      <c r="G22" s="163"/>
+      <c r="H22" s="163"/>
+      <c r="I22" s="163"/>
+      <c r="J22" s="163"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="155" t="s">
+      <c r="B23" s="156" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="155"/>
-      <c r="D23" s="155"/>
-      <c r="E23" s="155"/>
-      <c r="F23" s="155"/>
-      <c r="G23" s="155"/>
-      <c r="H23" s="155"/>
-      <c r="I23" s="155"/>
-      <c r="J23" s="155"/>
+      <c r="C23" s="156"/>
+      <c r="D23" s="156"/>
+      <c r="E23" s="156"/>
+      <c r="F23" s="156"/>
+      <c r="G23" s="156"/>
+      <c r="H23" s="156"/>
+      <c r="I23" s="156"/>
+      <c r="J23" s="156"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="163" t="s">
+      <c r="B24" s="157" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="163"/>
+      <c r="C24" s="157"/>
       <c r="D24" s="20">
         <f>IFERROR(ROUND((D20-D13)/D13,2),0)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="168"/>
-      <c r="F24" s="168"/>
-      <c r="G24" s="168"/>
-      <c r="H24" s="168"/>
-      <c r="I24" s="168"/>
-      <c r="J24" s="168"/>
+      <c r="E24" s="166"/>
+      <c r="F24" s="166"/>
+      <c r="G24" s="166"/>
+      <c r="H24" s="166"/>
+      <c r="I24" s="166"/>
+      <c r="J24" s="166"/>
     </row>
     <row r="25" spans="2:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="14"/>
@@ -4410,15 +4410,15 @@
       <c r="J25" s="21"/>
     </row>
     <row r="26" spans="2:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="163" t="s">
+      <c r="B26" s="157" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="163"/>
-      <c r="D26" s="164">
+      <c r="C26" s="157"/>
+      <c r="D26" s="167">
         <v>19809</v>
       </c>
-      <c r="E26" s="164"/>
-      <c r="F26" s="164"/>
+      <c r="E26" s="167"/>
+      <c r="F26" s="167"/>
       <c r="G26" s="22" t="s">
         <v>28</v>
       </c>
@@ -4432,17 +4432,17 @@
       </c>
     </row>
     <row r="27" spans="2:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="163" t="s">
+      <c r="B27" s="157" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="163"/>
-      <c r="D27" s="164" t="s">
+      <c r="C27" s="157"/>
+      <c r="D27" s="167" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="164"/>
-      <c r="F27" s="164"/>
-      <c r="G27" s="164"/>
-      <c r="H27" s="164"/>
+      <c r="E27" s="167"/>
+      <c r="F27" s="167"/>
+      <c r="G27" s="167"/>
+      <c r="H27" s="167"/>
       <c r="I27" s="22" t="s">
         <v>4</v>
       </c>
@@ -4451,28 +4451,28 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="163" t="s">
+      <c r="B28" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="163"/>
-      <c r="D28" s="164"/>
-      <c r="E28" s="164"/>
-      <c r="F28" s="164"/>
-      <c r="G28" s="164"/>
-      <c r="H28" s="164"/>
+      <c r="C28" s="157"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167"/>
+      <c r="F28" s="167"/>
+      <c r="G28" s="167"/>
+      <c r="H28" s="167"/>
       <c r="I28" s="22" t="s">
         <v>4</v>
       </c>
       <c r="J28" s="25"/>
     </row>
     <row r="29" spans="2:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="162" t="s">
+      <c r="B29" s="168" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="163" t="s">
+      <c r="C29" s="157" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="163"/>
+      <c r="D29" s="157"/>
       <c r="E29" s="26"/>
       <c r="F29" s="27"/>
       <c r="G29" s="27"/>
@@ -4481,11 +4481,11 @@
       <c r="J29" s="27"/>
     </row>
     <row r="30" spans="2:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="162"/>
-      <c r="C30" s="163" t="s">
+      <c r="B30" s="168"/>
+      <c r="C30" s="157" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="163"/>
+      <c r="D30" s="157"/>
       <c r="E30" s="26"/>
       <c r="F30" s="27"/>
       <c r="G30" s="27"/>
@@ -4498,11 +4498,11 @@
       </c>
     </row>
     <row r="31" spans="2:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="162"/>
-      <c r="C31" s="163" t="s">
+      <c r="B31" s="168"/>
+      <c r="C31" s="157" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="163"/>
+      <c r="D31" s="157"/>
       <c r="E31" s="26"/>
       <c r="F31" s="27"/>
       <c r="G31" s="27"/>
@@ -4516,11 +4516,11 @@
       </c>
     </row>
     <row r="32" spans="2:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="162"/>
-      <c r="C32" s="163" t="s">
+      <c r="B32" s="168"/>
+      <c r="C32" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="163"/>
+      <c r="D32" s="157"/>
       <c r="E32" s="26"/>
       <c r="F32" s="27"/>
       <c r="G32" s="27"/>
@@ -4534,11 +4534,11 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="162"/>
-      <c r="C33" s="163" t="s">
+      <c r="B33" s="168"/>
+      <c r="C33" s="157" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="163"/>
+      <c r="D33" s="157"/>
       <c r="E33" s="26" t="s">
         <v>43</v>
       </c>
@@ -4554,11 +4554,11 @@
       </c>
     </row>
     <row r="34" spans="2:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="162"/>
-      <c r="C34" s="163" t="s">
+      <c r="B34" s="168"/>
+      <c r="C34" s="157" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="163"/>
+      <c r="D34" s="157"/>
       <c r="E34" s="26"/>
       <c r="F34" s="27"/>
       <c r="G34" s="27"/>
@@ -4572,11 +4572,11 @@
       </c>
     </row>
     <row r="35" spans="2:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="162"/>
-      <c r="C35" s="163" t="s">
+      <c r="B35" s="168"/>
+      <c r="C35" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="163"/>
+      <c r="D35" s="157"/>
       <c r="E35" s="26"/>
       <c r="F35" s="27"/>
       <c r="G35" s="27"/>
@@ -4590,11 +4590,11 @@
       </c>
     </row>
     <row r="36" spans="2:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="162"/>
-      <c r="C36" s="163" t="s">
+      <c r="B36" s="168"/>
+      <c r="C36" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="163"/>
+      <c r="D36" s="157"/>
       <c r="E36" s="26"/>
       <c r="F36" s="32" t="s">
         <v>50</v>
@@ -4605,297 +4605,279 @@
       <c r="J36" s="27"/>
     </row>
     <row r="37" spans="2:10" s="33" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="160" t="str">
+      <c r="B37" s="169" t="str">
         <f>CONCATENATE(B16," = ",D20," PF")</f>
         <v>Contagem Fábrica de Métricas = 0 PF</v>
       </c>
-      <c r="C37" s="160"/>
-      <c r="D37" s="160"/>
-      <c r="E37" s="160"/>
-      <c r="F37" s="160"/>
-      <c r="G37" s="160"/>
-      <c r="H37" s="160"/>
-      <c r="I37" s="160"/>
-      <c r="J37" s="160"/>
+      <c r="C37" s="169"/>
+      <c r="D37" s="169"/>
+      <c r="E37" s="169"/>
+      <c r="F37" s="169"/>
+      <c r="G37" s="169"/>
+      <c r="H37" s="169"/>
+      <c r="I37" s="169"/>
+      <c r="J37" s="169"/>
     </row>
     <row r="38" spans="2:10" s="33" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="160" t="str">
+      <c r="B38" s="169" t="str">
         <f>CONCATENATE(E20,":",H20," PF")</f>
         <v>:0 PF</v>
       </c>
-      <c r="C38" s="160"/>
-      <c r="D38" s="160"/>
-      <c r="E38" s="160"/>
-      <c r="F38" s="160"/>
-      <c r="G38" s="160"/>
-      <c r="H38" s="160"/>
-      <c r="I38" s="160"/>
-      <c r="J38" s="160"/>
+      <c r="C38" s="169"/>
+      <c r="D38" s="169"/>
+      <c r="E38" s="169"/>
+      <c r="F38" s="169"/>
+      <c r="G38" s="169"/>
+      <c r="H38" s="169"/>
+      <c r="I38" s="169"/>
+      <c r="J38" s="169"/>
     </row>
     <row r="39" spans="2:10" s="33" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="160" t="str">
+      <c r="B39" s="169" t="str">
         <f>CONCATENATE(B24,":",D24*100,"%")</f>
         <v xml:space="preserve">    % de Divergência:0%</v>
       </c>
-      <c r="C39" s="160"/>
-      <c r="D39" s="160"/>
-      <c r="E39" s="160"/>
-      <c r="F39" s="160"/>
-      <c r="G39" s="160"/>
-      <c r="H39" s="160"/>
-      <c r="I39" s="160"/>
-      <c r="J39" s="160"/>
+      <c r="C39" s="169"/>
+      <c r="D39" s="169"/>
+      <c r="E39" s="169"/>
+      <c r="F39" s="169"/>
+      <c r="G39" s="169"/>
+      <c r="H39" s="169"/>
+      <c r="I39" s="169"/>
+      <c r="J39" s="169"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B40" s="161"/>
-      <c r="C40" s="161"/>
-      <c r="D40" s="161"/>
-      <c r="E40" s="161"/>
-      <c r="F40" s="161"/>
-      <c r="G40" s="161"/>
-      <c r="H40" s="161"/>
-      <c r="I40" s="161"/>
+      <c r="B40" s="170"/>
+      <c r="C40" s="170"/>
+      <c r="D40" s="170"/>
+      <c r="E40" s="170"/>
+      <c r="F40" s="170"/>
+      <c r="G40" s="170"/>
+      <c r="H40" s="170"/>
+      <c r="I40" s="170"/>
       <c r="J40" s="34"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B41" s="155" t="s">
+      <c r="B41" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="155"/>
-      <c r="D41" s="155"/>
-      <c r="E41" s="155"/>
-      <c r="F41" s="155"/>
-      <c r="G41" s="155"/>
-      <c r="H41" s="155"/>
-      <c r="I41" s="155"/>
-      <c r="J41" s="155"/>
+      <c r="C41" s="156"/>
+      <c r="D41" s="156"/>
+      <c r="E41" s="156"/>
+      <c r="F41" s="156"/>
+      <c r="G41" s="156"/>
+      <c r="H41" s="156"/>
+      <c r="I41" s="156"/>
+      <c r="J41" s="156"/>
     </row>
     <row r="42" spans="2:10" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="154"/>
-      <c r="C42" s="154"/>
-      <c r="D42" s="154"/>
-      <c r="E42" s="154"/>
-      <c r="F42" s="154"/>
-      <c r="G42" s="154"/>
-      <c r="H42" s="154"/>
-      <c r="I42" s="154"/>
+      <c r="B42" s="171"/>
+      <c r="C42" s="171"/>
+      <c r="D42" s="171"/>
+      <c r="E42" s="171"/>
+      <c r="F42" s="171"/>
+      <c r="G42" s="171"/>
+      <c r="H42" s="171"/>
+      <c r="I42" s="171"/>
       <c r="J42" s="35"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B43" s="155" t="s">
+      <c r="B43" s="156" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="155"/>
-      <c r="D43" s="155"/>
-      <c r="E43" s="155"/>
-      <c r="F43" s="155"/>
-      <c r="G43" s="155"/>
-      <c r="H43" s="155"/>
-      <c r="I43" s="155"/>
-      <c r="J43" s="155"/>
+      <c r="C43" s="156"/>
+      <c r="D43" s="156"/>
+      <c r="E43" s="156"/>
+      <c r="F43" s="156"/>
+      <c r="G43" s="156"/>
+      <c r="H43" s="156"/>
+      <c r="I43" s="156"/>
+      <c r="J43" s="156"/>
     </row>
     <row r="44" spans="2:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="154"/>
-      <c r="C44" s="154"/>
-      <c r="D44" s="154"/>
-      <c r="E44" s="154"/>
-      <c r="F44" s="154"/>
-      <c r="G44" s="154"/>
-      <c r="H44" s="154"/>
-      <c r="I44" s="154"/>
+      <c r="B44" s="171"/>
+      <c r="C44" s="171"/>
+      <c r="D44" s="171"/>
+      <c r="E44" s="171"/>
+      <c r="F44" s="171"/>
+      <c r="G44" s="171"/>
+      <c r="H44" s="171"/>
+      <c r="I44" s="171"/>
       <c r="J44" s="36"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B45" s="155" t="s">
+      <c r="B45" s="156" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="155"/>
-      <c r="D45" s="155"/>
-      <c r="E45" s="155"/>
-      <c r="F45" s="155"/>
-      <c r="G45" s="155"/>
-      <c r="H45" s="155"/>
-      <c r="I45" s="155"/>
-      <c r="J45" s="155"/>
+      <c r="C45" s="156"/>
+      <c r="D45" s="156"/>
+      <c r="E45" s="156"/>
+      <c r="F45" s="156"/>
+      <c r="G45" s="156"/>
+      <c r="H45" s="156"/>
+      <c r="I45" s="156"/>
+      <c r="J45" s="156"/>
     </row>
     <row r="46" spans="2:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="154"/>
-      <c r="C46" s="154"/>
-      <c r="D46" s="154"/>
-      <c r="E46" s="154"/>
-      <c r="F46" s="154"/>
-      <c r="G46" s="154"/>
-      <c r="H46" s="154"/>
-      <c r="I46" s="154"/>
+      <c r="B46" s="171"/>
+      <c r="C46" s="171"/>
+      <c r="D46" s="171"/>
+      <c r="E46" s="171"/>
+      <c r="F46" s="171"/>
+      <c r="G46" s="171"/>
+      <c r="H46" s="171"/>
+      <c r="I46" s="171"/>
       <c r="J46" s="35"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B47" s="155" t="s">
+      <c r="B47" s="156" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="155"/>
-      <c r="D47" s="155"/>
-      <c r="E47" s="155"/>
-      <c r="F47" s="155"/>
-      <c r="G47" s="155"/>
-      <c r="H47" s="155"/>
-      <c r="I47" s="155"/>
-      <c r="J47" s="155"/>
+      <c r="C47" s="156"/>
+      <c r="D47" s="156"/>
+      <c r="E47" s="156"/>
+      <c r="F47" s="156"/>
+      <c r="G47" s="156"/>
+      <c r="H47" s="156"/>
+      <c r="I47" s="156"/>
+      <c r="J47" s="156"/>
     </row>
     <row r="48" spans="2:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="154"/>
-      <c r="C48" s="154"/>
-      <c r="D48" s="154"/>
-      <c r="E48" s="154"/>
-      <c r="F48" s="154"/>
-      <c r="G48" s="154"/>
-      <c r="H48" s="154"/>
-      <c r="I48" s="154"/>
+      <c r="B48" s="171"/>
+      <c r="C48" s="171"/>
+      <c r="D48" s="171"/>
+      <c r="E48" s="171"/>
+      <c r="F48" s="171"/>
+      <c r="G48" s="171"/>
+      <c r="H48" s="171"/>
+      <c r="I48" s="171"/>
       <c r="J48" s="35"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B49" s="155" t="s">
+      <c r="B49" s="156" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="155"/>
-      <c r="D49" s="155"/>
-      <c r="E49" s="155"/>
-      <c r="F49" s="155"/>
-      <c r="G49" s="155"/>
-      <c r="H49" s="155"/>
-      <c r="I49" s="155"/>
-      <c r="J49" s="155"/>
+      <c r="C49" s="156"/>
+      <c r="D49" s="156"/>
+      <c r="E49" s="156"/>
+      <c r="F49" s="156"/>
+      <c r="G49" s="156"/>
+      <c r="H49" s="156"/>
+      <c r="I49" s="156"/>
+      <c r="J49" s="156"/>
     </row>
     <row r="50" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="157" t="s">
+      <c r="B50" s="172" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="157"/>
-      <c r="D50" s="158"/>
-      <c r="E50" s="158"/>
-      <c r="F50" s="158"/>
-      <c r="G50" s="158"/>
-      <c r="H50" s="158"/>
-      <c r="I50" s="158"/>
-      <c r="J50" s="158"/>
+      <c r="C50" s="172"/>
+      <c r="D50" s="173"/>
+      <c r="E50" s="173"/>
+      <c r="F50" s="173"/>
+      <c r="G50" s="173"/>
+      <c r="H50" s="173"/>
+      <c r="I50" s="173"/>
+      <c r="J50" s="173"/>
     </row>
     <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="157" t="s">
+      <c r="B51" s="172" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="157"/>
-      <c r="D51" s="158"/>
-      <c r="E51" s="158"/>
-      <c r="F51" s="158"/>
-      <c r="G51" s="158"/>
-      <c r="H51" s="158"/>
-      <c r="I51" s="158"/>
-      <c r="J51" s="158"/>
+      <c r="C51" s="172"/>
+      <c r="D51" s="173"/>
+      <c r="E51" s="173"/>
+      <c r="F51" s="173"/>
+      <c r="G51" s="173"/>
+      <c r="H51" s="173"/>
+      <c r="I51" s="173"/>
+      <c r="J51" s="173"/>
     </row>
     <row r="52" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="157" t="s">
+      <c r="B52" s="172" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="157"/>
-      <c r="D52" s="159"/>
-      <c r="E52" s="159"/>
-      <c r="F52" s="159"/>
-      <c r="G52" s="159"/>
-      <c r="H52" s="159"/>
-      <c r="I52" s="159"/>
-      <c r="J52" s="159"/>
+      <c r="C52" s="172"/>
+      <c r="D52" s="175"/>
+      <c r="E52" s="175"/>
+      <c r="F52" s="175"/>
+      <c r="G52" s="175"/>
+      <c r="H52" s="175"/>
+      <c r="I52" s="175"/>
+      <c r="J52" s="175"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B53" s="155" t="s">
+      <c r="B53" s="156" t="s">
         <v>59</v>
       </c>
-      <c r="C53" s="155"/>
-      <c r="D53" s="155"/>
-      <c r="E53" s="155"/>
-      <c r="F53" s="155"/>
-      <c r="G53" s="155"/>
-      <c r="H53" s="155"/>
-      <c r="I53" s="155"/>
-      <c r="J53" s="155"/>
+      <c r="C53" s="156"/>
+      <c r="D53" s="156"/>
+      <c r="E53" s="156"/>
+      <c r="F53" s="156"/>
+      <c r="G53" s="156"/>
+      <c r="H53" s="156"/>
+      <c r="I53" s="156"/>
+      <c r="J53" s="156"/>
     </row>
     <row r="54" spans="2:10" ht="87" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="154"/>
-      <c r="C54" s="154"/>
-      <c r="D54" s="154"/>
-      <c r="E54" s="154"/>
-      <c r="F54" s="154"/>
-      <c r="G54" s="154"/>
-      <c r="H54" s="154"/>
-      <c r="I54" s="154"/>
+      <c r="B54" s="171"/>
+      <c r="C54" s="171"/>
+      <c r="D54" s="171"/>
+      <c r="E54" s="171"/>
+      <c r="F54" s="171"/>
+      <c r="G54" s="171"/>
+      <c r="H54" s="171"/>
+      <c r="I54" s="171"/>
       <c r="J54" s="35"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B55" s="155" t="s">
+      <c r="B55" s="156" t="s">
         <v>60</v>
       </c>
-      <c r="C55" s="155"/>
-      <c r="D55" s="155"/>
-      <c r="E55" s="155"/>
-      <c r="F55" s="155"/>
-      <c r="G55" s="155"/>
-      <c r="H55" s="155"/>
-      <c r="I55" s="155"/>
-      <c r="J55" s="155"/>
+      <c r="C55" s="156"/>
+      <c r="D55" s="156"/>
+      <c r="E55" s="156"/>
+      <c r="F55" s="156"/>
+      <c r="G55" s="156"/>
+      <c r="H55" s="156"/>
+      <c r="I55" s="156"/>
+      <c r="J55" s="156"/>
     </row>
     <row r="56" spans="2:10" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="156"/>
-      <c r="C56" s="156"/>
-      <c r="D56" s="156"/>
-      <c r="E56" s="156"/>
-      <c r="F56" s="156"/>
-      <c r="G56" s="156"/>
-      <c r="H56" s="156"/>
-      <c r="I56" s="156"/>
-      <c r="J56" s="156"/>
+      <c r="B56" s="174"/>
+      <c r="C56" s="174"/>
+      <c r="D56" s="174"/>
+      <c r="E56" s="174"/>
+      <c r="F56" s="174"/>
+      <c r="G56" s="174"/>
+      <c r="H56" s="174"/>
+      <c r="I56" s="174"/>
+      <c r="J56" s="174"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:J12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:J18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="B54:I54"/>
+    <mergeCell ref="B55:J55"/>
+    <mergeCell ref="B56:J56"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:J51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:J52"/>
+    <mergeCell ref="B53:J53"/>
+    <mergeCell ref="B47:J47"/>
+    <mergeCell ref="B48:I48"/>
+    <mergeCell ref="B49:J49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:J50"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="B43:J43"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B45:J45"/>
+    <mergeCell ref="B46:I46"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="B38:J38"/>
+    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="B41:J41"/>
     <mergeCell ref="B29:B36"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
@@ -4905,29 +4887,47 @@
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="B38:J38"/>
-    <mergeCell ref="B39:J39"/>
-    <mergeCell ref="B40:I40"/>
-    <mergeCell ref="B41:J41"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="B43:J43"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="B45:J45"/>
-    <mergeCell ref="B46:I46"/>
-    <mergeCell ref="B47:J47"/>
-    <mergeCell ref="B48:I48"/>
-    <mergeCell ref="B49:J49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:J50"/>
-    <mergeCell ref="B54:I54"/>
-    <mergeCell ref="B55:J55"/>
-    <mergeCell ref="B56:J56"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:J51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:J52"/>
-    <mergeCell ref="B53:J53"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:J18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:J12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:J7"/>
   </mergeCells>
   <conditionalFormatting sqref="B5">
     <cfRule type="expression" dxfId="268" priority="2">
@@ -4979,13 +4979,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="50" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
       <c r="F1" s="45"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
@@ -5537,43 +5537,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="176" t="s">
+      <c r="B1" s="177" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="176"/>
-      <c r="L1" s="176"/>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176"/>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="176"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="177"/>
       <c r="S1" s="92"/>
-      <c r="T1" s="177" t="s">
+      <c r="T1" s="178" t="s">
         <v>72</v>
       </c>
-      <c r="U1" s="177"/>
-      <c r="V1" s="177"/>
-      <c r="W1" s="177"/>
-      <c r="X1" s="177"/>
-      <c r="Y1" s="177"/>
-      <c r="Z1" s="177"/>
-      <c r="AA1" s="177"/>
-      <c r="AB1" s="177"/>
-      <c r="AC1" s="177"/>
-      <c r="AD1" s="177"/>
-      <c r="AE1" s="177"/>
-      <c r="AF1" s="177"/>
-      <c r="AG1" s="177"/>
-      <c r="AH1" s="177"/>
+      <c r="U1" s="178"/>
+      <c r="V1" s="178"/>
+      <c r="W1" s="178"/>
+      <c r="X1" s="178"/>
+      <c r="Y1" s="178"/>
+      <c r="Z1" s="178"/>
+      <c r="AA1" s="178"/>
+      <c r="AB1" s="178"/>
+      <c r="AC1" s="178"/>
+      <c r="AD1" s="178"/>
+      <c r="AE1" s="178"/>
+      <c r="AF1" s="178"/>
+      <c r="AG1" s="178"/>
+      <c r="AH1" s="178"/>
       <c r="AI1" s="92"/>
       <c r="AJ1" s="93" t="s">
         <v>73</v>
@@ -24958,15 +24958,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="179" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="179"/>
+      <c r="H2" s="179"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="123"/>
@@ -25221,15 +25221,15 @@
       <c r="J11" s="126"/>
     </row>
     <row r="12" spans="2:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="178" t="s">
+      <c r="B12" s="179" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="178"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="178"/>
-      <c r="F12" s="178"/>
-      <c r="G12" s="178"/>
-      <c r="H12" s="178"/>
+      <c r="C12" s="179"/>
+      <c r="D12" s="179"/>
+      <c r="E12" s="179"/>
+      <c r="F12" s="179"/>
+      <c r="G12" s="179"/>
+      <c r="H12" s="179"/>
       <c r="I12" s="126"/>
       <c r="J12" s="126"/>
     </row>
@@ -25511,13 +25511,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="180" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
     </row>
     <row r="2" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="132" t="s">

</xml_diff>

<commit_message>
Ajustar planilhas - BASIS-241480
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/reports/planilhas/modelo3-anac.xlsx
+++ b/backend/src/main/resources/reports/planilhas/modelo3-anac.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wilson\Downloads\ModeloPlanilhaAbaco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E71FBAFF-D509-4B90-B8B6-2661DB4608B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B9A53CA-C638-447D-9CEC-5CF2E9F430F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32770" yWindow="32770" windowWidth="19200" windowHeight="6930" activeTab="1"/>
   </bookViews>
@@ -2052,25 +2052,6 @@
     <xf numFmtId="0" fontId="52" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2087,8 +2068,27 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -2127,6 +2127,9 @@
     <xf numFmtId="0" fontId="56" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -2134,9 +2137,6 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3758,7 +3758,7 @@
         <xdr:cNvPr id="7169" name="Imagem 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33CDED7A-1313-42E0-898C-DE52D9CD8233}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38125536-A8F5-4FF3-9F77-DC297A6C4982}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4789,17 +4789,17 @@
       <c r="J1" s="64"/>
     </row>
     <row r="2" spans="2:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="208" t="s">
+      <c r="B2" s="206" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="208"/>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
-      <c r="G2" s="208"/>
-      <c r="H2" s="208"/>
-      <c r="I2" s="208"/>
-      <c r="J2" s="208"/>
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="206"/>
+      <c r="F2" s="206"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="206"/>
+      <c r="I2" s="206"/>
+      <c r="J2" s="206"/>
     </row>
     <row r="3" spans="2:10" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="65"/>
@@ -4867,10 +4867,10 @@
       <c r="J6" s="197"/>
     </row>
     <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="188" t="s">
+      <c r="B7" s="182" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="188"/>
+      <c r="C7" s="182"/>
       <c r="D7" s="194"/>
       <c r="E7" s="194"/>
       <c r="F7" s="194"/>
@@ -4880,10 +4880,10 @@
       <c r="J7" s="194"/>
     </row>
     <row r="8" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="188" t="s">
+      <c r="B8" s="182" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="188"/>
+      <c r="C8" s="182"/>
       <c r="D8" s="210"/>
       <c r="E8" s="210"/>
       <c r="F8" s="210"/>
@@ -4893,10 +4893,10 @@
       <c r="J8" s="210"/>
     </row>
     <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="188" t="s">
+      <c r="B9" s="182" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="188"/>
+      <c r="C9" s="182"/>
       <c r="D9" s="194"/>
       <c r="E9" s="194"/>
       <c r="F9" s="194"/>
@@ -4906,10 +4906,10 @@
       <c r="J9" s="194"/>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="188" t="s">
+      <c r="B10" s="182" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="188"/>
+      <c r="C10" s="182"/>
       <c r="D10" s="194"/>
       <c r="E10" s="194"/>
       <c r="F10" s="194"/>
@@ -4919,23 +4919,23 @@
       <c r="J10" s="194"/>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="188" t="s">
+      <c r="B11" s="182" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="188"/>
-      <c r="D11" s="189"/>
-      <c r="E11" s="189"/>
-      <c r="F11" s="189"/>
-      <c r="G11" s="189"/>
-      <c r="H11" s="189"/>
-      <c r="I11" s="189"/>
-      <c r="J11" s="189"/>
+      <c r="C11" s="182"/>
+      <c r="D11" s="183"/>
+      <c r="E11" s="183"/>
+      <c r="F11" s="183"/>
+      <c r="G11" s="183"/>
+      <c r="H11" s="183"/>
+      <c r="I11" s="183"/>
+      <c r="J11" s="183"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="188" t="s">
+      <c r="B12" s="182" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="188"/>
+      <c r="C12" s="182"/>
       <c r="D12" s="194"/>
       <c r="E12" s="194"/>
       <c r="F12" s="194"/>
@@ -4945,19 +4945,19 @@
       <c r="J12" s="194"/>
     </row>
     <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="188" t="s">
+      <c r="B13" s="182" t="s">
         <v>184</v>
       </c>
-      <c r="C13" s="188"/>
+      <c r="C13" s="182"/>
       <c r="D13" s="68">
         <f>QuadroResumo!G10</f>
         <v>0</v>
       </c>
       <c r="E13" s="125"/>
-      <c r="F13" s="188" t="s">
+      <c r="F13" s="182" t="s">
         <v>183</v>
       </c>
-      <c r="G13" s="188"/>
+      <c r="G13" s="182"/>
       <c r="H13" s="68">
         <f>QuadroResumo!H10</f>
         <v>0</v>
@@ -4966,31 +4966,31 @@
       <c r="J13" s="127"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="184" t="s">
+      <c r="B14" s="191" t="s">
         <v>179</v>
       </c>
-      <c r="C14" s="185"/>
+      <c r="C14" s="192"/>
       <c r="D14" s="68">
         <f>SUMIF(Funções!D3:'Funções'!D202, "=RT1", Funções!Q3:Q202) + SUMIF(Funções!D3:'Funções'!D202, "=RT2", Funções!Q3:Q202)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="182"/>
-      <c r="F14" s="183"/>
-      <c r="G14" s="183"/>
-      <c r="H14" s="183"/>
-      <c r="I14" s="183"/>
+      <c r="E14" s="187"/>
+      <c r="F14" s="188"/>
+      <c r="G14" s="188"/>
+      <c r="H14" s="188"/>
+      <c r="I14" s="188"/>
       <c r="J14" s="69"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="182"/>
-      <c r="C15" s="183"/>
-      <c r="D15" s="183"/>
-      <c r="E15" s="183"/>
-      <c r="F15" s="183"/>
-      <c r="G15" s="183"/>
-      <c r="H15" s="183"/>
-      <c r="I15" s="183"/>
-      <c r="J15" s="186"/>
+      <c r="B15" s="187"/>
+      <c r="C15" s="188"/>
+      <c r="D15" s="188"/>
+      <c r="E15" s="188"/>
+      <c r="F15" s="188"/>
+      <c r="G15" s="188"/>
+      <c r="H15" s="188"/>
+      <c r="I15" s="188"/>
+      <c r="J15" s="189"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="195" t="s">
@@ -5006,10 +5006,10 @@
       <c r="J16" s="197"/>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="188" t="s">
+      <c r="B17" s="182" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="188"/>
+      <c r="C17" s="182"/>
       <c r="D17" s="198"/>
       <c r="E17" s="198"/>
       <c r="F17" s="198"/>
@@ -5019,10 +5019,10 @@
       <c r="J17" s="198"/>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="188" t="s">
+      <c r="B18" s="182" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="188"/>
+      <c r="C18" s="182"/>
       <c r="D18" s="198"/>
       <c r="E18" s="198"/>
       <c r="F18" s="198"/>
@@ -5032,32 +5032,32 @@
       <c r="J18" s="198"/>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="188" t="s">
+      <c r="B19" s="182" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="188"/>
-      <c r="D19" s="187"/>
-      <c r="E19" s="187"/>
-      <c r="F19" s="187"/>
-      <c r="G19" s="187"/>
-      <c r="H19" s="187"/>
-      <c r="I19" s="187"/>
-      <c r="J19" s="187"/>
+      <c r="C19" s="182"/>
+      <c r="D19" s="193"/>
+      <c r="E19" s="193"/>
+      <c r="F19" s="193"/>
+      <c r="G19" s="193"/>
+      <c r="H19" s="193"/>
+      <c r="I19" s="193"/>
+      <c r="J19" s="193"/>
     </row>
     <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="188" t="s">
+      <c r="B20" s="182" t="s">
         <v>184</v>
       </c>
-      <c r="C20" s="188"/>
+      <c r="C20" s="182"/>
       <c r="D20" s="68">
         <f>QuadroResumo!G20</f>
         <v>0</v>
       </c>
       <c r="E20" s="125"/>
-      <c r="F20" s="188" t="s">
+      <c r="F20" s="182" t="s">
         <v>183</v>
       </c>
-      <c r="G20" s="188"/>
+      <c r="G20" s="182"/>
       <c r="H20" s="68">
         <f>QuadroResumo!H20</f>
         <v>0</v>
@@ -5066,60 +5066,60 @@
       <c r="J20" s="127"/>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="184" t="s">
+      <c r="B21" s="191" t="s">
         <v>179</v>
       </c>
-      <c r="C21" s="185"/>
+      <c r="C21" s="192"/>
       <c r="D21" s="68">
         <f>SUMIF(Funções!V3:'Funções'!V202, "=RT1", Funções!AG3:AG202) + SUMIF(Funções!V3:'Funções'!V202, "=RT2", Funções!AG3:AG202)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="182"/>
-      <c r="F21" s="183"/>
-      <c r="G21" s="183"/>
-      <c r="H21" s="183"/>
-      <c r="I21" s="183"/>
+      <c r="E21" s="187"/>
+      <c r="F21" s="188"/>
+      <c r="G21" s="188"/>
+      <c r="H21" s="188"/>
+      <c r="I21" s="188"/>
       <c r="J21" s="70"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="182"/>
-      <c r="C22" s="183"/>
-      <c r="D22" s="183"/>
-      <c r="E22" s="183"/>
-      <c r="F22" s="183"/>
-      <c r="G22" s="183"/>
-      <c r="H22" s="183"/>
-      <c r="I22" s="183"/>
-      <c r="J22" s="186"/>
+      <c r="B22" s="187"/>
+      <c r="C22" s="188"/>
+      <c r="D22" s="188"/>
+      <c r="E22" s="188"/>
+      <c r="F22" s="188"/>
+      <c r="G22" s="188"/>
+      <c r="H22" s="188"/>
+      <c r="I22" s="188"/>
+      <c r="J22" s="189"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="193" t="s">
+      <c r="B23" s="190" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="193"/>
-      <c r="D23" s="193"/>
-      <c r="E23" s="193"/>
-      <c r="F23" s="193"/>
-      <c r="G23" s="193"/>
-      <c r="H23" s="193"/>
-      <c r="I23" s="193"/>
-      <c r="J23" s="193"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="190"/>
+      <c r="F23" s="190"/>
+      <c r="G23" s="190"/>
+      <c r="H23" s="190"/>
+      <c r="I23" s="190"/>
+      <c r="J23" s="190"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="188" t="s">
+      <c r="B24" s="182" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="188"/>
+      <c r="C24" s="182"/>
       <c r="D24" s="71">
         <f>IFERROR(ROUND((D20-D13)/D13,2),0)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="190"/>
-      <c r="F24" s="191"/>
-      <c r="G24" s="191"/>
-      <c r="H24" s="191"/>
-      <c r="I24" s="191"/>
-      <c r="J24" s="192"/>
+      <c r="E24" s="184"/>
+      <c r="F24" s="185"/>
+      <c r="G24" s="185"/>
+      <c r="H24" s="185"/>
+      <c r="I24" s="185"/>
+      <c r="J24" s="186"/>
     </row>
     <row r="25" spans="2:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="72"/>
@@ -5133,10 +5133,10 @@
       <c r="J25" s="73"/>
     </row>
     <row r="26" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="188" t="s">
+      <c r="B26" s="182" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="188"/>
+      <c r="C26" s="182"/>
       <c r="D26" s="199">
         <v>19809</v>
       </c>
@@ -5155,10 +5155,10 @@
       </c>
     </row>
     <row r="27" spans="2:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="188" t="s">
+      <c r="B27" s="182" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="188"/>
+      <c r="C27" s="182"/>
       <c r="D27" s="199" t="s">
         <v>50</v>
       </c>
@@ -5174,10 +5174,10 @@
       </c>
     </row>
     <row r="28" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="188" t="s">
+      <c r="B28" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="188"/>
+      <c r="C28" s="182"/>
       <c r="D28" s="199"/>
       <c r="E28" s="199"/>
       <c r="F28" s="199"/>
@@ -5192,10 +5192,10 @@
       <c r="B29" s="212" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="188" t="s">
+      <c r="C29" s="182" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="188"/>
+      <c r="D29" s="182"/>
       <c r="E29" s="78"/>
       <c r="F29" s="79"/>
       <c r="G29" s="79"/>
@@ -5205,10 +5205,10 @@
     </row>
     <row r="30" spans="2:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="212"/>
-      <c r="C30" s="188" t="s">
+      <c r="C30" s="182" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="188"/>
+      <c r="D30" s="182"/>
       <c r="E30" s="78"/>
       <c r="F30" s="79"/>
       <c r="G30" s="79"/>
@@ -5222,10 +5222,10 @@
     </row>
     <row r="31" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B31" s="212"/>
-      <c r="C31" s="188" t="s">
+      <c r="C31" s="182" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="188"/>
+      <c r="D31" s="182"/>
       <c r="E31" s="78"/>
       <c r="F31" s="79"/>
       <c r="G31" s="79"/>
@@ -5240,10 +5240,10 @@
     </row>
     <row r="32" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B32" s="212"/>
-      <c r="C32" s="188" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="188"/>
+      <c r="C32" s="182" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="182"/>
       <c r="E32" s="78"/>
       <c r="F32" s="79"/>
       <c r="G32" s="79"/>
@@ -5258,10 +5258,10 @@
     </row>
     <row r="33" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B33" s="212"/>
-      <c r="C33" s="188" t="s">
+      <c r="C33" s="182" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="188"/>
+      <c r="D33" s="182"/>
       <c r="E33" s="78" t="s">
         <v>51</v>
       </c>
@@ -5278,10 +5278,10 @@
     </row>
     <row r="34" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B34" s="212"/>
-      <c r="C34" s="188" t="s">
+      <c r="C34" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="188"/>
+      <c r="D34" s="182"/>
       <c r="E34" s="78"/>
       <c r="F34" s="79"/>
       <c r="G34" s="79"/>
@@ -5296,10 +5296,10 @@
     </row>
     <row r="35" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B35" s="212"/>
-      <c r="C35" s="188" t="s">
+      <c r="C35" s="182" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="188"/>
+      <c r="D35" s="182"/>
       <c r="E35" s="78"/>
       <c r="F35" s="79"/>
       <c r="G35" s="79"/>
@@ -5314,10 +5314,10 @@
     </row>
     <row r="36" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B36" s="212"/>
-      <c r="C36" s="188" t="s">
+      <c r="C36" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="188"/>
+      <c r="D36" s="182"/>
       <c r="E36" s="78"/>
       <c r="F36" s="84" t="s">
         <v>34</v>
@@ -5381,113 +5381,113 @@
       <c r="J40" s="86"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B41" s="193" t="s">
+      <c r="B41" s="190" t="s">
         <v>95</v>
       </c>
-      <c r="C41" s="193"/>
-      <c r="D41" s="193"/>
-      <c r="E41" s="193"/>
-      <c r="F41" s="193"/>
-      <c r="G41" s="193"/>
-      <c r="H41" s="193"/>
-      <c r="I41" s="193"/>
-      <c r="J41" s="193"/>
+      <c r="C41" s="190"/>
+      <c r="D41" s="190"/>
+      <c r="E41" s="190"/>
+      <c r="F41" s="190"/>
+      <c r="G41" s="190"/>
+      <c r="H41" s="190"/>
+      <c r="I41" s="190"/>
+      <c r="J41" s="190"/>
     </row>
     <row r="42" spans="2:10" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="206"/>
-      <c r="C42" s="207"/>
-      <c r="D42" s="207"/>
-      <c r="E42" s="207"/>
-      <c r="F42" s="207"/>
-      <c r="G42" s="207"/>
-      <c r="H42" s="207"/>
-      <c r="I42" s="207"/>
+      <c r="B42" s="207"/>
+      <c r="C42" s="208"/>
+      <c r="D42" s="208"/>
+      <c r="E42" s="208"/>
+      <c r="F42" s="208"/>
+      <c r="G42" s="208"/>
+      <c r="H42" s="208"/>
+      <c r="I42" s="208"/>
       <c r="J42" s="87"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B43" s="193" t="s">
+      <c r="B43" s="190" t="s">
         <v>96</v>
       </c>
-      <c r="C43" s="193"/>
-      <c r="D43" s="193"/>
-      <c r="E43" s="193"/>
-      <c r="F43" s="193"/>
-      <c r="G43" s="193"/>
-      <c r="H43" s="193"/>
-      <c r="I43" s="193"/>
-      <c r="J43" s="193"/>
+      <c r="C43" s="190"/>
+      <c r="D43" s="190"/>
+      <c r="E43" s="190"/>
+      <c r="F43" s="190"/>
+      <c r="G43" s="190"/>
+      <c r="H43" s="190"/>
+      <c r="I43" s="190"/>
+      <c r="J43" s="190"/>
     </row>
     <row r="44" spans="2:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="206"/>
-      <c r="C44" s="207"/>
-      <c r="D44" s="207"/>
-      <c r="E44" s="207"/>
-      <c r="F44" s="207"/>
-      <c r="G44" s="207"/>
-      <c r="H44" s="207"/>
-      <c r="I44" s="207"/>
+      <c r="B44" s="207"/>
+      <c r="C44" s="208"/>
+      <c r="D44" s="208"/>
+      <c r="E44" s="208"/>
+      <c r="F44" s="208"/>
+      <c r="G44" s="208"/>
+      <c r="H44" s="208"/>
+      <c r="I44" s="208"/>
       <c r="J44" s="88"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B45" s="193" t="s">
+      <c r="B45" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="193"/>
-      <c r="D45" s="193"/>
-      <c r="E45" s="193"/>
-      <c r="F45" s="193"/>
-      <c r="G45" s="193"/>
-      <c r="H45" s="193"/>
-      <c r="I45" s="193"/>
-      <c r="J45" s="193"/>
+      <c r="C45" s="190"/>
+      <c r="D45" s="190"/>
+      <c r="E45" s="190"/>
+      <c r="F45" s="190"/>
+      <c r="G45" s="190"/>
+      <c r="H45" s="190"/>
+      <c r="I45" s="190"/>
+      <c r="J45" s="190"/>
     </row>
     <row r="46" spans="2:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="206"/>
-      <c r="C46" s="207"/>
-      <c r="D46" s="207"/>
-      <c r="E46" s="207"/>
-      <c r="F46" s="207"/>
-      <c r="G46" s="207"/>
-      <c r="H46" s="207"/>
-      <c r="I46" s="207"/>
+      <c r="B46" s="207"/>
+      <c r="C46" s="208"/>
+      <c r="D46" s="208"/>
+      <c r="E46" s="208"/>
+      <c r="F46" s="208"/>
+      <c r="G46" s="208"/>
+      <c r="H46" s="208"/>
+      <c r="I46" s="208"/>
       <c r="J46" s="87"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B47" s="193" t="s">
+      <c r="B47" s="190" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="193"/>
-      <c r="D47" s="193"/>
-      <c r="E47" s="193"/>
-      <c r="F47" s="193"/>
-      <c r="G47" s="193"/>
-      <c r="H47" s="193"/>
-      <c r="I47" s="193"/>
-      <c r="J47" s="193"/>
+      <c r="C47" s="190"/>
+      <c r="D47" s="190"/>
+      <c r="E47" s="190"/>
+      <c r="F47" s="190"/>
+      <c r="G47" s="190"/>
+      <c r="H47" s="190"/>
+      <c r="I47" s="190"/>
+      <c r="J47" s="190"/>
     </row>
     <row r="48" spans="2:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="206"/>
-      <c r="C48" s="207"/>
-      <c r="D48" s="207"/>
-      <c r="E48" s="207"/>
-      <c r="F48" s="207"/>
-      <c r="G48" s="207"/>
-      <c r="H48" s="207"/>
-      <c r="I48" s="207"/>
+      <c r="B48" s="207"/>
+      <c r="C48" s="208"/>
+      <c r="D48" s="208"/>
+      <c r="E48" s="208"/>
+      <c r="F48" s="208"/>
+      <c r="G48" s="208"/>
+      <c r="H48" s="208"/>
+      <c r="I48" s="208"/>
       <c r="J48" s="87"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B49" s="193" t="s">
+      <c r="B49" s="190" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="193"/>
-      <c r="D49" s="193"/>
-      <c r="E49" s="193"/>
-      <c r="F49" s="193"/>
-      <c r="G49" s="193"/>
-      <c r="H49" s="193"/>
-      <c r="I49" s="193"/>
-      <c r="J49" s="193"/>
+      <c r="C49" s="190"/>
+      <c r="D49" s="190"/>
+      <c r="E49" s="190"/>
+      <c r="F49" s="190"/>
+      <c r="G49" s="190"/>
+      <c r="H49" s="190"/>
+      <c r="I49" s="190"/>
+      <c r="J49" s="190"/>
     </row>
     <row r="50" spans="2:10" ht="14.5" x14ac:dyDescent="0.3">
       <c r="B50" s="201" t="s">
@@ -5529,41 +5529,41 @@
       <c r="J52" s="204"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B53" s="193" t="s">
+      <c r="B53" s="190" t="s">
         <v>44</v>
       </c>
-      <c r="C53" s="193"/>
-      <c r="D53" s="193"/>
-      <c r="E53" s="193"/>
-      <c r="F53" s="193"/>
-      <c r="G53" s="193"/>
-      <c r="H53" s="193"/>
-      <c r="I53" s="193"/>
-      <c r="J53" s="193"/>
+      <c r="C53" s="190"/>
+      <c r="D53" s="190"/>
+      <c r="E53" s="190"/>
+      <c r="F53" s="190"/>
+      <c r="G53" s="190"/>
+      <c r="H53" s="190"/>
+      <c r="I53" s="190"/>
+      <c r="J53" s="190"/>
     </row>
     <row r="54" spans="2:10" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="206"/>
-      <c r="C54" s="207"/>
-      <c r="D54" s="207"/>
-      <c r="E54" s="207"/>
-      <c r="F54" s="207"/>
-      <c r="G54" s="207"/>
-      <c r="H54" s="207"/>
-      <c r="I54" s="207"/>
+      <c r="B54" s="207"/>
+      <c r="C54" s="208"/>
+      <c r="D54" s="208"/>
+      <c r="E54" s="208"/>
+      <c r="F54" s="208"/>
+      <c r="G54" s="208"/>
+      <c r="H54" s="208"/>
+      <c r="I54" s="208"/>
       <c r="J54" s="87"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B55" s="193" t="s">
+      <c r="B55" s="190" t="s">
         <v>47</v>
       </c>
-      <c r="C55" s="193"/>
-      <c r="D55" s="193"/>
-      <c r="E55" s="193"/>
-      <c r="F55" s="193"/>
-      <c r="G55" s="193"/>
-      <c r="H55" s="193"/>
-      <c r="I55" s="193"/>
-      <c r="J55" s="193"/>
+      <c r="C55" s="190"/>
+      <c r="D55" s="190"/>
+      <c r="E55" s="190"/>
+      <c r="F55" s="190"/>
+      <c r="G55" s="190"/>
+      <c r="H55" s="190"/>
+      <c r="I55" s="190"/>
+      <c r="J55" s="190"/>
     </row>
     <row r="56" spans="2:10" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="200"/>
@@ -5579,38 +5579,37 @@
   </sheetData>
   <sheetProtection sheet="1" selectLockedCells="1"/>
   <mergeCells count="73">
-    <mergeCell ref="B39:J39"/>
-    <mergeCell ref="B42:I42"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C35:D35"/>
-    <mergeCell ref="B45:J45"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="B29:B36"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B40:I40"/>
     <mergeCell ref="B38:J38"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D52:J52"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="B42:I42"/>
     <mergeCell ref="B54:I54"/>
     <mergeCell ref="B48:I48"/>
     <mergeCell ref="B46:I46"/>
     <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="B45:J45"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="D9:J9"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B6:J6"/>
+    <mergeCell ref="D52:J52"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="B29:B36"/>
     <mergeCell ref="B55:J55"/>
     <mergeCell ref="B56:J56"/>
     <mergeCell ref="B47:J47"/>
@@ -5627,6 +5626,8 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D12:J12"/>
     <mergeCell ref="B16:J16"/>
@@ -5634,7 +5635,14 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:J17"/>
     <mergeCell ref="F13:G13"/>
-    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="D11:J11"/>
     <mergeCell ref="E24:J24"/>
     <mergeCell ref="B15:J15"/>
@@ -5644,14 +5652,6 @@
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B23:J23"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F20:G20"/>
   </mergeCells>
   <conditionalFormatting sqref="B5">
     <cfRule type="expression" dxfId="268" priority="6">
@@ -6221,10 +6221,10 @@
   <dimension ref="A1:AK371"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V3" sqref="V3"/>
+      <selection pane="bottomRight" activeCell="U3" sqref="U3:U202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6507,7 +6507,7 @@
     <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="55"/>
       <c r="B4" s="135"/>
-      <c r="C4" s="55"/>
+      <c r="C4" s="147"/>
       <c r="D4" s="55"/>
       <c r="E4" s="55"/>
       <c r="F4" s="155"/>
@@ -6598,7 +6598,7 @@
     <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="55"/>
       <c r="B5" s="135"/>
-      <c r="C5" s="55"/>
+      <c r="C5" s="147"/>
       <c r="D5" s="55"/>
       <c r="E5" s="55"/>
       <c r="F5" s="132"/>
@@ -6689,7 +6689,7 @@
     <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="55"/>
       <c r="B6" s="135"/>
-      <c r="C6" s="55"/>
+      <c r="C6" s="147"/>
       <c r="D6" s="55"/>
       <c r="E6" s="55"/>
       <c r="F6" s="155"/>
@@ -6780,7 +6780,7 @@
     <row r="7" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="55"/>
       <c r="B7" s="135"/>
-      <c r="C7" s="55"/>
+      <c r="C7" s="147"/>
       <c r="D7" s="55"/>
       <c r="E7" s="55"/>
       <c r="F7" s="132"/>
@@ -6824,7 +6824,7 @@
         <v>92</v>
       </c>
       <c r="T7" s="153"/>
-      <c r="U7" s="147"/>
+      <c r="U7" s="154"/>
       <c r="V7" s="147"/>
       <c r="W7" s="147"/>
       <c r="X7" s="55"/>
@@ -6871,7 +6871,7 @@
     <row r="8" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="55"/>
       <c r="B8" s="135"/>
-      <c r="C8" s="55"/>
+      <c r="C8" s="147"/>
       <c r="D8" s="55"/>
       <c r="E8" s="55"/>
       <c r="F8" s="132"/>
@@ -6915,7 +6915,7 @@
         <v>92</v>
       </c>
       <c r="T8" s="153"/>
-      <c r="U8" s="147"/>
+      <c r="U8" s="154"/>
       <c r="V8" s="147"/>
       <c r="W8" s="55"/>
       <c r="X8" s="55"/>
@@ -6962,7 +6962,7 @@
     <row r="9" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="55"/>
       <c r="B9" s="135"/>
-      <c r="C9" s="55"/>
+      <c r="C9" s="147"/>
       <c r="D9" s="55"/>
       <c r="E9" s="55"/>
       <c r="F9" s="132"/>
@@ -7053,7 +7053,7 @@
     <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="134"/>
       <c r="B10" s="135"/>
-      <c r="C10" s="55"/>
+      <c r="C10" s="147"/>
       <c r="D10" s="55"/>
       <c r="E10" s="55"/>
       <c r="F10" s="132"/>
@@ -7144,7 +7144,7 @@
     <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="134"/>
       <c r="B11" s="135"/>
-      <c r="C11" s="55"/>
+      <c r="C11" s="147"/>
       <c r="D11" s="55"/>
       <c r="E11" s="55"/>
       <c r="F11" s="132"/>
@@ -7188,7 +7188,7 @@
         <v>92</v>
       </c>
       <c r="T11" s="61"/>
-      <c r="U11" s="55"/>
+      <c r="U11" s="154"/>
       <c r="V11" s="154"/>
       <c r="W11" s="55"/>
       <c r="X11" s="55"/>
@@ -7235,7 +7235,7 @@
     <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="134"/>
       <c r="B12" s="135"/>
-      <c r="C12" s="55"/>
+      <c r="C12" s="147"/>
       <c r="D12" s="55"/>
       <c r="E12" s="55"/>
       <c r="F12" s="132"/>
@@ -7326,7 +7326,7 @@
     <row r="13" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="134"/>
       <c r="B13" s="135"/>
-      <c r="C13" s="55"/>
+      <c r="C13" s="147"/>
       <c r="D13" s="55"/>
       <c r="E13" s="143"/>
       <c r="F13" s="155"/>
@@ -7417,7 +7417,7 @@
     <row r="14" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="134"/>
       <c r="B14" s="135"/>
-      <c r="C14" s="55"/>
+      <c r="C14" s="147"/>
       <c r="D14" s="55"/>
       <c r="E14" s="55"/>
       <c r="F14" s="132"/>
@@ -7508,7 +7508,7 @@
     <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="134"/>
       <c r="B15" s="135"/>
-      <c r="C15" s="55"/>
+      <c r="C15" s="147"/>
       <c r="D15" s="55"/>
       <c r="E15" s="142"/>
       <c r="F15" s="141"/>
@@ -7599,7 +7599,7 @@
     <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="134"/>
       <c r="B16" s="135"/>
-      <c r="C16" s="55"/>
+      <c r="C16" s="147"/>
       <c r="D16" s="55"/>
       <c r="E16" s="55"/>
       <c r="F16" s="132"/>
@@ -7690,7 +7690,7 @@
     <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="134"/>
       <c r="B17" s="135"/>
-      <c r="C17" s="55"/>
+      <c r="C17" s="147"/>
       <c r="D17" s="55"/>
       <c r="E17" s="55"/>
       <c r="F17" s="132"/>
@@ -7734,7 +7734,7 @@
         <v>92</v>
       </c>
       <c r="T17" s="153"/>
-      <c r="U17" s="147"/>
+      <c r="U17" s="154"/>
       <c r="V17" s="147"/>
       <c r="W17" s="147"/>
       <c r="X17" s="55"/>
@@ -7781,7 +7781,7 @@
     <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="134"/>
       <c r="B18" s="135"/>
-      <c r="C18" s="55"/>
+      <c r="C18" s="147"/>
       <c r="D18" s="55"/>
       <c r="E18" s="146"/>
       <c r="F18" s="145"/>
@@ -7872,7 +7872,7 @@
     <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="134"/>
       <c r="B19" s="135"/>
-      <c r="C19" s="55"/>
+      <c r="C19" s="147"/>
       <c r="D19" s="55"/>
       <c r="E19" s="55"/>
       <c r="F19" s="132"/>
@@ -7963,7 +7963,7 @@
     <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="134"/>
       <c r="B20" s="135"/>
-      <c r="C20" s="55"/>
+      <c r="C20" s="147"/>
       <c r="D20" s="55"/>
       <c r="E20" s="55"/>
       <c r="F20" s="132"/>
@@ -8007,7 +8007,7 @@
         <v>92</v>
       </c>
       <c r="T20" s="153"/>
-      <c r="U20" s="55"/>
+      <c r="U20" s="154"/>
       <c r="V20" s="154"/>
       <c r="W20" s="55"/>
       <c r="X20" s="55"/>
@@ -8054,7 +8054,7 @@
     <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="134"/>
       <c r="B21" s="135"/>
-      <c r="C21" s="55"/>
+      <c r="C21" s="147"/>
       <c r="D21" s="55"/>
       <c r="E21" s="55"/>
       <c r="F21" s="132"/>
@@ -8098,7 +8098,7 @@
         <v>92</v>
       </c>
       <c r="T21" s="153"/>
-      <c r="U21" s="147"/>
+      <c r="U21" s="154"/>
       <c r="V21" s="147"/>
       <c r="W21" s="147"/>
       <c r="X21" s="55"/>
@@ -8145,7 +8145,7 @@
     <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="134"/>
       <c r="B22" s="135"/>
-      <c r="C22" s="55"/>
+      <c r="C22" s="147"/>
       <c r="D22" s="55"/>
       <c r="E22" s="55"/>
       <c r="F22" s="132"/>
@@ -8189,7 +8189,7 @@
         <v>92</v>
       </c>
       <c r="T22" s="153"/>
-      <c r="U22" s="147"/>
+      <c r="U22" s="154"/>
       <c r="V22" s="147"/>
       <c r="W22" s="147"/>
       <c r="X22" s="55"/>
@@ -8236,7 +8236,7 @@
     <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="134"/>
       <c r="B23" s="135"/>
-      <c r="C23" s="55"/>
+      <c r="C23" s="147"/>
       <c r="D23" s="55"/>
       <c r="E23" s="55"/>
       <c r="F23" s="132"/>
@@ -8327,7 +8327,7 @@
     <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="134"/>
       <c r="B24" s="135"/>
-      <c r="C24" s="55"/>
+      <c r="C24" s="147"/>
       <c r="D24" s="55"/>
       <c r="E24" s="146"/>
       <c r="F24" s="145"/>
@@ -8371,7 +8371,7 @@
         <v>92</v>
       </c>
       <c r="T24" s="153"/>
-      <c r="U24" s="147"/>
+      <c r="U24" s="154"/>
       <c r="V24" s="147"/>
       <c r="W24" s="150"/>
       <c r="X24" s="55"/>
@@ -8418,7 +8418,7 @@
     <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="134"/>
       <c r="B25" s="135"/>
-      <c r="C25" s="55"/>
+      <c r="C25" s="147"/>
       <c r="D25" s="55"/>
       <c r="E25" s="55"/>
       <c r="F25" s="132"/>
@@ -8462,7 +8462,7 @@
         <v>92</v>
       </c>
       <c r="T25" s="153"/>
-      <c r="U25" s="55"/>
+      <c r="U25" s="154"/>
       <c r="V25" s="154"/>
       <c r="W25" s="55"/>
       <c r="X25" s="55"/>
@@ -8509,7 +8509,7 @@
     <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="134"/>
       <c r="B26" s="156"/>
-      <c r="C26" s="55"/>
+      <c r="C26" s="147"/>
       <c r="D26" s="55"/>
       <c r="E26" s="55"/>
       <c r="F26" s="132"/>
@@ -8553,7 +8553,7 @@
         <v>92</v>
       </c>
       <c r="T26" s="153"/>
-      <c r="U26" s="147"/>
+      <c r="U26" s="154"/>
       <c r="V26" s="147"/>
       <c r="W26" s="147"/>
       <c r="X26" s="55"/>
@@ -8600,7 +8600,7 @@
     <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="134"/>
       <c r="B27" s="135"/>
-      <c r="C27" s="55"/>
+      <c r="C27" s="147"/>
       <c r="D27" s="55"/>
       <c r="E27" s="55"/>
       <c r="F27" s="132"/>
@@ -8644,7 +8644,7 @@
         <v>92</v>
       </c>
       <c r="T27" s="153"/>
-      <c r="U27" s="147"/>
+      <c r="U27" s="154"/>
       <c r="V27" s="147"/>
       <c r="W27" s="147"/>
       <c r="X27" s="55"/>
@@ -8691,7 +8691,7 @@
     <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="134"/>
       <c r="B28" s="135"/>
-      <c r="C28" s="55"/>
+      <c r="C28" s="147"/>
       <c r="D28" s="55"/>
       <c r="E28" s="55"/>
       <c r="F28" s="132"/>
@@ -8735,7 +8735,7 @@
         <v>92</v>
       </c>
       <c r="T28" s="153"/>
-      <c r="U28" s="55"/>
+      <c r="U28" s="154"/>
       <c r="V28" s="154"/>
       <c r="W28" s="55"/>
       <c r="X28" s="55"/>
@@ -8782,7 +8782,7 @@
     <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="134"/>
       <c r="B29" s="135"/>
-      <c r="C29" s="55"/>
+      <c r="C29" s="147"/>
       <c r="D29" s="55"/>
       <c r="E29" s="55"/>
       <c r="F29" s="132"/>
@@ -8826,7 +8826,7 @@
         <v>92</v>
       </c>
       <c r="T29" s="153"/>
-      <c r="U29" s="55"/>
+      <c r="U29" s="154"/>
       <c r="V29" s="154"/>
       <c r="W29" s="55"/>
       <c r="X29" s="55"/>
@@ -8873,7 +8873,7 @@
     <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="134"/>
       <c r="B30" s="135"/>
-      <c r="C30" s="55"/>
+      <c r="C30" s="147"/>
       <c r="D30" s="55"/>
       <c r="E30" s="55"/>
       <c r="F30" s="132"/>
@@ -8917,7 +8917,7 @@
         <v>92</v>
       </c>
       <c r="T30" s="153"/>
-      <c r="U30" s="147"/>
+      <c r="U30" s="154"/>
       <c r="V30" s="147"/>
       <c r="W30" s="147"/>
       <c r="X30" s="147"/>
@@ -8964,7 +8964,7 @@
     <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="134"/>
       <c r="B31" s="156"/>
-      <c r="C31" s="55"/>
+      <c r="C31" s="147"/>
       <c r="D31" s="55"/>
       <c r="E31" s="55"/>
       <c r="F31" s="132"/>
@@ -9008,7 +9008,7 @@
         <v>92</v>
       </c>
       <c r="T31" s="153"/>
-      <c r="U31" s="147"/>
+      <c r="U31" s="154"/>
       <c r="V31" s="147"/>
       <c r="W31" s="147"/>
       <c r="X31" s="147"/>
@@ -9055,7 +9055,7 @@
     <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="134"/>
       <c r="B32" s="135"/>
-      <c r="C32" s="55"/>
+      <c r="C32" s="147"/>
       <c r="D32" s="55"/>
       <c r="E32" s="55"/>
       <c r="F32" s="132"/>
@@ -9099,7 +9099,7 @@
         <v>92</v>
       </c>
       <c r="T32" s="153"/>
-      <c r="U32" s="147"/>
+      <c r="U32" s="154"/>
       <c r="V32" s="147"/>
       <c r="W32" s="147"/>
       <c r="X32" s="147"/>
@@ -9146,7 +9146,7 @@
     <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="134"/>
       <c r="B33" s="135"/>
-      <c r="C33" s="55"/>
+      <c r="C33" s="147"/>
       <c r="D33" s="55"/>
       <c r="E33" s="55"/>
       <c r="F33" s="132"/>
@@ -9190,7 +9190,7 @@
         <v>92</v>
       </c>
       <c r="T33" s="153"/>
-      <c r="U33" s="147"/>
+      <c r="U33" s="154"/>
       <c r="V33" s="147"/>
       <c r="W33" s="147"/>
       <c r="X33" s="147"/>
@@ -9237,7 +9237,7 @@
     <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="134"/>
       <c r="B34" s="135"/>
-      <c r="C34" s="55"/>
+      <c r="C34" s="147"/>
       <c r="D34" s="55"/>
       <c r="E34" s="55"/>
       <c r="F34" s="132"/>
@@ -9281,7 +9281,7 @@
         <v>92</v>
       </c>
       <c r="T34" s="153"/>
-      <c r="U34" s="147"/>
+      <c r="U34" s="154"/>
       <c r="V34" s="147"/>
       <c r="W34" s="147"/>
       <c r="X34" s="147"/>
@@ -9328,7 +9328,7 @@
     <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="134"/>
       <c r="B35" s="135"/>
-      <c r="C35" s="55"/>
+      <c r="C35" s="147"/>
       <c r="D35" s="55"/>
       <c r="E35" s="55"/>
       <c r="F35" s="132"/>
@@ -9372,7 +9372,7 @@
         <v>92</v>
       </c>
       <c r="T35" s="153"/>
-      <c r="U35" s="147"/>
+      <c r="U35" s="154"/>
       <c r="V35" s="147"/>
       <c r="W35" s="147"/>
       <c r="X35" s="147"/>
@@ -9419,7 +9419,7 @@
     <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="134"/>
       <c r="B36" s="135"/>
-      <c r="C36" s="55"/>
+      <c r="C36" s="147"/>
       <c r="D36" s="55"/>
       <c r="E36" s="55"/>
       <c r="F36" s="132"/>
@@ -9463,7 +9463,7 @@
         <v>92</v>
       </c>
       <c r="T36" s="153"/>
-      <c r="U36" s="147"/>
+      <c r="U36" s="154"/>
       <c r="V36" s="147"/>
       <c r="W36" s="147"/>
       <c r="X36" s="147"/>
@@ -9510,7 +9510,7 @@
     <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="134"/>
       <c r="B37" s="135"/>
-      <c r="C37" s="55"/>
+      <c r="C37" s="147"/>
       <c r="D37" s="55"/>
       <c r="E37" s="55"/>
       <c r="F37" s="132"/>
@@ -9554,7 +9554,7 @@
         <v>92</v>
       </c>
       <c r="T37" s="153"/>
-      <c r="U37" s="147"/>
+      <c r="U37" s="154"/>
       <c r="V37" s="147"/>
       <c r="W37" s="147"/>
       <c r="X37" s="147"/>
@@ -9601,7 +9601,7 @@
     <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="134"/>
       <c r="B38" s="135"/>
-      <c r="C38" s="55"/>
+      <c r="C38" s="147"/>
       <c r="D38" s="55"/>
       <c r="E38" s="55"/>
       <c r="F38" s="132"/>
@@ -9645,7 +9645,7 @@
         <v>92</v>
       </c>
       <c r="T38" s="153"/>
-      <c r="U38" s="147"/>
+      <c r="U38" s="154"/>
       <c r="V38" s="147"/>
       <c r="W38" s="147"/>
       <c r="X38" s="147"/>
@@ -9692,7 +9692,7 @@
     <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="134"/>
       <c r="B39" s="135"/>
-      <c r="C39" s="55"/>
+      <c r="C39" s="147"/>
       <c r="D39" s="55"/>
       <c r="E39" s="55"/>
       <c r="F39" s="132"/>
@@ -9736,7 +9736,7 @@
         <v>92</v>
       </c>
       <c r="T39" s="153"/>
-      <c r="U39" s="147"/>
+      <c r="U39" s="154"/>
       <c r="V39" s="147"/>
       <c r="W39" s="147"/>
       <c r="X39" s="147"/>
@@ -9783,7 +9783,7 @@
     <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="134"/>
       <c r="B40" s="135"/>
-      <c r="C40" s="55"/>
+      <c r="C40" s="147"/>
       <c r="D40" s="55"/>
       <c r="E40" s="55"/>
       <c r="F40" s="132"/>
@@ -9827,7 +9827,7 @@
         <v>92</v>
       </c>
       <c r="T40" s="153"/>
-      <c r="U40" s="147"/>
+      <c r="U40" s="154"/>
       <c r="V40" s="147"/>
       <c r="W40" s="147"/>
       <c r="X40" s="147"/>
@@ -9874,7 +9874,7 @@
     <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="134"/>
       <c r="B41" s="135"/>
-      <c r="C41" s="55"/>
+      <c r="C41" s="147"/>
       <c r="D41" s="55"/>
       <c r="E41" s="55"/>
       <c r="F41" s="132"/>
@@ -9918,7 +9918,7 @@
         <v>92</v>
       </c>
       <c r="T41" s="153"/>
-      <c r="U41" s="147"/>
+      <c r="U41" s="154"/>
       <c r="V41" s="147"/>
       <c r="W41" s="147"/>
       <c r="X41" s="147"/>
@@ -9965,7 +9965,7 @@
     <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="134"/>
       <c r="B42" s="135"/>
-      <c r="C42" s="55"/>
+      <c r="C42" s="147"/>
       <c r="D42" s="55"/>
       <c r="E42" s="55"/>
       <c r="F42" s="132"/>
@@ -10009,7 +10009,7 @@
         <v>92</v>
       </c>
       <c r="T42" s="153"/>
-      <c r="U42" s="147"/>
+      <c r="U42" s="154"/>
       <c r="V42" s="147"/>
       <c r="W42" s="147"/>
       <c r="X42" s="147"/>
@@ -10056,7 +10056,7 @@
     <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="134"/>
       <c r="B43" s="135"/>
-      <c r="C43" s="55"/>
+      <c r="C43" s="147"/>
       <c r="D43" s="55"/>
       <c r="E43" s="55"/>
       <c r="F43" s="132"/>
@@ -10100,7 +10100,7 @@
         <v>92</v>
       </c>
       <c r="T43" s="153"/>
-      <c r="U43" s="147"/>
+      <c r="U43" s="154"/>
       <c r="V43" s="147"/>
       <c r="W43" s="147"/>
       <c r="X43" s="147"/>
@@ -10147,7 +10147,7 @@
     <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="134"/>
       <c r="B44" s="135"/>
-      <c r="C44" s="55"/>
+      <c r="C44" s="147"/>
       <c r="D44" s="55"/>
       <c r="E44" s="55"/>
       <c r="F44" s="132"/>
@@ -10191,7 +10191,7 @@
         <v>92</v>
       </c>
       <c r="T44" s="153"/>
-      <c r="U44" s="147"/>
+      <c r="U44" s="154"/>
       <c r="V44" s="147"/>
       <c r="W44" s="147"/>
       <c r="X44" s="147"/>
@@ -10238,7 +10238,7 @@
     <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="134"/>
       <c r="B45" s="135"/>
-      <c r="C45" s="55"/>
+      <c r="C45" s="147"/>
       <c r="D45" s="55"/>
       <c r="E45" s="55"/>
       <c r="F45" s="132"/>
@@ -10282,7 +10282,7 @@
         <v>92</v>
       </c>
       <c r="T45" s="153"/>
-      <c r="U45" s="147"/>
+      <c r="U45" s="154"/>
       <c r="V45" s="147"/>
       <c r="W45" s="147"/>
       <c r="X45" s="147"/>
@@ -10329,7 +10329,7 @@
     <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="134"/>
       <c r="B46" s="135"/>
-      <c r="C46" s="55"/>
+      <c r="C46" s="147"/>
       <c r="D46" s="55"/>
       <c r="E46" s="55"/>
       <c r="F46" s="132"/>
@@ -10373,7 +10373,7 @@
         <v>92</v>
       </c>
       <c r="T46" s="153"/>
-      <c r="U46" s="147"/>
+      <c r="U46" s="154"/>
       <c r="V46" s="147"/>
       <c r="W46" s="147"/>
       <c r="X46" s="147"/>
@@ -10420,7 +10420,7 @@
     <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="134"/>
       <c r="B47" s="135"/>
-      <c r="C47" s="55"/>
+      <c r="C47" s="147"/>
       <c r="D47" s="55"/>
       <c r="E47" s="55"/>
       <c r="F47" s="132"/>
@@ -10464,7 +10464,7 @@
         <v>92</v>
       </c>
       <c r="T47" s="153"/>
-      <c r="U47" s="147"/>
+      <c r="U47" s="154"/>
       <c r="V47" s="147"/>
       <c r="W47" s="147"/>
       <c r="X47" s="147"/>
@@ -10511,7 +10511,7 @@
     <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="134"/>
       <c r="B48" s="135"/>
-      <c r="C48" s="55"/>
+      <c r="C48" s="147"/>
       <c r="D48" s="55"/>
       <c r="E48" s="55"/>
       <c r="F48" s="132"/>
@@ -10555,7 +10555,7 @@
         <v>92</v>
       </c>
       <c r="T48" s="153"/>
-      <c r="U48" s="147"/>
+      <c r="U48" s="154"/>
       <c r="V48" s="147"/>
       <c r="W48" s="147"/>
       <c r="X48" s="147"/>
@@ -10602,7 +10602,7 @@
     <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="134"/>
       <c r="B49" s="135"/>
-      <c r="C49" s="55"/>
+      <c r="C49" s="147"/>
       <c r="D49" s="55"/>
       <c r="E49" s="55"/>
       <c r="F49" s="132"/>
@@ -10646,7 +10646,7 @@
         <v>92</v>
       </c>
       <c r="T49" s="153"/>
-      <c r="U49" s="147"/>
+      <c r="U49" s="154"/>
       <c r="V49" s="147"/>
       <c r="W49" s="147"/>
       <c r="X49" s="147"/>
@@ -10693,7 +10693,7 @@
     <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="134"/>
       <c r="B50" s="135"/>
-      <c r="C50" s="55"/>
+      <c r="C50" s="147"/>
       <c r="D50" s="55"/>
       <c r="E50" s="55"/>
       <c r="F50" s="132"/>
@@ -10737,7 +10737,7 @@
         <v>92</v>
       </c>
       <c r="T50" s="153"/>
-      <c r="U50" s="147"/>
+      <c r="U50" s="154"/>
       <c r="V50" s="147"/>
       <c r="W50" s="147"/>
       <c r="X50" s="147"/>
@@ -10784,7 +10784,7 @@
     <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="134"/>
       <c r="B51" s="135"/>
-      <c r="C51" s="55"/>
+      <c r="C51" s="147"/>
       <c r="D51" s="55"/>
       <c r="E51" s="55"/>
       <c r="F51" s="132"/>
@@ -10828,7 +10828,7 @@
         <v>92</v>
       </c>
       <c r="T51" s="153"/>
-      <c r="U51" s="147"/>
+      <c r="U51" s="154"/>
       <c r="V51" s="147"/>
       <c r="W51" s="147"/>
       <c r="X51" s="147"/>
@@ -10875,7 +10875,7 @@
     <row r="52" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="134"/>
       <c r="B52" s="135"/>
-      <c r="C52" s="55"/>
+      <c r="C52" s="147"/>
       <c r="D52" s="55"/>
       <c r="E52" s="55"/>
       <c r="F52" s="132"/>
@@ -10919,7 +10919,7 @@
         <v>92</v>
       </c>
       <c r="T52" s="153"/>
-      <c r="U52" s="147"/>
+      <c r="U52" s="154"/>
       <c r="V52" s="147"/>
       <c r="W52" s="147"/>
       <c r="X52" s="147"/>
@@ -10966,7 +10966,7 @@
     <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="134"/>
       <c r="B53" s="135"/>
-      <c r="C53" s="55"/>
+      <c r="C53" s="147"/>
       <c r="D53" s="55"/>
       <c r="E53" s="55"/>
       <c r="F53" s="132"/>
@@ -11010,7 +11010,7 @@
         <v>92</v>
       </c>
       <c r="T53" s="153"/>
-      <c r="U53" s="147"/>
+      <c r="U53" s="154"/>
       <c r="V53" s="147"/>
       <c r="W53" s="147"/>
       <c r="X53" s="147"/>
@@ -11057,7 +11057,7 @@
     <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="134"/>
       <c r="B54" s="135"/>
-      <c r="C54" s="55"/>
+      <c r="C54" s="147"/>
       <c r="D54" s="55"/>
       <c r="E54" s="55"/>
       <c r="F54" s="132"/>
@@ -11101,7 +11101,7 @@
         <v>92</v>
       </c>
       <c r="T54" s="153"/>
-      <c r="U54" s="147"/>
+      <c r="U54" s="154"/>
       <c r="V54" s="147"/>
       <c r="W54" s="147"/>
       <c r="X54" s="147"/>
@@ -11148,7 +11148,7 @@
     <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="134"/>
       <c r="B55" s="135"/>
-      <c r="C55" s="55"/>
+      <c r="C55" s="147"/>
       <c r="D55" s="55"/>
       <c r="E55" s="55"/>
       <c r="F55" s="132"/>
@@ -11192,7 +11192,7 @@
         <v>92</v>
       </c>
       <c r="T55" s="153"/>
-      <c r="U55" s="147"/>
+      <c r="U55" s="154"/>
       <c r="V55" s="147"/>
       <c r="W55" s="147"/>
       <c r="X55" s="147"/>
@@ -11239,7 +11239,7 @@
     <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="134"/>
       <c r="B56" s="135"/>
-      <c r="C56" s="55"/>
+      <c r="C56" s="147"/>
       <c r="D56" s="55"/>
       <c r="E56" s="55"/>
       <c r="F56" s="132"/>
@@ -11283,7 +11283,7 @@
         <v>92</v>
       </c>
       <c r="T56" s="153"/>
-      <c r="U56" s="147"/>
+      <c r="U56" s="154"/>
       <c r="V56" s="147"/>
       <c r="W56" s="147"/>
       <c r="X56" s="147"/>
@@ -11330,7 +11330,7 @@
     <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="134"/>
       <c r="B57" s="135"/>
-      <c r="C57" s="55"/>
+      <c r="C57" s="147"/>
       <c r="D57" s="55"/>
       <c r="E57" s="55"/>
       <c r="F57" s="132"/>
@@ -11374,7 +11374,7 @@
         <v>92</v>
       </c>
       <c r="T57" s="153"/>
-      <c r="U57" s="147"/>
+      <c r="U57" s="154"/>
       <c r="V57" s="147"/>
       <c r="W57" s="147"/>
       <c r="X57" s="147"/>
@@ -11421,7 +11421,7 @@
     <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="134"/>
       <c r="B58" s="135"/>
-      <c r="C58" s="55"/>
+      <c r="C58" s="147"/>
       <c r="D58" s="55"/>
       <c r="E58" s="55"/>
       <c r="F58" s="132"/>
@@ -11465,7 +11465,7 @@
         <v>92</v>
       </c>
       <c r="T58" s="153"/>
-      <c r="U58" s="147"/>
+      <c r="U58" s="154"/>
       <c r="V58" s="147"/>
       <c r="W58" s="147"/>
       <c r="X58" s="147"/>
@@ -11512,7 +11512,7 @@
     <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="134"/>
       <c r="B59" s="135"/>
-      <c r="C59" s="55"/>
+      <c r="C59" s="147"/>
       <c r="D59" s="55"/>
       <c r="E59" s="55"/>
       <c r="F59" s="132"/>
@@ -11556,7 +11556,7 @@
         <v>92</v>
       </c>
       <c r="T59" s="153"/>
-      <c r="U59" s="147"/>
+      <c r="U59" s="154"/>
       <c r="V59" s="147"/>
       <c r="W59" s="147"/>
       <c r="X59" s="147"/>
@@ -11603,7 +11603,7 @@
     <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="134"/>
       <c r="B60" s="135"/>
-      <c r="C60" s="55"/>
+      <c r="C60" s="147"/>
       <c r="D60" s="55"/>
       <c r="E60" s="55"/>
       <c r="F60" s="132"/>
@@ -11647,7 +11647,7 @@
         <v>92</v>
       </c>
       <c r="T60" s="153"/>
-      <c r="U60" s="147"/>
+      <c r="U60" s="154"/>
       <c r="V60" s="147"/>
       <c r="W60" s="147"/>
       <c r="X60" s="147"/>
@@ -11694,7 +11694,7 @@
     <row r="61" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="134"/>
       <c r="B61" s="135"/>
-      <c r="C61" s="55"/>
+      <c r="C61" s="147"/>
       <c r="D61" s="55"/>
       <c r="E61" s="55"/>
       <c r="F61" s="132"/>
@@ -11738,7 +11738,7 @@
         <v>92</v>
       </c>
       <c r="T61" s="153"/>
-      <c r="U61" s="147"/>
+      <c r="U61" s="154"/>
       <c r="V61" s="147"/>
       <c r="W61" s="147"/>
       <c r="X61" s="147"/>
@@ -11785,7 +11785,7 @@
     <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="134"/>
       <c r="B62" s="135"/>
-      <c r="C62" s="55"/>
+      <c r="C62" s="147"/>
       <c r="D62" s="55"/>
       <c r="E62" s="55"/>
       <c r="F62" s="132"/>
@@ -11829,7 +11829,7 @@
         <v>92</v>
       </c>
       <c r="T62" s="153"/>
-      <c r="U62" s="147"/>
+      <c r="U62" s="154"/>
       <c r="V62" s="147"/>
       <c r="W62" s="147"/>
       <c r="X62" s="147"/>
@@ -11876,7 +11876,7 @@
     <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="134"/>
       <c r="B63" s="135"/>
-      <c r="C63" s="55"/>
+      <c r="C63" s="147"/>
       <c r="D63" s="55"/>
       <c r="E63" s="55"/>
       <c r="F63" s="132"/>
@@ -11920,7 +11920,7 @@
         <v>92</v>
       </c>
       <c r="T63" s="153"/>
-      <c r="U63" s="147"/>
+      <c r="U63" s="154"/>
       <c r="V63" s="147"/>
       <c r="W63" s="147"/>
       <c r="X63" s="147"/>
@@ -11967,7 +11967,7 @@
     <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="134"/>
       <c r="B64" s="135"/>
-      <c r="C64" s="55"/>
+      <c r="C64" s="147"/>
       <c r="D64" s="55"/>
       <c r="E64" s="55"/>
       <c r="F64" s="132"/>
@@ -12011,7 +12011,7 @@
         <v>92</v>
       </c>
       <c r="T64" s="153"/>
-      <c r="U64" s="147"/>
+      <c r="U64" s="154"/>
       <c r="V64" s="147"/>
       <c r="W64" s="147"/>
       <c r="X64" s="147"/>
@@ -12058,7 +12058,7 @@
     <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="134"/>
       <c r="B65" s="135"/>
-      <c r="C65" s="55"/>
+      <c r="C65" s="147"/>
       <c r="D65" s="55"/>
       <c r="E65" s="55"/>
       <c r="F65" s="132"/>
@@ -12102,7 +12102,7 @@
         <v>92</v>
       </c>
       <c r="T65" s="153"/>
-      <c r="U65" s="147"/>
+      <c r="U65" s="154"/>
       <c r="V65" s="147"/>
       <c r="W65" s="147"/>
       <c r="X65" s="147"/>
@@ -12149,7 +12149,7 @@
     <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="134"/>
       <c r="B66" s="135"/>
-      <c r="C66" s="55"/>
+      <c r="C66" s="147"/>
       <c r="D66" s="55"/>
       <c r="E66" s="55"/>
       <c r="F66" s="132"/>
@@ -12193,7 +12193,7 @@
         <v>92</v>
       </c>
       <c r="T66" s="153"/>
-      <c r="U66" s="147"/>
+      <c r="U66" s="154"/>
       <c r="V66" s="147"/>
       <c r="W66" s="147"/>
       <c r="X66" s="147"/>
@@ -12240,7 +12240,7 @@
     <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="134"/>
       <c r="B67" s="135"/>
-      <c r="C67" s="55"/>
+      <c r="C67" s="147"/>
       <c r="D67" s="55"/>
       <c r="E67" s="55"/>
       <c r="F67" s="132"/>
@@ -12284,7 +12284,7 @@
         <v>92</v>
       </c>
       <c r="T67" s="153"/>
-      <c r="U67" s="147"/>
+      <c r="U67" s="154"/>
       <c r="V67" s="147"/>
       <c r="W67" s="147"/>
       <c r="X67" s="147"/>
@@ -12331,7 +12331,7 @@
     <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="134"/>
       <c r="B68" s="135"/>
-      <c r="C68" s="55"/>
+      <c r="C68" s="147"/>
       <c r="D68" s="55"/>
       <c r="E68" s="55"/>
       <c r="F68" s="132"/>
@@ -12375,7 +12375,7 @@
         <v>92</v>
       </c>
       <c r="T68" s="153"/>
-      <c r="U68" s="147"/>
+      <c r="U68" s="154"/>
       <c r="V68" s="147"/>
       <c r="W68" s="147"/>
       <c r="X68" s="147"/>
@@ -12422,7 +12422,7 @@
     <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="134"/>
       <c r="B69" s="135"/>
-      <c r="C69" s="55"/>
+      <c r="C69" s="147"/>
       <c r="D69" s="55"/>
       <c r="E69" s="55"/>
       <c r="F69" s="132"/>
@@ -12466,7 +12466,7 @@
         <v>92</v>
       </c>
       <c r="T69" s="153"/>
-      <c r="U69" s="147"/>
+      <c r="U69" s="154"/>
       <c r="V69" s="147"/>
       <c r="W69" s="147"/>
       <c r="X69" s="147"/>
@@ -12513,7 +12513,7 @@
     <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="134"/>
       <c r="B70" s="135"/>
-      <c r="C70" s="55"/>
+      <c r="C70" s="147"/>
       <c r="D70" s="55"/>
       <c r="E70" s="55"/>
       <c r="F70" s="132"/>
@@ -12557,7 +12557,7 @@
         <v>92</v>
       </c>
       <c r="T70" s="153"/>
-      <c r="U70" s="147"/>
+      <c r="U70" s="154"/>
       <c r="V70" s="147"/>
       <c r="W70" s="147"/>
       <c r="X70" s="147"/>
@@ -12604,7 +12604,7 @@
     <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="134"/>
       <c r="B71" s="135"/>
-      <c r="C71" s="55"/>
+      <c r="C71" s="147"/>
       <c r="D71" s="55"/>
       <c r="E71" s="55"/>
       <c r="F71" s="132"/>
@@ -12648,7 +12648,7 @@
         <v>92</v>
       </c>
       <c r="T71" s="153"/>
-      <c r="U71" s="147"/>
+      <c r="U71" s="154"/>
       <c r="V71" s="147"/>
       <c r="W71" s="147"/>
       <c r="X71" s="147"/>
@@ -12695,7 +12695,7 @@
     <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="134"/>
       <c r="B72" s="135"/>
-      <c r="C72" s="55"/>
+      <c r="C72" s="147"/>
       <c r="D72" s="55"/>
       <c r="E72" s="55"/>
       <c r="F72" s="132"/>
@@ -12739,7 +12739,7 @@
         <v>92</v>
       </c>
       <c r="T72" s="153"/>
-      <c r="U72" s="147"/>
+      <c r="U72" s="154"/>
       <c r="V72" s="147"/>
       <c r="W72" s="147"/>
       <c r="X72" s="147"/>
@@ -12786,7 +12786,7 @@
     <row r="73" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="134"/>
       <c r="B73" s="135"/>
-      <c r="C73" s="55"/>
+      <c r="C73" s="147"/>
       <c r="D73" s="55"/>
       <c r="E73" s="55"/>
       <c r="F73" s="132"/>
@@ -12830,7 +12830,7 @@
         <v>92</v>
       </c>
       <c r="T73" s="153"/>
-      <c r="U73" s="147"/>
+      <c r="U73" s="154"/>
       <c r="V73" s="147"/>
       <c r="W73" s="147"/>
       <c r="X73" s="147"/>
@@ -12877,7 +12877,7 @@
     <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="134"/>
       <c r="B74" s="135"/>
-      <c r="C74" s="55"/>
+      <c r="C74" s="147"/>
       <c r="D74" s="55"/>
       <c r="E74" s="55"/>
       <c r="F74" s="132"/>
@@ -12921,7 +12921,7 @@
         <v>92</v>
       </c>
       <c r="T74" s="153"/>
-      <c r="U74" s="147"/>
+      <c r="U74" s="154"/>
       <c r="V74" s="147"/>
       <c r="W74" s="147"/>
       <c r="X74" s="147"/>
@@ -12968,7 +12968,7 @@
     <row r="75" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="134"/>
       <c r="B75" s="135"/>
-      <c r="C75" s="55"/>
+      <c r="C75" s="147"/>
       <c r="D75" s="55"/>
       <c r="E75" s="55"/>
       <c r="F75" s="132"/>
@@ -13012,7 +13012,7 @@
         <v>92</v>
       </c>
       <c r="T75" s="153"/>
-      <c r="U75" s="147"/>
+      <c r="U75" s="154"/>
       <c r="V75" s="147"/>
       <c r="W75" s="147"/>
       <c r="X75" s="147"/>
@@ -13059,7 +13059,7 @@
     <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="134"/>
       <c r="B76" s="135"/>
-      <c r="C76" s="55"/>
+      <c r="C76" s="147"/>
       <c r="D76" s="55"/>
       <c r="E76" s="55"/>
       <c r="F76" s="132"/>
@@ -13103,7 +13103,7 @@
         <v>92</v>
       </c>
       <c r="T76" s="153"/>
-      <c r="U76" s="147"/>
+      <c r="U76" s="154"/>
       <c r="V76" s="147"/>
       <c r="W76" s="147"/>
       <c r="X76" s="147"/>
@@ -13150,7 +13150,7 @@
     <row r="77" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="134"/>
       <c r="B77" s="135"/>
-      <c r="C77" s="55"/>
+      <c r="C77" s="147"/>
       <c r="D77" s="55"/>
       <c r="E77" s="55"/>
       <c r="F77" s="132"/>
@@ -13194,7 +13194,7 @@
         <v>92</v>
       </c>
       <c r="T77" s="153"/>
-      <c r="U77" s="147"/>
+      <c r="U77" s="154"/>
       <c r="V77" s="147"/>
       <c r="W77" s="147"/>
       <c r="X77" s="147"/>
@@ -13241,7 +13241,7 @@
     <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="134"/>
       <c r="B78" s="135"/>
-      <c r="C78" s="55"/>
+      <c r="C78" s="147"/>
       <c r="D78" s="55"/>
       <c r="E78" s="55"/>
       <c r="F78" s="132"/>
@@ -13285,7 +13285,7 @@
         <v>92</v>
       </c>
       <c r="T78" s="153"/>
-      <c r="U78" s="147"/>
+      <c r="U78" s="154"/>
       <c r="V78" s="147"/>
       <c r="W78" s="147"/>
       <c r="X78" s="147"/>
@@ -13332,7 +13332,7 @@
     <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="134"/>
       <c r="B79" s="135"/>
-      <c r="C79" s="55"/>
+      <c r="C79" s="147"/>
       <c r="D79" s="55"/>
       <c r="E79" s="55"/>
       <c r="F79" s="132"/>
@@ -13376,7 +13376,7 @@
         <v>92</v>
       </c>
       <c r="T79" s="153"/>
-      <c r="U79" s="147"/>
+      <c r="U79" s="154"/>
       <c r="V79" s="147"/>
       <c r="W79" s="147"/>
       <c r="X79" s="147"/>
@@ -13423,7 +13423,7 @@
     <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="134"/>
       <c r="B80" s="135"/>
-      <c r="C80" s="55"/>
+      <c r="C80" s="147"/>
       <c r="D80" s="55"/>
       <c r="E80" s="55"/>
       <c r="F80" s="132"/>
@@ -13467,7 +13467,7 @@
         <v>92</v>
       </c>
       <c r="T80" s="153"/>
-      <c r="U80" s="147"/>
+      <c r="U80" s="154"/>
       <c r="V80" s="147"/>
       <c r="W80" s="147"/>
       <c r="X80" s="147"/>
@@ -13514,7 +13514,7 @@
     <row r="81" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="134"/>
       <c r="B81" s="135"/>
-      <c r="C81" s="55"/>
+      <c r="C81" s="147"/>
       <c r="D81" s="55"/>
       <c r="E81" s="55"/>
       <c r="F81" s="132"/>
@@ -13558,7 +13558,7 @@
         <v>92</v>
       </c>
       <c r="T81" s="153"/>
-      <c r="U81" s="147"/>
+      <c r="U81" s="154"/>
       <c r="V81" s="147"/>
       <c r="W81" s="147"/>
       <c r="X81" s="147"/>
@@ -13605,7 +13605,7 @@
     <row r="82" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="134"/>
       <c r="B82" s="135"/>
-      <c r="C82" s="55"/>
+      <c r="C82" s="147"/>
       <c r="D82" s="55"/>
       <c r="E82" s="55"/>
       <c r="F82" s="132"/>
@@ -13649,7 +13649,7 @@
         <v>92</v>
       </c>
       <c r="T82" s="153"/>
-      <c r="U82" s="147"/>
+      <c r="U82" s="154"/>
       <c r="V82" s="147"/>
       <c r="W82" s="147"/>
       <c r="X82" s="147"/>
@@ -13696,7 +13696,7 @@
     <row r="83" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="134"/>
       <c r="B83" s="135"/>
-      <c r="C83" s="55"/>
+      <c r="C83" s="147"/>
       <c r="D83" s="55"/>
       <c r="E83" s="55"/>
       <c r="F83" s="132"/>
@@ -13740,7 +13740,7 @@
         <v>92</v>
       </c>
       <c r="T83" s="153"/>
-      <c r="U83" s="147"/>
+      <c r="U83" s="154"/>
       <c r="V83" s="147"/>
       <c r="W83" s="147"/>
       <c r="X83" s="147"/>
@@ -13787,7 +13787,7 @@
     <row r="84" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="134"/>
       <c r="B84" s="135"/>
-      <c r="C84" s="55"/>
+      <c r="C84" s="147"/>
       <c r="D84" s="55"/>
       <c r="E84" s="55"/>
       <c r="F84" s="132"/>
@@ -13831,7 +13831,7 @@
         <v>92</v>
       </c>
       <c r="T84" s="153"/>
-      <c r="U84" s="147"/>
+      <c r="U84" s="154"/>
       <c r="V84" s="147"/>
       <c r="W84" s="147"/>
       <c r="X84" s="147"/>
@@ -13878,7 +13878,7 @@
     <row r="85" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="134"/>
       <c r="B85" s="135"/>
-      <c r="C85" s="55"/>
+      <c r="C85" s="147"/>
       <c r="D85" s="55"/>
       <c r="E85" s="55"/>
       <c r="F85" s="132"/>
@@ -13922,7 +13922,7 @@
         <v>92</v>
       </c>
       <c r="T85" s="153"/>
-      <c r="U85" s="147"/>
+      <c r="U85" s="154"/>
       <c r="V85" s="147"/>
       <c r="W85" s="147"/>
       <c r="X85" s="147"/>
@@ -13969,7 +13969,7 @@
     <row r="86" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="134"/>
       <c r="B86" s="135"/>
-      <c r="C86" s="55"/>
+      <c r="C86" s="147"/>
       <c r="D86" s="55"/>
       <c r="E86" s="55"/>
       <c r="F86" s="132"/>
@@ -14013,7 +14013,7 @@
         <v>92</v>
       </c>
       <c r="T86" s="153"/>
-      <c r="U86" s="147"/>
+      <c r="U86" s="154"/>
       <c r="V86" s="147"/>
       <c r="W86" s="147"/>
       <c r="X86" s="147"/>
@@ -14060,7 +14060,7 @@
     <row r="87" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="134"/>
       <c r="B87" s="135"/>
-      <c r="C87" s="55"/>
+      <c r="C87" s="147"/>
       <c r="D87" s="55"/>
       <c r="E87" s="55"/>
       <c r="F87" s="132"/>
@@ -14104,7 +14104,7 @@
         <v>92</v>
       </c>
       <c r="T87" s="153"/>
-      <c r="U87" s="147"/>
+      <c r="U87" s="154"/>
       <c r="V87" s="147"/>
       <c r="W87" s="147"/>
       <c r="X87" s="147"/>
@@ -14151,7 +14151,7 @@
     <row r="88" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="134"/>
       <c r="B88" s="135"/>
-      <c r="C88" s="55"/>
+      <c r="C88" s="147"/>
       <c r="D88" s="55"/>
       <c r="E88" s="55"/>
       <c r="F88" s="132"/>
@@ -14195,7 +14195,7 @@
         <v>92</v>
       </c>
       <c r="T88" s="153"/>
-      <c r="U88" s="147"/>
+      <c r="U88" s="154"/>
       <c r="V88" s="147"/>
       <c r="W88" s="147"/>
       <c r="X88" s="147"/>
@@ -14286,7 +14286,7 @@
         <v>92</v>
       </c>
       <c r="T89" s="153"/>
-      <c r="U89" s="147"/>
+      <c r="U89" s="154"/>
       <c r="V89" s="147"/>
       <c r="W89" s="147"/>
       <c r="X89" s="147"/>
@@ -14377,7 +14377,7 @@
         <v>92</v>
       </c>
       <c r="T90" s="153"/>
-      <c r="U90" s="147"/>
+      <c r="U90" s="154"/>
       <c r="V90" s="147"/>
       <c r="W90" s="147"/>
       <c r="X90" s="147"/>
@@ -14468,7 +14468,7 @@
         <v>92</v>
       </c>
       <c r="T91" s="153"/>
-      <c r="U91" s="147"/>
+      <c r="U91" s="154"/>
       <c r="V91" s="147"/>
       <c r="W91" s="150"/>
       <c r="X91" s="147"/>
@@ -14515,7 +14515,7 @@
     <row r="92" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="134"/>
       <c r="B92" s="135"/>
-      <c r="C92" s="55"/>
+      <c r="C92" s="147"/>
       <c r="D92" s="55"/>
       <c r="E92" s="55"/>
       <c r="F92" s="132"/>
@@ -14559,7 +14559,7 @@
         <v>92</v>
       </c>
       <c r="T92" s="61"/>
-      <c r="U92" s="147"/>
+      <c r="U92" s="154"/>
       <c r="V92" s="147"/>
       <c r="W92" s="147"/>
       <c r="X92" s="147"/>
@@ -14650,7 +14650,7 @@
         <v>92</v>
       </c>
       <c r="T93" s="153"/>
-      <c r="U93" s="147"/>
+      <c r="U93" s="154"/>
       <c r="V93" s="147"/>
       <c r="W93" s="147"/>
       <c r="X93" s="147"/>
@@ -14741,7 +14741,7 @@
         <v>92</v>
       </c>
       <c r="T94" s="153"/>
-      <c r="U94" s="147"/>
+      <c r="U94" s="154"/>
       <c r="V94" s="147"/>
       <c r="W94" s="147"/>
       <c r="X94" s="147"/>
@@ -14832,7 +14832,7 @@
         <v>92</v>
       </c>
       <c r="T95" s="153"/>
-      <c r="U95" s="147"/>
+      <c r="U95" s="154"/>
       <c r="V95" s="147"/>
       <c r="W95" s="147"/>
       <c r="X95" s="147"/>
@@ -14923,7 +14923,7 @@
         <v>92</v>
       </c>
       <c r="T96" s="153"/>
-      <c r="U96" s="147"/>
+      <c r="U96" s="154"/>
       <c r="V96" s="147"/>
       <c r="W96" s="147"/>
       <c r="X96" s="147"/>
@@ -15014,7 +15014,7 @@
         <v>92</v>
       </c>
       <c r="T97" s="153"/>
-      <c r="U97" s="147"/>
+      <c r="U97" s="154"/>
       <c r="V97" s="147"/>
       <c r="W97" s="147"/>
       <c r="X97" s="147"/>
@@ -15105,7 +15105,7 @@
         <v>92</v>
       </c>
       <c r="T98" s="153"/>
-      <c r="U98" s="147"/>
+      <c r="U98" s="154"/>
       <c r="V98" s="147"/>
       <c r="W98" s="147"/>
       <c r="X98" s="147"/>
@@ -15196,7 +15196,7 @@
         <v>92</v>
       </c>
       <c r="T99" s="153"/>
-      <c r="U99" s="147"/>
+      <c r="U99" s="154"/>
       <c r="V99" s="147"/>
       <c r="W99" s="147"/>
       <c r="X99" s="147"/>
@@ -15287,7 +15287,7 @@
         <v>92</v>
       </c>
       <c r="T100" s="153"/>
-      <c r="U100" s="147"/>
+      <c r="U100" s="154"/>
       <c r="V100" s="147"/>
       <c r="W100" s="147"/>
       <c r="X100" s="147"/>
@@ -15378,7 +15378,7 @@
         <v>92</v>
       </c>
       <c r="T101" s="153"/>
-      <c r="U101" s="147"/>
+      <c r="U101" s="154"/>
       <c r="V101" s="147"/>
       <c r="W101" s="147"/>
       <c r="X101" s="147"/>
@@ -15425,7 +15425,7 @@
     <row r="102" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="134"/>
       <c r="B102" s="135"/>
-      <c r="C102" s="55"/>
+      <c r="C102" s="147"/>
       <c r="D102" s="55"/>
       <c r="E102" s="55"/>
       <c r="F102" s="132"/>
@@ -15469,7 +15469,7 @@
         <v>92</v>
       </c>
       <c r="T102" s="61"/>
-      <c r="U102" s="55"/>
+      <c r="U102" s="154"/>
       <c r="V102" s="55"/>
       <c r="W102" s="55"/>
       <c r="X102" s="55"/>
@@ -15560,7 +15560,7 @@
         <v>92</v>
       </c>
       <c r="T103" s="61"/>
-      <c r="U103" s="55"/>
+      <c r="U103" s="154"/>
       <c r="V103" s="154"/>
       <c r="W103" s="55"/>
       <c r="X103" s="55"/>
@@ -15651,7 +15651,7 @@
         <v>92</v>
       </c>
       <c r="T104" s="61"/>
-      <c r="U104" s="55"/>
+      <c r="U104" s="154"/>
       <c r="V104" s="154"/>
       <c r="W104" s="55"/>
       <c r="X104" s="55"/>
@@ -15742,7 +15742,7 @@
         <v>92</v>
       </c>
       <c r="T105" s="61"/>
-      <c r="U105" s="55"/>
+      <c r="U105" s="154"/>
       <c r="V105" s="55"/>
       <c r="W105" s="55"/>
       <c r="X105" s="55"/>
@@ -15789,7 +15789,7 @@
     <row r="106" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="134"/>
       <c r="B106" s="135"/>
-      <c r="C106" s="55"/>
+      <c r="C106" s="147"/>
       <c r="D106" s="55"/>
       <c r="E106" s="55"/>
       <c r="F106" s="132"/>
@@ -15833,7 +15833,7 @@
         <v>92</v>
       </c>
       <c r="T106" s="61"/>
-      <c r="U106" s="55"/>
+      <c r="U106" s="154"/>
       <c r="V106" s="55"/>
       <c r="W106" s="55"/>
       <c r="X106" s="55"/>
@@ -15880,7 +15880,7 @@
     <row r="107" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="134"/>
       <c r="B107" s="135"/>
-      <c r="C107" s="55"/>
+      <c r="C107" s="147"/>
       <c r="D107" s="55"/>
       <c r="E107" s="55"/>
       <c r="F107" s="132"/>
@@ -15924,7 +15924,7 @@
         <v>92</v>
       </c>
       <c r="T107" s="61"/>
-      <c r="U107" s="55"/>
+      <c r="U107" s="154"/>
       <c r="V107" s="55"/>
       <c r="W107" s="55"/>
       <c r="X107" s="55"/>
@@ -15971,7 +15971,7 @@
     <row r="108" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="134"/>
       <c r="B108" s="135"/>
-      <c r="C108" s="55"/>
+      <c r="C108" s="147"/>
       <c r="D108" s="55"/>
       <c r="E108" s="55"/>
       <c r="F108" s="132"/>
@@ -16015,7 +16015,7 @@
         <v>92</v>
       </c>
       <c r="T108" s="61"/>
-      <c r="U108" s="55"/>
+      <c r="U108" s="154"/>
       <c r="V108" s="55"/>
       <c r="W108" s="55"/>
       <c r="X108" s="55"/>
@@ -16062,7 +16062,7 @@
     <row r="109" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="134"/>
       <c r="B109" s="135"/>
-      <c r="C109" s="55"/>
+      <c r="C109" s="147"/>
       <c r="D109" s="55"/>
       <c r="E109" s="55"/>
       <c r="F109" s="132"/>
@@ -16106,7 +16106,7 @@
         <v>92</v>
       </c>
       <c r="T109" s="61"/>
-      <c r="U109" s="55"/>
+      <c r="U109" s="154"/>
       <c r="V109" s="55"/>
       <c r="W109" s="55"/>
       <c r="X109" s="55"/>
@@ -16153,7 +16153,7 @@
     <row r="110" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="134"/>
       <c r="B110" s="135"/>
-      <c r="C110" s="55"/>
+      <c r="C110" s="147"/>
       <c r="D110" s="55"/>
       <c r="E110" s="55"/>
       <c r="F110" s="132"/>
@@ -16197,7 +16197,7 @@
         <v>92</v>
       </c>
       <c r="T110" s="61"/>
-      <c r="U110" s="55"/>
+      <c r="U110" s="154"/>
       <c r="V110" s="55"/>
       <c r="W110" s="55"/>
       <c r="X110" s="55"/>
@@ -16244,7 +16244,7 @@
     <row r="111" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="134"/>
       <c r="B111" s="135"/>
-      <c r="C111" s="55"/>
+      <c r="C111" s="147"/>
       <c r="D111" s="55"/>
       <c r="E111" s="55"/>
       <c r="F111" s="132"/>
@@ -16288,7 +16288,7 @@
         <v>92</v>
       </c>
       <c r="T111" s="61"/>
-      <c r="U111" s="55"/>
+      <c r="U111" s="154"/>
       <c r="V111" s="55"/>
       <c r="W111" s="55"/>
       <c r="X111" s="55"/>
@@ -16335,7 +16335,7 @@
     <row r="112" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="134"/>
       <c r="B112" s="135"/>
-      <c r="C112" s="55"/>
+      <c r="C112" s="147"/>
       <c r="D112" s="55"/>
       <c r="E112" s="55"/>
       <c r="F112" s="132"/>
@@ -16379,7 +16379,7 @@
         <v>92</v>
       </c>
       <c r="T112" s="61"/>
-      <c r="U112" s="55"/>
+      <c r="U112" s="154"/>
       <c r="V112" s="55"/>
       <c r="W112" s="55"/>
       <c r="X112" s="55"/>
@@ -16426,7 +16426,7 @@
     <row r="113" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="134"/>
       <c r="B113" s="135"/>
-      <c r="C113" s="55"/>
+      <c r="C113" s="147"/>
       <c r="D113" s="55"/>
       <c r="E113" s="55"/>
       <c r="F113" s="132"/>
@@ -16470,7 +16470,7 @@
         <v>92</v>
       </c>
       <c r="T113" s="61"/>
-      <c r="U113" s="55"/>
+      <c r="U113" s="154"/>
       <c r="V113" s="55"/>
       <c r="W113" s="55"/>
       <c r="X113" s="55"/>
@@ -16517,7 +16517,7 @@
     <row r="114" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="134"/>
       <c r="B114" s="135"/>
-      <c r="C114" s="55"/>
+      <c r="C114" s="147"/>
       <c r="D114" s="55"/>
       <c r="E114" s="55"/>
       <c r="F114" s="132"/>
@@ -16561,7 +16561,7 @@
         <v>92</v>
       </c>
       <c r="T114" s="61"/>
-      <c r="U114" s="55"/>
+      <c r="U114" s="154"/>
       <c r="V114" s="55"/>
       <c r="W114" s="55"/>
       <c r="X114" s="55"/>
@@ -16608,7 +16608,7 @@
     <row r="115" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="134"/>
       <c r="B115" s="135"/>
-      <c r="C115" s="55"/>
+      <c r="C115" s="147"/>
       <c r="D115" s="55"/>
       <c r="E115" s="55"/>
       <c r="F115" s="132"/>
@@ -16652,7 +16652,7 @@
         <v>92</v>
       </c>
       <c r="T115" s="61"/>
-      <c r="U115" s="55"/>
+      <c r="U115" s="154"/>
       <c r="V115" s="55"/>
       <c r="W115" s="55"/>
       <c r="X115" s="55"/>
@@ -16699,7 +16699,7 @@
     <row r="116" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="134"/>
       <c r="B116" s="135"/>
-      <c r="C116" s="55"/>
+      <c r="C116" s="147"/>
       <c r="D116" s="55"/>
       <c r="E116" s="55"/>
       <c r="F116" s="132"/>
@@ -16743,7 +16743,7 @@
         <v>92</v>
       </c>
       <c r="T116" s="61"/>
-      <c r="U116" s="55"/>
+      <c r="U116" s="154"/>
       <c r="V116" s="55"/>
       <c r="W116" s="55"/>
       <c r="X116" s="55"/>
@@ -16790,7 +16790,7 @@
     <row r="117" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="134"/>
       <c r="B117" s="135"/>
-      <c r="C117" s="55"/>
+      <c r="C117" s="147"/>
       <c r="D117" s="55"/>
       <c r="E117" s="55"/>
       <c r="F117" s="132"/>
@@ -16834,7 +16834,7 @@
         <v>92</v>
       </c>
       <c r="T117" s="61"/>
-      <c r="U117" s="55"/>
+      <c r="U117" s="154"/>
       <c r="V117" s="55"/>
       <c r="W117" s="55"/>
       <c r="X117" s="55"/>
@@ -16881,7 +16881,7 @@
     <row r="118" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="134"/>
       <c r="B118" s="135"/>
-      <c r="C118" s="55"/>
+      <c r="C118" s="147"/>
       <c r="D118" s="55"/>
       <c r="E118" s="55"/>
       <c r="F118" s="132"/>
@@ -16925,7 +16925,7 @@
         <v>92</v>
       </c>
       <c r="T118" s="61"/>
-      <c r="U118" s="55"/>
+      <c r="U118" s="154"/>
       <c r="V118" s="55"/>
       <c r="W118" s="55"/>
       <c r="X118" s="55"/>
@@ -16972,7 +16972,7 @@
     <row r="119" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="134"/>
       <c r="B119" s="135"/>
-      <c r="C119" s="55"/>
+      <c r="C119" s="147"/>
       <c r="D119" s="55"/>
       <c r="E119" s="55"/>
       <c r="F119" s="132"/>
@@ -17016,7 +17016,7 @@
         <v>92</v>
       </c>
       <c r="T119" s="61"/>
-      <c r="U119" s="55"/>
+      <c r="U119" s="154"/>
       <c r="V119" s="55"/>
       <c r="W119" s="55"/>
       <c r="X119" s="55"/>
@@ -17063,7 +17063,7 @@
     <row r="120" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="134"/>
       <c r="B120" s="135"/>
-      <c r="C120" s="55"/>
+      <c r="C120" s="147"/>
       <c r="D120" s="55"/>
       <c r="E120" s="55"/>
       <c r="F120" s="132"/>
@@ -17107,7 +17107,7 @@
         <v>92</v>
       </c>
       <c r="T120" s="61"/>
-      <c r="U120" s="55"/>
+      <c r="U120" s="154"/>
       <c r="V120" s="55"/>
       <c r="W120" s="55"/>
       <c r="X120" s="55"/>
@@ -17154,7 +17154,7 @@
     <row r="121" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="134"/>
       <c r="B121" s="135"/>
-      <c r="C121" s="55"/>
+      <c r="C121" s="147"/>
       <c r="D121" s="55"/>
       <c r="E121" s="55"/>
       <c r="F121" s="132"/>
@@ -17198,7 +17198,7 @@
         <v>92</v>
       </c>
       <c r="T121" s="61"/>
-      <c r="U121" s="55"/>
+      <c r="U121" s="154"/>
       <c r="V121" s="55"/>
       <c r="W121" s="55"/>
       <c r="X121" s="55"/>
@@ -17245,7 +17245,7 @@
     <row r="122" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="134"/>
       <c r="B122" s="135"/>
-      <c r="C122" s="55"/>
+      <c r="C122" s="147"/>
       <c r="D122" s="55"/>
       <c r="E122" s="55"/>
       <c r="F122" s="132"/>
@@ -17289,7 +17289,7 @@
         <v>92</v>
       </c>
       <c r="T122" s="61"/>
-      <c r="U122" s="55"/>
+      <c r="U122" s="154"/>
       <c r="V122" s="55"/>
       <c r="W122" s="55"/>
       <c r="X122" s="55"/>
@@ -17336,7 +17336,7 @@
     <row r="123" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="134"/>
       <c r="B123" s="135"/>
-      <c r="C123" s="55"/>
+      <c r="C123" s="147"/>
       <c r="D123" s="55"/>
       <c r="E123" s="55"/>
       <c r="F123" s="132"/>
@@ -17380,7 +17380,7 @@
         <v>92</v>
       </c>
       <c r="T123" s="61"/>
-      <c r="U123" s="55"/>
+      <c r="U123" s="154"/>
       <c r="V123" s="55"/>
       <c r="W123" s="55"/>
       <c r="X123" s="55"/>
@@ -17427,7 +17427,7 @@
     <row r="124" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="134"/>
       <c r="B124" s="135"/>
-      <c r="C124" s="55"/>
+      <c r="C124" s="147"/>
       <c r="D124" s="55"/>
       <c r="E124" s="55"/>
       <c r="F124" s="132"/>
@@ -17471,7 +17471,7 @@
         <v>92</v>
       </c>
       <c r="T124" s="61"/>
-      <c r="U124" s="55"/>
+      <c r="U124" s="154"/>
       <c r="V124" s="55"/>
       <c r="W124" s="55"/>
       <c r="X124" s="55"/>
@@ -17518,7 +17518,7 @@
     <row r="125" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="134"/>
       <c r="B125" s="135"/>
-      <c r="C125" s="55"/>
+      <c r="C125" s="147"/>
       <c r="D125" s="55"/>
       <c r="E125" s="55"/>
       <c r="F125" s="132"/>
@@ -17562,7 +17562,7 @@
         <v>92</v>
       </c>
       <c r="T125" s="61"/>
-      <c r="U125" s="55"/>
+      <c r="U125" s="154"/>
       <c r="V125" s="55"/>
       <c r="W125" s="55"/>
       <c r="X125" s="55"/>
@@ -17609,7 +17609,7 @@
     <row r="126" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="134"/>
       <c r="B126" s="135"/>
-      <c r="C126" s="55"/>
+      <c r="C126" s="147"/>
       <c r="D126" s="55"/>
       <c r="E126" s="55"/>
       <c r="F126" s="132"/>
@@ -17653,7 +17653,7 @@
         <v>92</v>
       </c>
       <c r="T126" s="61"/>
-      <c r="U126" s="55"/>
+      <c r="U126" s="154"/>
       <c r="V126" s="55"/>
       <c r="W126" s="55"/>
       <c r="X126" s="55"/>
@@ -17700,7 +17700,7 @@
     <row r="127" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="134"/>
       <c r="B127" s="135"/>
-      <c r="C127" s="55"/>
+      <c r="C127" s="147"/>
       <c r="D127" s="55"/>
       <c r="E127" s="55"/>
       <c r="F127" s="132"/>
@@ -17744,7 +17744,7 @@
         <v>92</v>
       </c>
       <c r="T127" s="61"/>
-      <c r="U127" s="55"/>
+      <c r="U127" s="154"/>
       <c r="V127" s="55"/>
       <c r="W127" s="55"/>
       <c r="X127" s="55"/>
@@ -17791,7 +17791,7 @@
     <row r="128" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="134"/>
       <c r="B128" s="135"/>
-      <c r="C128" s="55"/>
+      <c r="C128" s="147"/>
       <c r="D128" s="55"/>
       <c r="E128" s="55"/>
       <c r="F128" s="132"/>
@@ -17835,7 +17835,7 @@
         <v>92</v>
       </c>
       <c r="T128" s="61"/>
-      <c r="U128" s="55"/>
+      <c r="U128" s="154"/>
       <c r="V128" s="55"/>
       <c r="W128" s="55"/>
       <c r="X128" s="55"/>
@@ -17882,7 +17882,7 @@
     <row r="129" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="134"/>
       <c r="B129" s="135"/>
-      <c r="C129" s="55"/>
+      <c r="C129" s="147"/>
       <c r="D129" s="55"/>
       <c r="E129" s="55"/>
       <c r="F129" s="132"/>
@@ -17926,7 +17926,7 @@
         <v>92</v>
       </c>
       <c r="T129" s="61"/>
-      <c r="U129" s="55"/>
+      <c r="U129" s="154"/>
       <c r="V129" s="55"/>
       <c r="W129" s="55"/>
       <c r="X129" s="55"/>
@@ -17973,7 +17973,7 @@
     <row r="130" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="134"/>
       <c r="B130" s="135"/>
-      <c r="C130" s="55"/>
+      <c r="C130" s="147"/>
       <c r="D130" s="55"/>
       <c r="E130" s="55"/>
       <c r="F130" s="132"/>
@@ -18017,7 +18017,7 @@
         <v>92</v>
       </c>
       <c r="T130" s="61"/>
-      <c r="U130" s="55"/>
+      <c r="U130" s="154"/>
       <c r="V130" s="55"/>
       <c r="W130" s="55"/>
       <c r="X130" s="55"/>
@@ -18064,7 +18064,7 @@
     <row r="131" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="134"/>
       <c r="B131" s="135"/>
-      <c r="C131" s="55"/>
+      <c r="C131" s="147"/>
       <c r="D131" s="55"/>
       <c r="E131" s="55"/>
       <c r="F131" s="132"/>
@@ -18108,7 +18108,7 @@
         <v>92</v>
       </c>
       <c r="T131" s="61"/>
-      <c r="U131" s="55"/>
+      <c r="U131" s="154"/>
       <c r="V131" s="55"/>
       <c r="W131" s="55"/>
       <c r="X131" s="55"/>
@@ -18155,7 +18155,7 @@
     <row r="132" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="134"/>
       <c r="B132" s="135"/>
-      <c r="C132" s="55"/>
+      <c r="C132" s="147"/>
       <c r="D132" s="55"/>
       <c r="E132" s="55"/>
       <c r="F132" s="132"/>
@@ -18199,7 +18199,7 @@
         <v>92</v>
       </c>
       <c r="T132" s="61"/>
-      <c r="U132" s="55"/>
+      <c r="U132" s="154"/>
       <c r="V132" s="55"/>
       <c r="W132" s="55"/>
       <c r="X132" s="55"/>
@@ -18246,7 +18246,7 @@
     <row r="133" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="134"/>
       <c r="B133" s="135"/>
-      <c r="C133" s="55"/>
+      <c r="C133" s="147"/>
       <c r="D133" s="55"/>
       <c r="E133" s="55"/>
       <c r="F133" s="132"/>
@@ -18290,7 +18290,7 @@
         <v>92</v>
       </c>
       <c r="T133" s="61"/>
-      <c r="U133" s="55"/>
+      <c r="U133" s="154"/>
       <c r="V133" s="55"/>
       <c r="W133" s="55"/>
       <c r="X133" s="55"/>
@@ -18337,7 +18337,7 @@
     <row r="134" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="134"/>
       <c r="B134" s="135"/>
-      <c r="C134" s="55"/>
+      <c r="C134" s="147"/>
       <c r="D134" s="55"/>
       <c r="E134" s="55"/>
       <c r="F134" s="132"/>
@@ -18381,7 +18381,7 @@
         <v>92</v>
       </c>
       <c r="T134" s="61"/>
-      <c r="U134" s="55"/>
+      <c r="U134" s="154"/>
       <c r="V134" s="55"/>
       <c r="W134" s="55"/>
       <c r="X134" s="55"/>
@@ -18428,7 +18428,7 @@
     <row r="135" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="134"/>
       <c r="B135" s="135"/>
-      <c r="C135" s="55"/>
+      <c r="C135" s="147"/>
       <c r="D135" s="55"/>
       <c r="E135" s="55"/>
       <c r="F135" s="132"/>
@@ -18472,7 +18472,7 @@
         <v>92</v>
       </c>
       <c r="T135" s="61"/>
-      <c r="U135" s="55"/>
+      <c r="U135" s="154"/>
       <c r="V135" s="55"/>
       <c r="W135" s="55"/>
       <c r="X135" s="55"/>
@@ -18519,7 +18519,7 @@
     <row r="136" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="134"/>
       <c r="B136" s="135"/>
-      <c r="C136" s="55"/>
+      <c r="C136" s="147"/>
       <c r="D136" s="55"/>
       <c r="E136" s="55"/>
       <c r="F136" s="132"/>
@@ -18563,7 +18563,7 @@
         <v>92</v>
       </c>
       <c r="T136" s="61"/>
-      <c r="U136" s="55"/>
+      <c r="U136" s="154"/>
       <c r="V136" s="55"/>
       <c r="W136" s="55"/>
       <c r="X136" s="55"/>
@@ -18610,7 +18610,7 @@
     <row r="137" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="134"/>
       <c r="B137" s="135"/>
-      <c r="C137" s="55"/>
+      <c r="C137" s="147"/>
       <c r="D137" s="55"/>
       <c r="E137" s="55"/>
       <c r="F137" s="132"/>
@@ -18654,7 +18654,7 @@
         <v>92</v>
       </c>
       <c r="T137" s="61"/>
-      <c r="U137" s="55"/>
+      <c r="U137" s="154"/>
       <c r="V137" s="55"/>
       <c r="W137" s="55"/>
       <c r="X137" s="55"/>
@@ -18701,7 +18701,7 @@
     <row r="138" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="134"/>
       <c r="B138" s="135"/>
-      <c r="C138" s="55"/>
+      <c r="C138" s="147"/>
       <c r="D138" s="55"/>
       <c r="E138" s="55"/>
       <c r="F138" s="132"/>
@@ -18745,7 +18745,7 @@
         <v>92</v>
       </c>
       <c r="T138" s="61"/>
-      <c r="U138" s="55"/>
+      <c r="U138" s="154"/>
       <c r="V138" s="55"/>
       <c r="W138" s="55"/>
       <c r="X138" s="55"/>
@@ -18792,7 +18792,7 @@
     <row r="139" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="134"/>
       <c r="B139" s="135"/>
-      <c r="C139" s="55"/>
+      <c r="C139" s="147"/>
       <c r="D139" s="55"/>
       <c r="E139" s="55"/>
       <c r="F139" s="132"/>
@@ -18836,7 +18836,7 @@
         <v>92</v>
       </c>
       <c r="T139" s="61"/>
-      <c r="U139" s="55"/>
+      <c r="U139" s="154"/>
       <c r="V139" s="55"/>
       <c r="W139" s="55"/>
       <c r="X139" s="55"/>
@@ -18883,7 +18883,7 @@
     <row r="140" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="134"/>
       <c r="B140" s="135"/>
-      <c r="C140" s="55"/>
+      <c r="C140" s="147"/>
       <c r="D140" s="55"/>
       <c r="E140" s="55"/>
       <c r="F140" s="132"/>
@@ -18927,7 +18927,7 @@
         <v>92</v>
       </c>
       <c r="T140" s="61"/>
-      <c r="U140" s="55"/>
+      <c r="U140" s="154"/>
       <c r="V140" s="55"/>
       <c r="W140" s="55"/>
       <c r="X140" s="55"/>
@@ -18974,7 +18974,7 @@
     <row r="141" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="134"/>
       <c r="B141" s="135"/>
-      <c r="C141" s="55"/>
+      <c r="C141" s="147"/>
       <c r="D141" s="55"/>
       <c r="E141" s="55"/>
       <c r="F141" s="132"/>
@@ -19018,7 +19018,7 @@
         <v>92</v>
       </c>
       <c r="T141" s="61"/>
-      <c r="U141" s="55"/>
+      <c r="U141" s="154"/>
       <c r="V141" s="55"/>
       <c r="W141" s="55"/>
       <c r="X141" s="55"/>
@@ -19065,7 +19065,7 @@
     <row r="142" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="134"/>
       <c r="B142" s="135"/>
-      <c r="C142" s="55"/>
+      <c r="C142" s="147"/>
       <c r="D142" s="55"/>
       <c r="E142" s="55"/>
       <c r="F142" s="132"/>
@@ -19109,7 +19109,7 @@
         <v>92</v>
       </c>
       <c r="T142" s="61"/>
-      <c r="U142" s="55"/>
+      <c r="U142" s="154"/>
       <c r="V142" s="55"/>
       <c r="W142" s="55"/>
       <c r="X142" s="55"/>
@@ -19156,7 +19156,7 @@
     <row r="143" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="134"/>
       <c r="B143" s="135"/>
-      <c r="C143" s="55"/>
+      <c r="C143" s="147"/>
       <c r="D143" s="55"/>
       <c r="E143" s="55"/>
       <c r="F143" s="132"/>
@@ -19200,7 +19200,7 @@
         <v>92</v>
       </c>
       <c r="T143" s="61"/>
-      <c r="U143" s="55"/>
+      <c r="U143" s="154"/>
       <c r="V143" s="55"/>
       <c r="W143" s="55"/>
       <c r="X143" s="55"/>
@@ -19247,7 +19247,7 @@
     <row r="144" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="134"/>
       <c r="B144" s="135"/>
-      <c r="C144" s="55"/>
+      <c r="C144" s="147"/>
       <c r="D144" s="55"/>
       <c r="E144" s="55"/>
       <c r="F144" s="132"/>
@@ -19291,7 +19291,7 @@
         <v>92</v>
       </c>
       <c r="T144" s="61"/>
-      <c r="U144" s="55"/>
+      <c r="U144" s="154"/>
       <c r="V144" s="55"/>
       <c r="W144" s="55"/>
       <c r="X144" s="55"/>
@@ -19338,7 +19338,7 @@
     <row r="145" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="134"/>
       <c r="B145" s="135"/>
-      <c r="C145" s="55"/>
+      <c r="C145" s="147"/>
       <c r="D145" s="55"/>
       <c r="E145" s="55"/>
       <c r="F145" s="132"/>
@@ -19382,7 +19382,7 @@
         <v>92</v>
       </c>
       <c r="T145" s="61"/>
-      <c r="U145" s="55"/>
+      <c r="U145" s="154"/>
       <c r="V145" s="55"/>
       <c r="W145" s="55"/>
       <c r="X145" s="55"/>
@@ -19429,7 +19429,7 @@
     <row r="146" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" s="134"/>
       <c r="B146" s="135"/>
-      <c r="C146" s="55"/>
+      <c r="C146" s="147"/>
       <c r="D146" s="55"/>
       <c r="E146" s="55"/>
       <c r="F146" s="132"/>
@@ -19473,7 +19473,7 @@
         <v>92</v>
       </c>
       <c r="T146" s="61"/>
-      <c r="U146" s="55"/>
+      <c r="U146" s="154"/>
       <c r="V146" s="55"/>
       <c r="W146" s="55"/>
       <c r="X146" s="55"/>
@@ -19520,7 +19520,7 @@
     <row r="147" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="134"/>
       <c r="B147" s="135"/>
-      <c r="C147" s="55"/>
+      <c r="C147" s="147"/>
       <c r="D147" s="55"/>
       <c r="E147" s="55"/>
       <c r="F147" s="132"/>
@@ -19564,7 +19564,7 @@
         <v>92</v>
       </c>
       <c r="T147" s="61"/>
-      <c r="U147" s="55"/>
+      <c r="U147" s="154"/>
       <c r="V147" s="55"/>
       <c r="W147" s="55"/>
       <c r="X147" s="55"/>
@@ -19611,7 +19611,7 @@
     <row r="148" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="134"/>
       <c r="B148" s="135"/>
-      <c r="C148" s="55"/>
+      <c r="C148" s="147"/>
       <c r="D148" s="55"/>
       <c r="E148" s="55"/>
       <c r="F148" s="132"/>
@@ -19655,7 +19655,7 @@
         <v>92</v>
       </c>
       <c r="T148" s="61"/>
-      <c r="U148" s="55"/>
+      <c r="U148" s="154"/>
       <c r="V148" s="55"/>
       <c r="W148" s="55"/>
       <c r="X148" s="55"/>
@@ -19702,7 +19702,7 @@
     <row r="149" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="134"/>
       <c r="B149" s="135"/>
-      <c r="C149" s="55"/>
+      <c r="C149" s="147"/>
       <c r="D149" s="55"/>
       <c r="E149" s="55"/>
       <c r="F149" s="132"/>
@@ -19746,7 +19746,7 @@
         <v>92</v>
       </c>
       <c r="T149" s="61"/>
-      <c r="U149" s="55"/>
+      <c r="U149" s="154"/>
       <c r="V149" s="55"/>
       <c r="W149" s="55"/>
       <c r="X149" s="55"/>
@@ -19793,7 +19793,7 @@
     <row r="150" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="134"/>
       <c r="B150" s="135"/>
-      <c r="C150" s="55"/>
+      <c r="C150" s="147"/>
       <c r="D150" s="55"/>
       <c r="E150" s="55"/>
       <c r="F150" s="132"/>
@@ -19837,7 +19837,7 @@
         <v>92</v>
       </c>
       <c r="T150" s="61"/>
-      <c r="U150" s="55"/>
+      <c r="U150" s="154"/>
       <c r="V150" s="55"/>
       <c r="W150" s="55"/>
       <c r="X150" s="55"/>
@@ -19884,7 +19884,7 @@
     <row r="151" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="134"/>
       <c r="B151" s="135"/>
-      <c r="C151" s="55"/>
+      <c r="C151" s="147"/>
       <c r="D151" s="55"/>
       <c r="E151" s="55"/>
       <c r="F151" s="132"/>
@@ -19928,7 +19928,7 @@
         <v>92</v>
       </c>
       <c r="T151" s="61"/>
-      <c r="U151" s="55"/>
+      <c r="U151" s="154"/>
       <c r="V151" s="55"/>
       <c r="W151" s="55"/>
       <c r="X151" s="55"/>
@@ -19975,7 +19975,7 @@
     <row r="152" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="134"/>
       <c r="B152" s="135"/>
-      <c r="C152" s="55"/>
+      <c r="C152" s="147"/>
       <c r="D152" s="55"/>
       <c r="E152" s="55"/>
       <c r="F152" s="132"/>
@@ -20019,7 +20019,7 @@
         <v>92</v>
       </c>
       <c r="T152" s="61"/>
-      <c r="U152" s="55"/>
+      <c r="U152" s="154"/>
       <c r="V152" s="55"/>
       <c r="W152" s="55"/>
       <c r="X152" s="55"/>
@@ -20066,7 +20066,7 @@
     <row r="153" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="134"/>
       <c r="B153" s="135"/>
-      <c r="C153" s="55"/>
+      <c r="C153" s="147"/>
       <c r="D153" s="55"/>
       <c r="E153" s="55"/>
       <c r="F153" s="132"/>
@@ -20110,7 +20110,7 @@
         <v>92</v>
       </c>
       <c r="T153" s="61"/>
-      <c r="U153" s="55"/>
+      <c r="U153" s="154"/>
       <c r="V153" s="55"/>
       <c r="W153" s="55"/>
       <c r="X153" s="55"/>
@@ -20157,7 +20157,7 @@
     <row r="154" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="134"/>
       <c r="B154" s="135"/>
-      <c r="C154" s="55"/>
+      <c r="C154" s="147"/>
       <c r="D154" s="55"/>
       <c r="E154" s="55"/>
       <c r="F154" s="132"/>
@@ -20201,7 +20201,7 @@
         <v>92</v>
       </c>
       <c r="T154" s="61"/>
-      <c r="U154" s="55"/>
+      <c r="U154" s="154"/>
       <c r="V154" s="55"/>
       <c r="W154" s="55"/>
       <c r="X154" s="55"/>
@@ -20248,7 +20248,7 @@
     <row r="155" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="134"/>
       <c r="B155" s="135"/>
-      <c r="C155" s="55"/>
+      <c r="C155" s="147"/>
       <c r="D155" s="55"/>
       <c r="E155" s="55"/>
       <c r="F155" s="132"/>
@@ -20292,7 +20292,7 @@
         <v>92</v>
       </c>
       <c r="T155" s="61"/>
-      <c r="U155" s="55"/>
+      <c r="U155" s="154"/>
       <c r="V155" s="55"/>
       <c r="W155" s="55"/>
       <c r="X155" s="55"/>
@@ -20339,7 +20339,7 @@
     <row r="156" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="134"/>
       <c r="B156" s="135"/>
-      <c r="C156" s="55"/>
+      <c r="C156" s="147"/>
       <c r="D156" s="55"/>
       <c r="E156" s="55"/>
       <c r="F156" s="132"/>
@@ -20383,7 +20383,7 @@
         <v>92</v>
       </c>
       <c r="T156" s="61"/>
-      <c r="U156" s="55"/>
+      <c r="U156" s="154"/>
       <c r="V156" s="55"/>
       <c r="W156" s="55"/>
       <c r="X156" s="55"/>
@@ -20430,7 +20430,7 @@
     <row r="157" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="134"/>
       <c r="B157" s="135"/>
-      <c r="C157" s="55"/>
+      <c r="C157" s="147"/>
       <c r="D157" s="55"/>
       <c r="E157" s="55"/>
       <c r="F157" s="132"/>
@@ -20474,7 +20474,7 @@
         <v>92</v>
       </c>
       <c r="T157" s="61"/>
-      <c r="U157" s="55"/>
+      <c r="U157" s="154"/>
       <c r="V157" s="55"/>
       <c r="W157" s="55"/>
       <c r="X157" s="55"/>
@@ -20521,7 +20521,7 @@
     <row r="158" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="134"/>
       <c r="B158" s="135"/>
-      <c r="C158" s="55"/>
+      <c r="C158" s="147"/>
       <c r="D158" s="55"/>
       <c r="E158" s="55"/>
       <c r="F158" s="132"/>
@@ -20565,7 +20565,7 @@
         <v>92</v>
       </c>
       <c r="T158" s="61"/>
-      <c r="U158" s="55"/>
+      <c r="U158" s="154"/>
       <c r="V158" s="55"/>
       <c r="W158" s="55"/>
       <c r="X158" s="55"/>
@@ -20612,7 +20612,7 @@
     <row r="159" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="134"/>
       <c r="B159" s="135"/>
-      <c r="C159" s="55"/>
+      <c r="C159" s="147"/>
       <c r="D159" s="55"/>
       <c r="E159" s="55"/>
       <c r="F159" s="132"/>
@@ -20656,7 +20656,7 @@
         <v>92</v>
       </c>
       <c r="T159" s="61"/>
-      <c r="U159" s="55"/>
+      <c r="U159" s="154"/>
       <c r="V159" s="55"/>
       <c r="W159" s="55"/>
       <c r="X159" s="55"/>
@@ -20703,7 +20703,7 @@
     <row r="160" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="134"/>
       <c r="B160" s="135"/>
-      <c r="C160" s="55"/>
+      <c r="C160" s="147"/>
       <c r="D160" s="55"/>
       <c r="E160" s="55"/>
       <c r="F160" s="132"/>
@@ -20747,7 +20747,7 @@
         <v>92</v>
       </c>
       <c r="T160" s="61"/>
-      <c r="U160" s="55"/>
+      <c r="U160" s="154"/>
       <c r="V160" s="55"/>
       <c r="W160" s="55"/>
       <c r="X160" s="55"/>
@@ -20794,7 +20794,7 @@
     <row r="161" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="134"/>
       <c r="B161" s="135"/>
-      <c r="C161" s="55"/>
+      <c r="C161" s="147"/>
       <c r="D161" s="55"/>
       <c r="E161" s="55"/>
       <c r="F161" s="132"/>
@@ -20838,7 +20838,7 @@
         <v>92</v>
       </c>
       <c r="T161" s="61"/>
-      <c r="U161" s="55"/>
+      <c r="U161" s="154"/>
       <c r="V161" s="55"/>
       <c r="W161" s="55"/>
       <c r="X161" s="55"/>
@@ -20885,7 +20885,7 @@
     <row r="162" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="134"/>
       <c r="B162" s="135"/>
-      <c r="C162" s="55"/>
+      <c r="C162" s="147"/>
       <c r="D162" s="55"/>
       <c r="E162" s="55"/>
       <c r="F162" s="132"/>
@@ -20929,7 +20929,7 @@
         <v>92</v>
       </c>
       <c r="T162" s="61"/>
-      <c r="U162" s="55"/>
+      <c r="U162" s="154"/>
       <c r="V162" s="55"/>
       <c r="W162" s="55"/>
       <c r="X162" s="55"/>
@@ -20976,7 +20976,7 @@
     <row r="163" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="134"/>
       <c r="B163" s="135"/>
-      <c r="C163" s="55"/>
+      <c r="C163" s="147"/>
       <c r="D163" s="55"/>
       <c r="E163" s="55"/>
       <c r="F163" s="132"/>
@@ -21020,7 +21020,7 @@
         <v>92</v>
       </c>
       <c r="T163" s="61"/>
-      <c r="U163" s="55"/>
+      <c r="U163" s="154"/>
       <c r="V163" s="55"/>
       <c r="W163" s="55"/>
       <c r="X163" s="55"/>
@@ -21067,7 +21067,7 @@
     <row r="164" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="134"/>
       <c r="B164" s="135"/>
-      <c r="C164" s="55"/>
+      <c r="C164" s="147"/>
       <c r="D164" s="55"/>
       <c r="E164" s="55"/>
       <c r="F164" s="132"/>
@@ -21111,7 +21111,7 @@
         <v>92</v>
       </c>
       <c r="T164" s="61"/>
-      <c r="U164" s="55"/>
+      <c r="U164" s="154"/>
       <c r="V164" s="55"/>
       <c r="W164" s="55"/>
       <c r="X164" s="55"/>
@@ -21158,7 +21158,7 @@
     <row r="165" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="134"/>
       <c r="B165" s="135"/>
-      <c r="C165" s="55"/>
+      <c r="C165" s="147"/>
       <c r="D165" s="55"/>
       <c r="E165" s="55"/>
       <c r="F165" s="132"/>
@@ -21202,7 +21202,7 @@
         <v>92</v>
       </c>
       <c r="T165" s="61"/>
-      <c r="U165" s="55"/>
+      <c r="U165" s="154"/>
       <c r="V165" s="55"/>
       <c r="W165" s="55"/>
       <c r="X165" s="55"/>
@@ -21249,7 +21249,7 @@
     <row r="166" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="134"/>
       <c r="B166" s="135"/>
-      <c r="C166" s="55"/>
+      <c r="C166" s="147"/>
       <c r="D166" s="55"/>
       <c r="E166" s="55"/>
       <c r="F166" s="132"/>
@@ -21293,7 +21293,7 @@
         <v>92</v>
       </c>
       <c r="T166" s="61"/>
-      <c r="U166" s="55"/>
+      <c r="U166" s="154"/>
       <c r="V166" s="55"/>
       <c r="W166" s="55"/>
       <c r="X166" s="55"/>
@@ -21340,7 +21340,7 @@
     <row r="167" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="134"/>
       <c r="B167" s="135"/>
-      <c r="C167" s="55"/>
+      <c r="C167" s="147"/>
       <c r="D167" s="55"/>
       <c r="E167" s="55"/>
       <c r="F167" s="132"/>
@@ -21384,7 +21384,7 @@
         <v>92</v>
       </c>
       <c r="T167" s="61"/>
-      <c r="U167" s="55"/>
+      <c r="U167" s="154"/>
       <c r="V167" s="55"/>
       <c r="W167" s="55"/>
       <c r="X167" s="55"/>
@@ -21431,7 +21431,7 @@
     <row r="168" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="134"/>
       <c r="B168" s="135"/>
-      <c r="C168" s="55"/>
+      <c r="C168" s="147"/>
       <c r="D168" s="55"/>
       <c r="E168" s="55"/>
       <c r="F168" s="132"/>
@@ -21475,7 +21475,7 @@
         <v>92</v>
       </c>
       <c r="T168" s="61"/>
-      <c r="U168" s="55"/>
+      <c r="U168" s="154"/>
       <c r="V168" s="55"/>
       <c r="W168" s="55"/>
       <c r="X168" s="55"/>
@@ -21522,7 +21522,7 @@
     <row r="169" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" s="134"/>
       <c r="B169" s="135"/>
-      <c r="C169" s="55"/>
+      <c r="C169" s="147"/>
       <c r="D169" s="55"/>
       <c r="E169" s="55"/>
       <c r="F169" s="132"/>
@@ -21566,7 +21566,7 @@
         <v>92</v>
       </c>
       <c r="T169" s="61"/>
-      <c r="U169" s="55"/>
+      <c r="U169" s="154"/>
       <c r="V169" s="55"/>
       <c r="W169" s="55"/>
       <c r="X169" s="55"/>
@@ -21613,7 +21613,7 @@
     <row r="170" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="134"/>
       <c r="B170" s="135"/>
-      <c r="C170" s="55"/>
+      <c r="C170" s="147"/>
       <c r="D170" s="55"/>
       <c r="E170" s="55"/>
       <c r="F170" s="132"/>
@@ -21657,7 +21657,7 @@
         <v>92</v>
       </c>
       <c r="T170" s="61"/>
-      <c r="U170" s="55"/>
+      <c r="U170" s="154"/>
       <c r="V170" s="55"/>
       <c r="W170" s="55"/>
       <c r="X170" s="55"/>
@@ -21704,7 +21704,7 @@
     <row r="171" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="134"/>
       <c r="B171" s="135"/>
-      <c r="C171" s="55"/>
+      <c r="C171" s="147"/>
       <c r="D171" s="55"/>
       <c r="E171" s="55"/>
       <c r="F171" s="132"/>
@@ -21748,7 +21748,7 @@
         <v>92</v>
       </c>
       <c r="T171" s="61"/>
-      <c r="U171" s="55"/>
+      <c r="U171" s="154"/>
       <c r="V171" s="55"/>
       <c r="W171" s="55"/>
       <c r="X171" s="55"/>
@@ -21795,7 +21795,7 @@
     <row r="172" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" s="134"/>
       <c r="B172" s="135"/>
-      <c r="C172" s="55"/>
+      <c r="C172" s="147"/>
       <c r="D172" s="55"/>
       <c r="E172" s="55"/>
       <c r="F172" s="132"/>
@@ -21839,7 +21839,7 @@
         <v>92</v>
       </c>
       <c r="T172" s="61"/>
-      <c r="U172" s="55"/>
+      <c r="U172" s="154"/>
       <c r="V172" s="55"/>
       <c r="W172" s="55"/>
       <c r="X172" s="55"/>
@@ -21886,7 +21886,7 @@
     <row r="173" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="134"/>
       <c r="B173" s="135"/>
-      <c r="C173" s="55"/>
+      <c r="C173" s="147"/>
       <c r="D173" s="55"/>
       <c r="E173" s="55"/>
       <c r="F173" s="132"/>
@@ -21930,7 +21930,7 @@
         <v>92</v>
       </c>
       <c r="T173" s="61"/>
-      <c r="U173" s="55"/>
+      <c r="U173" s="154"/>
       <c r="V173" s="55"/>
       <c r="W173" s="55"/>
       <c r="X173" s="55"/>
@@ -21977,7 +21977,7 @@
     <row r="174" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="134"/>
       <c r="B174" s="135"/>
-      <c r="C174" s="55"/>
+      <c r="C174" s="147"/>
       <c r="D174" s="55"/>
       <c r="E174" s="55"/>
       <c r="F174" s="132"/>
@@ -22021,7 +22021,7 @@
         <v>92</v>
       </c>
       <c r="T174" s="61"/>
-      <c r="U174" s="55"/>
+      <c r="U174" s="154"/>
       <c r="V174" s="55"/>
       <c r="W174" s="55"/>
       <c r="X174" s="55"/>
@@ -22068,7 +22068,7 @@
     <row r="175" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" s="134"/>
       <c r="B175" s="135"/>
-      <c r="C175" s="55"/>
+      <c r="C175" s="147"/>
       <c r="D175" s="55"/>
       <c r="E175" s="55"/>
       <c r="F175" s="132"/>
@@ -22112,7 +22112,7 @@
         <v>92</v>
       </c>
       <c r="T175" s="61"/>
-      <c r="U175" s="55"/>
+      <c r="U175" s="154"/>
       <c r="V175" s="55"/>
       <c r="W175" s="55"/>
       <c r="X175" s="55"/>
@@ -22159,7 +22159,7 @@
     <row r="176" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" s="134"/>
       <c r="B176" s="135"/>
-      <c r="C176" s="55"/>
+      <c r="C176" s="147"/>
       <c r="D176" s="55"/>
       <c r="E176" s="55"/>
       <c r="F176" s="132"/>
@@ -22203,7 +22203,7 @@
         <v>92</v>
       </c>
       <c r="T176" s="61"/>
-      <c r="U176" s="55"/>
+      <c r="U176" s="154"/>
       <c r="V176" s="55"/>
       <c r="W176" s="55"/>
       <c r="X176" s="55"/>
@@ -22250,7 +22250,7 @@
     <row r="177" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="134"/>
       <c r="B177" s="135"/>
-      <c r="C177" s="55"/>
+      <c r="C177" s="147"/>
       <c r="D177" s="55"/>
       <c r="E177" s="55"/>
       <c r="F177" s="132"/>
@@ -22294,7 +22294,7 @@
         <v>92</v>
       </c>
       <c r="T177" s="61"/>
-      <c r="U177" s="55"/>
+      <c r="U177" s="154"/>
       <c r="V177" s="55"/>
       <c r="W177" s="55"/>
       <c r="X177" s="55"/>
@@ -22341,7 +22341,7 @@
     <row r="178" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="134"/>
       <c r="B178" s="135"/>
-      <c r="C178" s="55"/>
+      <c r="C178" s="147"/>
       <c r="D178" s="55"/>
       <c r="E178" s="55"/>
       <c r="F178" s="132"/>
@@ -22385,7 +22385,7 @@
         <v>92</v>
       </c>
       <c r="T178" s="61"/>
-      <c r="U178" s="55"/>
+      <c r="U178" s="154"/>
       <c r="V178" s="55"/>
       <c r="W178" s="55"/>
       <c r="X178" s="55"/>
@@ -22432,7 +22432,7 @@
     <row r="179" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="134"/>
       <c r="B179" s="135"/>
-      <c r="C179" s="55"/>
+      <c r="C179" s="147"/>
       <c r="D179" s="55"/>
       <c r="E179" s="55"/>
       <c r="F179" s="132"/>
@@ -22476,7 +22476,7 @@
         <v>92</v>
       </c>
       <c r="T179" s="61"/>
-      <c r="U179" s="55"/>
+      <c r="U179" s="154"/>
       <c r="V179" s="55"/>
       <c r="W179" s="55"/>
       <c r="X179" s="55"/>
@@ -22523,7 +22523,7 @@
     <row r="180" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="134"/>
       <c r="B180" s="135"/>
-      <c r="C180" s="55"/>
+      <c r="C180" s="147"/>
       <c r="D180" s="55"/>
       <c r="E180" s="55"/>
       <c r="F180" s="132"/>
@@ -22567,7 +22567,7 @@
         <v>92</v>
       </c>
       <c r="T180" s="61"/>
-      <c r="U180" s="55"/>
+      <c r="U180" s="154"/>
       <c r="V180" s="55"/>
       <c r="W180" s="55"/>
       <c r="X180" s="55"/>
@@ -22614,7 +22614,7 @@
     <row r="181" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="134"/>
       <c r="B181" s="135"/>
-      <c r="C181" s="55"/>
+      <c r="C181" s="147"/>
       <c r="D181" s="55"/>
       <c r="E181" s="55"/>
       <c r="F181" s="132"/>
@@ -22658,7 +22658,7 @@
         <v>92</v>
       </c>
       <c r="T181" s="61"/>
-      <c r="U181" s="55"/>
+      <c r="U181" s="154"/>
       <c r="V181" s="55"/>
       <c r="W181" s="55"/>
       <c r="X181" s="55"/>
@@ -22705,7 +22705,7 @@
     <row r="182" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="134"/>
       <c r="B182" s="135"/>
-      <c r="C182" s="55"/>
+      <c r="C182" s="147"/>
       <c r="D182" s="55"/>
       <c r="E182" s="55"/>
       <c r="F182" s="132"/>
@@ -22749,7 +22749,7 @@
         <v>92</v>
       </c>
       <c r="T182" s="61"/>
-      <c r="U182" s="55"/>
+      <c r="U182" s="154"/>
       <c r="V182" s="55"/>
       <c r="W182" s="55"/>
       <c r="X182" s="55"/>
@@ -22796,7 +22796,7 @@
     <row r="183" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="134"/>
       <c r="B183" s="135"/>
-      <c r="C183" s="55"/>
+      <c r="C183" s="147"/>
       <c r="D183" s="55"/>
       <c r="E183" s="55"/>
       <c r="F183" s="132"/>
@@ -22840,7 +22840,7 @@
         <v>92</v>
       </c>
       <c r="T183" s="61"/>
-      <c r="U183" s="55"/>
+      <c r="U183" s="154"/>
       <c r="V183" s="55"/>
       <c r="W183" s="55"/>
       <c r="X183" s="55"/>
@@ -22887,7 +22887,7 @@
     <row r="184" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="134"/>
       <c r="B184" s="135"/>
-      <c r="C184" s="55"/>
+      <c r="C184" s="147"/>
       <c r="D184" s="55"/>
       <c r="E184" s="55"/>
       <c r="F184" s="132"/>
@@ -22931,7 +22931,7 @@
         <v>92</v>
       </c>
       <c r="T184" s="61"/>
-      <c r="U184" s="55"/>
+      <c r="U184" s="154"/>
       <c r="V184" s="55"/>
       <c r="W184" s="55"/>
       <c r="X184" s="55"/>
@@ -22978,7 +22978,7 @@
     <row r="185" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="134"/>
       <c r="B185" s="135"/>
-      <c r="C185" s="55"/>
+      <c r="C185" s="147"/>
       <c r="D185" s="55"/>
       <c r="E185" s="55"/>
       <c r="F185" s="132"/>
@@ -23022,7 +23022,7 @@
         <v>92</v>
       </c>
       <c r="T185" s="61"/>
-      <c r="U185" s="55"/>
+      <c r="U185" s="154"/>
       <c r="V185" s="55"/>
       <c r="W185" s="55"/>
       <c r="X185" s="55"/>
@@ -23069,7 +23069,7 @@
     <row r="186" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="134"/>
       <c r="B186" s="135"/>
-      <c r="C186" s="55"/>
+      <c r="C186" s="147"/>
       <c r="D186" s="55"/>
       <c r="E186" s="55"/>
       <c r="F186" s="132"/>
@@ -23113,7 +23113,7 @@
         <v>92</v>
       </c>
       <c r="T186" s="61"/>
-      <c r="U186" s="55"/>
+      <c r="U186" s="154"/>
       <c r="V186" s="55"/>
       <c r="W186" s="55"/>
       <c r="X186" s="55"/>
@@ -23160,7 +23160,7 @@
     <row r="187" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="134"/>
       <c r="B187" s="135"/>
-      <c r="C187" s="55"/>
+      <c r="C187" s="147"/>
       <c r="D187" s="55"/>
       <c r="E187" s="55"/>
       <c r="F187" s="132"/>
@@ -23204,7 +23204,7 @@
         <v>92</v>
       </c>
       <c r="T187" s="61"/>
-      <c r="U187" s="55"/>
+      <c r="U187" s="154"/>
       <c r="V187" s="55"/>
       <c r="W187" s="55"/>
       <c r="X187" s="55"/>
@@ -23251,7 +23251,7 @@
     <row r="188" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="134"/>
       <c r="B188" s="135"/>
-      <c r="C188" s="55"/>
+      <c r="C188" s="147"/>
       <c r="D188" s="55"/>
       <c r="E188" s="55"/>
       <c r="F188" s="132"/>
@@ -23295,7 +23295,7 @@
         <v>92</v>
       </c>
       <c r="T188" s="61"/>
-      <c r="U188" s="55"/>
+      <c r="U188" s="154"/>
       <c r="V188" s="55"/>
       <c r="W188" s="55"/>
       <c r="X188" s="55"/>
@@ -23342,7 +23342,7 @@
     <row r="189" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="134"/>
       <c r="B189" s="135"/>
-      <c r="C189" s="55"/>
+      <c r="C189" s="147"/>
       <c r="D189" s="55"/>
       <c r="E189" s="55"/>
       <c r="F189" s="132"/>
@@ -23386,7 +23386,7 @@
         <v>92</v>
       </c>
       <c r="T189" s="61"/>
-      <c r="U189" s="55"/>
+      <c r="U189" s="154"/>
       <c r="V189" s="55"/>
       <c r="W189" s="55"/>
       <c r="X189" s="55"/>
@@ -23433,7 +23433,7 @@
     <row r="190" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" s="134"/>
       <c r="B190" s="135"/>
-      <c r="C190" s="55"/>
+      <c r="C190" s="147"/>
       <c r="D190" s="55"/>
       <c r="E190" s="55"/>
       <c r="F190" s="132"/>
@@ -23477,7 +23477,7 @@
         <v>92</v>
       </c>
       <c r="T190" s="61"/>
-      <c r="U190" s="55"/>
+      <c r="U190" s="154"/>
       <c r="V190" s="55"/>
       <c r="W190" s="55"/>
       <c r="X190" s="55"/>
@@ -23524,7 +23524,7 @@
     <row r="191" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" s="134"/>
       <c r="B191" s="135"/>
-      <c r="C191" s="55"/>
+      <c r="C191" s="147"/>
       <c r="D191" s="55"/>
       <c r="E191" s="55"/>
       <c r="F191" s="132"/>
@@ -23568,7 +23568,7 @@
         <v>92</v>
       </c>
       <c r="T191" s="61"/>
-      <c r="U191" s="55"/>
+      <c r="U191" s="154"/>
       <c r="V191" s="55"/>
       <c r="W191" s="55"/>
       <c r="X191" s="55"/>
@@ -23615,7 +23615,7 @@
     <row r="192" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="134"/>
       <c r="B192" s="135"/>
-      <c r="C192" s="55"/>
+      <c r="C192" s="147"/>
       <c r="D192" s="55"/>
       <c r="E192" s="55"/>
       <c r="F192" s="132"/>
@@ -23659,7 +23659,7 @@
         <v>92</v>
       </c>
       <c r="T192" s="61"/>
-      <c r="U192" s="55"/>
+      <c r="U192" s="154"/>
       <c r="V192" s="55"/>
       <c r="W192" s="55"/>
       <c r="X192" s="55"/>
@@ -23706,7 +23706,7 @@
     <row r="193" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" s="134"/>
       <c r="B193" s="135"/>
-      <c r="C193" s="55"/>
+      <c r="C193" s="147"/>
       <c r="D193" s="55"/>
       <c r="E193" s="55"/>
       <c r="F193" s="132"/>
@@ -23750,7 +23750,7 @@
         <v>92</v>
       </c>
       <c r="T193" s="61"/>
-      <c r="U193" s="55"/>
+      <c r="U193" s="154"/>
       <c r="V193" s="55"/>
       <c r="W193" s="55"/>
       <c r="X193" s="55"/>
@@ -23797,7 +23797,7 @@
     <row r="194" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" s="134"/>
       <c r="B194" s="135"/>
-      <c r="C194" s="55"/>
+      <c r="C194" s="147"/>
       <c r="D194" s="55"/>
       <c r="E194" s="55"/>
       <c r="F194" s="132"/>
@@ -23841,7 +23841,7 @@
         <v>92</v>
       </c>
       <c r="T194" s="61"/>
-      <c r="U194" s="55"/>
+      <c r="U194" s="154"/>
       <c r="V194" s="55"/>
       <c r="W194" s="55"/>
       <c r="X194" s="55"/>
@@ -23888,7 +23888,7 @@
     <row r="195" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" s="134"/>
       <c r="B195" s="135"/>
-      <c r="C195" s="55"/>
+      <c r="C195" s="147"/>
       <c r="D195" s="55"/>
       <c r="E195" s="55"/>
       <c r="F195" s="132"/>
@@ -23932,7 +23932,7 @@
         <v>92</v>
       </c>
       <c r="T195" s="61"/>
-      <c r="U195" s="55"/>
+      <c r="U195" s="154"/>
       <c r="V195" s="55"/>
       <c r="W195" s="55"/>
       <c r="X195" s="55"/>
@@ -23979,7 +23979,7 @@
     <row r="196" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" s="134"/>
       <c r="B196" s="135"/>
-      <c r="C196" s="55"/>
+      <c r="C196" s="147"/>
       <c r="D196" s="55"/>
       <c r="E196" s="55"/>
       <c r="F196" s="132"/>
@@ -24023,7 +24023,7 @@
         <v>92</v>
       </c>
       <c r="T196" s="61"/>
-      <c r="U196" s="55"/>
+      <c r="U196" s="154"/>
       <c r="V196" s="55"/>
       <c r="W196" s="55"/>
       <c r="X196" s="55"/>
@@ -24070,7 +24070,7 @@
     <row r="197" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" s="134"/>
       <c r="B197" s="135"/>
-      <c r="C197" s="55"/>
+      <c r="C197" s="147"/>
       <c r="D197" s="55"/>
       <c r="E197" s="55"/>
       <c r="F197" s="132"/>
@@ -24114,7 +24114,7 @@
         <v>92</v>
       </c>
       <c r="T197" s="61"/>
-      <c r="U197" s="55"/>
+      <c r="U197" s="154"/>
       <c r="V197" s="55"/>
       <c r="W197" s="55"/>
       <c r="X197" s="55"/>
@@ -24161,7 +24161,7 @@
     <row r="198" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="134"/>
       <c r="B198" s="135"/>
-      <c r="C198" s="55"/>
+      <c r="C198" s="147"/>
       <c r="D198" s="55"/>
       <c r="E198" s="55"/>
       <c r="F198" s="132"/>
@@ -24205,7 +24205,7 @@
         <v>92</v>
       </c>
       <c r="T198" s="61"/>
-      <c r="U198" s="55"/>
+      <c r="U198" s="154"/>
       <c r="V198" s="55"/>
       <c r="W198" s="55"/>
       <c r="X198" s="55"/>
@@ -24252,7 +24252,7 @@
     <row r="199" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" s="134"/>
       <c r="B199" s="135"/>
-      <c r="C199" s="55"/>
+      <c r="C199" s="147"/>
       <c r="D199" s="55"/>
       <c r="E199" s="55"/>
       <c r="F199" s="132"/>
@@ -24296,7 +24296,7 @@
         <v>92</v>
       </c>
       <c r="T199" s="61"/>
-      <c r="U199" s="55"/>
+      <c r="U199" s="154"/>
       <c r="V199" s="55"/>
       <c r="W199" s="55"/>
       <c r="X199" s="55"/>
@@ -24343,7 +24343,7 @@
     <row r="200" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" s="134"/>
       <c r="B200" s="135"/>
-      <c r="C200" s="55"/>
+      <c r="C200" s="147"/>
       <c r="D200" s="55"/>
       <c r="E200" s="55"/>
       <c r="F200" s="132"/>
@@ -24387,7 +24387,7 @@
         <v>92</v>
       </c>
       <c r="T200" s="61"/>
-      <c r="U200" s="55"/>
+      <c r="U200" s="154"/>
       <c r="V200" s="55"/>
       <c r="W200" s="55"/>
       <c r="X200" s="55"/>
@@ -24434,7 +24434,7 @@
     <row r="201" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" s="134"/>
       <c r="B201" s="135"/>
-      <c r="C201" s="55"/>
+      <c r="C201" s="147"/>
       <c r="D201" s="55"/>
       <c r="E201" s="55"/>
       <c r="F201" s="132"/>
@@ -24478,7 +24478,7 @@
         <v>92</v>
       </c>
       <c r="T201" s="61"/>
-      <c r="U201" s="55"/>
+      <c r="U201" s="154"/>
       <c r="V201" s="55"/>
       <c r="W201" s="55"/>
       <c r="X201" s="55"/>
@@ -24525,7 +24525,7 @@
     <row r="202" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" s="134"/>
       <c r="B202" s="135"/>
-      <c r="C202" s="55"/>
+      <c r="C202" s="147"/>
       <c r="D202" s="55"/>
       <c r="E202" s="55"/>
       <c r="F202" s="132"/>
@@ -24569,7 +24569,7 @@
         <v>92</v>
       </c>
       <c r="T202" s="61"/>
-      <c r="U202" s="55"/>
+      <c r="U202" s="154"/>
       <c r="V202" s="55"/>
       <c r="W202" s="55"/>
       <c r="X202" s="55"/>
@@ -25165,7 +25165,7 @@
     <mergeCell ref="B1:R1"/>
     <mergeCell ref="T1:AH1"/>
   </mergeCells>
-  <conditionalFormatting sqref="Z4:AB4 Z3:AG3 Y5:AB16 T6:T12 S4:S203 AJ102:AM202 AC102:AH102 C3:E3 C102:R102 B203:B371 G3 I3:Q3 S3:T3 AI3:AI203 T102:AB202 I98:Q99 G100:Q101 G92:Q97 C4:Q88 C106:R202 I103:Q105 C92:E101 C93:H95 I89:Q91 G96:H101 AC4:AG101 AC104:AH202 AC103:AG103 T17:AB29 Y30:AB101 T92:T101 T30:T88 AJ98:AJ101 AL3:AM101">
+  <conditionalFormatting sqref="Z4:AB4 Z3:AG3 Y5:AB16 T6:T12 S4:S203 AJ102:AM202 AC102:AH102 C3:E3 D102:R102 B203:B371 G3 I3:Q3 S3:T3 AI3:AI203 I98:Q99 G100:Q101 G92:Q97 D106:R202 I103:Q105 D93:H95 I89:Q91 G96:H101 AC4:AG101 AC104:AH202 AC103:AG103 Y30:AB101 T92:T202 T17:T88 AJ98:AJ101 AL3:AM101 C4:Q19 D20:Q88 D92:E101 C20:C202 V17:AB29 V102:AB202">
     <cfRule type="expression" dxfId="266" priority="328">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
@@ -25187,7 +25187,7 @@
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U3:X3 U6:X6 X7 U9:X12 W8:X8">
+  <conditionalFormatting sqref="U3:X3 V6:X6 X7 V9:X12 W8:X8 U4:U202">
     <cfRule type="expression" dxfId="260" priority="316">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
@@ -25297,7 +25297,7 @@
       <formula>$I5&lt;&gt;$Y5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C98 G98 E98">
+  <conditionalFormatting sqref="G98 E98">
     <cfRule type="expression" dxfId="230" priority="283">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
@@ -25341,7 +25341,7 @@
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C99:E99 G99">
+  <conditionalFormatting sqref="D99:E99 G99">
     <cfRule type="expression" dxfId="218" priority="256">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
@@ -25396,7 +25396,7 @@
       <formula>$K92&lt;&gt;$AA92</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C105 E105 G105:H105">
+  <conditionalFormatting sqref="E105 G105:H105">
     <cfRule type="expression" dxfId="203" priority="226">
       <formula>ISBLANK($T105)</formula>
     </cfRule>
@@ -25418,7 +25418,7 @@
       <formula>$K105&lt;&gt;$AA105</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C103 G103 E103">
+  <conditionalFormatting sqref="G103 E103">
     <cfRule type="expression" dxfId="197" priority="220">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
@@ -25462,7 +25462,7 @@
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C104:E104 G104">
+  <conditionalFormatting sqref="D104:E104 G104">
     <cfRule type="expression" dxfId="185" priority="208">
       <formula>ISBLANK($T104)</formula>
     </cfRule>
@@ -25550,7 +25550,7 @@
       <formula>$I99&lt;&gt;$Y99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C91 E91 G91:H91">
+  <conditionalFormatting sqref="E91 G91:H91">
     <cfRule type="expression" dxfId="161" priority="184">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
@@ -25572,7 +25572,7 @@
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C89 G89 E89">
+  <conditionalFormatting sqref="G89 E89">
     <cfRule type="expression" dxfId="155" priority="178">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
@@ -25616,7 +25616,7 @@
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C90:E90 G90">
+  <conditionalFormatting sqref="D90:E90 G90">
     <cfRule type="expression" dxfId="143" priority="166">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
@@ -25704,7 +25704,7 @@
       <formula>$K4&lt;&gt;$AA4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U4:X4">
+  <conditionalFormatting sqref="V4:X4">
     <cfRule type="expression" dxfId="119" priority="142">
       <formula>ISBLANK($T4)</formula>
     </cfRule>
@@ -25726,7 +25726,7 @@
       <formula>$K5&lt;&gt;$AA5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U5:X5">
+  <conditionalFormatting sqref="V5:X5">
     <cfRule type="expression" dxfId="113" priority="136">
       <formula>ISBLANK($T5)</formula>
     </cfRule>
@@ -25748,7 +25748,7 @@
       <formula>$I103&lt;&gt;$Y103</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U7:W7">
+  <conditionalFormatting sqref="V7:W7">
     <cfRule type="expression" dxfId="107" priority="130">
       <formula>ISBLANK($T7)</formula>
     </cfRule>
@@ -25770,7 +25770,7 @@
       <formula>$K13&lt;&gt;$AA13</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U13:X13">
+  <conditionalFormatting sqref="V13:X13">
     <cfRule type="expression" dxfId="101" priority="124">
       <formula>ISBLANK($T13)</formula>
     </cfRule>
@@ -25792,7 +25792,7 @@
       <formula>$K14&lt;&gt;$AA14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U14:X14">
+  <conditionalFormatting sqref="V14:X14">
     <cfRule type="expression" dxfId="95" priority="118">
       <formula>ISBLANK($T14)</formula>
     </cfRule>
@@ -25814,7 +25814,7 @@
       <formula>$K15&lt;&gt;$AA15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U15:X15">
+  <conditionalFormatting sqref="V15:X15">
     <cfRule type="expression" dxfId="89" priority="112">
       <formula>ISBLANK($T15)</formula>
     </cfRule>
@@ -25836,7 +25836,7 @@
       <formula>$K16&lt;&gt;$AA16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U16:X16">
+  <conditionalFormatting sqref="V16:X16">
     <cfRule type="expression" dxfId="83" priority="106">
       <formula>ISBLANK($T16)</formula>
     </cfRule>
@@ -25847,7 +25847,7 @@
       <formula>$K16&lt;&gt;$AA16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U92:W101 U30:W39 U41:W88 W40">
+  <conditionalFormatting sqref="V92:W101 V30:W39 V41:W88 W40">
     <cfRule type="expression" dxfId="80" priority="103">
       <formula>ISBLANK($T30)</formula>
     </cfRule>
@@ -25858,7 +25858,7 @@
       <formula>$K30&lt;&gt;$AA30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U98 W98">
+  <conditionalFormatting sqref="W98">
     <cfRule type="expression" dxfId="77" priority="100">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
@@ -25880,7 +25880,7 @@
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U99:W99">
+  <conditionalFormatting sqref="V99:W99">
     <cfRule type="expression" dxfId="71" priority="94">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
@@ -26023,7 +26023,7 @@
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U89:V91">
+  <conditionalFormatting sqref="V89:V91">
     <cfRule type="expression" dxfId="32" priority="49">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
@@ -26122,7 +26122,7 @@
       <formula>$I8&lt;&gt;$Y8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U40:V40">
+  <conditionalFormatting sqref="V40">
     <cfRule type="expression" dxfId="5" priority="4">
       <formula>ISBLANK($T40)</formula>
     </cfRule>
@@ -26133,7 +26133,7 @@
       <formula>$K40&lt;&gt;$AA40</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U8:V8">
+  <conditionalFormatting sqref="V8">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>ISBLANK($T8)</formula>
     </cfRule>
@@ -28599,18 +28599,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D360421-6903-41F3-93C2-FBADB5CFBCA5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{115A91EE-C02B-43A5-B6F9-CC7805B21DE0}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="aa4bd7cc-4ceb-4a8e-b11a-de8db8ccf9d9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="aa4bd7cc-4ceb-4a8e-b11a-de8db8ccf9d9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ajustar planilha da anac - BASIS-262013
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/reports/planilhas/modelo3-anac.xlsx
+++ b/backend/src/main/resources/reports/planilhas/modelo3-anac.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IBAMA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wilson\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B586618-560A-496B-84C2-AB7EB9C66E73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5084B64C-5E78-46EC-AC10-316A4FFD01A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32770" yWindow="32770" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32770" yWindow="32770" windowWidth="19200" windowHeight="6930" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revisão" sheetId="1" r:id="rId1"/>
@@ -48,12 +48,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,12 +72,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -92,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -118,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -135,7 +135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -163,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
+    <comment ref="R2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -179,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
+    <comment ref="T2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
+    <comment ref="U2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -219,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
+    <comment ref="V2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -235,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
+    <comment ref="W2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -249,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
+    <comment ref="X2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -268,12 +268,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -941,7 +941,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-416]d/mmm"/>
     <numFmt numFmtId="165" formatCode="[$-416]d/m/yyyy"/>
@@ -1971,22 +1971,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="23" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2004,19 +1989,79 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2026,57 +2071,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2106,11 +2106,11 @@
   <cellStyles count="8">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 7" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="3"/>
+    <cellStyle name="Normal 7" xfId="4"/>
     <cellStyle name="Porcentagem" xfId="5" builtinId="5"/>
-    <cellStyle name="Porcentagem 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Porcentagem 2" xfId="6"/>
     <cellStyle name="Vírgula" xfId="7" builtinId="3"/>
   </cellStyles>
   <dxfs count="269">
@@ -4902,10 +4902,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1027" name="_x0000_t202" hidden="1">
+        <xdr:cNvPr id="1026" name="_x0000_t202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A903BDF2-39E0-470A-9D06-B777CE1AD43C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A7F2D73-8EC9-4183-885C-DD512543709F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4951,10 +4951,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1028" name="AutoShape 2">
+        <xdr:cNvPr id="1027" name="AutoShape 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54A8FDB5-E812-4FCD-BA05-41C631369F51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4CBC628-F880-4FFD-A152-53F407885803}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5010,10 +5010,157 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
+        <xdr:cNvPr id="2070" name="_x0000_t202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D10C564-2851-4C02-8F83-F16C2E6FA420}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6350000" cy="6350000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2071" name="_x0000_t202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D319D6B-2399-4C69-8E1C-79D5439F391B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6350000" cy="6350000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2072" name="_x0000_t202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECF1A08D-C2C9-42BC-8D9C-3CAF74746F6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6350000" cy="6350000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
         <xdr:cNvPr id="2073" name="_x0000_t202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03C59B5D-2D31-4F16-8709-6F02A1F4360E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F83C8BD0-C38D-4299-A8B6-0D7D290D370E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5062,7 +5209,7 @@
         <xdr:cNvPr id="2074" name="_x0000_t202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C42E97F-0BA4-4DEC-81C8-4F832B9A08D3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38820986-3736-4404-97C2-9ACA88026EF8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5111,7 +5258,7 @@
         <xdr:cNvPr id="2075" name="_x0000_t202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E05567F-19E9-4485-8C26-F7A75C059A1E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{540412E1-E45F-4904-9467-1229E65A184E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5160,7 +5307,7 @@
         <xdr:cNvPr id="2076" name="_x0000_t202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C9E1B2A-BA6A-4BB7-9127-91000E917EEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2483F2A5-A1F2-4BE9-89EC-8A8CF8C91836}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5209,7 +5356,7 @@
         <xdr:cNvPr id="2077" name="_x0000_t202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32764E44-9F45-46D7-9F95-FB8863BA16E4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2AE6422-CDB0-4F88-AD79-BB8B66E67D71}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5258,7 +5405,7 @@
         <xdr:cNvPr id="2078" name="_x0000_t202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1946E91A-E54B-4632-9044-E23900B52815}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A704E56-A0FF-4FA5-A795-76DF77B3FCA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5307,7 +5454,7 @@
         <xdr:cNvPr id="2079" name="_x0000_t202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6261E746-F434-4C8E-B91F-B3404DE5126E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F24941E8-2731-4210-8A54-7417B8513014}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5356,7 +5503,7 @@
         <xdr:cNvPr id="2080" name="_x0000_t202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4964E21-1806-4CB2-8063-0B14E9DBF8E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AB76243-5912-4575-BB31-2B14FBEDB31F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5402,157 +5549,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2081" name="_x0000_t202" hidden="1">
+        <xdr:cNvPr id="2081" name="AutoShape 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B3C11F3-D5E7-442C-83F5-5F14C4EA0CCF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="6350000" cy="6350000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2082" name="_x0000_t202" hidden="1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75565F5A-B5A7-4B0F-AA39-AE65530AA40B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="6350000" cy="6350000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2083" name="_x0000_t202" hidden="1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{889562CA-A0D5-43B3-8EDA-9441FF46CAA4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="6350000" cy="6350000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2084" name="AutoShape 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{746BEE65-9FCF-4B2C-A637-26A47161F67A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E85B938A-9453-4EE0-BD1C-F48CBC146A3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5603,10 +5603,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2085" name="AutoShape 20">
+        <xdr:cNvPr id="2082" name="AutoShape 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68FCAF8D-B9EB-4A4C-B334-BE8507927EE3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7457178-B9C7-47A3-9656-777D2FBAD778}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5657,10 +5657,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2086" name="AutoShape 18">
+        <xdr:cNvPr id="2083" name="AutoShape 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEB6962C-2D0C-4B66-AF01-5A79EA033FE8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6180CE5-8CE8-4431-8DD4-C0D00B22A363}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5711,10 +5711,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2087" name="AutoShape 16">
+        <xdr:cNvPr id="2084" name="AutoShape 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28BCB2BF-409E-446D-8498-6B04A47F7CAC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98E9BCFF-0D16-4091-B914-00E3900385E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5765,10 +5765,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2088" name="AutoShape 14">
+        <xdr:cNvPr id="2085" name="AutoShape 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59E7888C-F5A5-42B3-820E-36D41463D21F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28AA5A6D-35D8-4843-9CE3-40EBF8DE9EC9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5819,10 +5819,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2089" name="AutoShape 12">
+        <xdr:cNvPr id="2086" name="AutoShape 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CB15C98-FB2C-41D8-B1A4-6384F813385B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAA76B34-53D1-4E9E-B109-F5C54D9C5C76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5873,10 +5873,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2090" name="AutoShape 10">
+        <xdr:cNvPr id="2087" name="AutoShape 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4106DE4B-467D-4FD0-91F6-3FF45AD578E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FE6DBED-5014-4CB1-B705-A6C96151AAED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5927,10 +5927,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2091" name="AutoShape 8">
+        <xdr:cNvPr id="2088" name="AutoShape 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1D01FD5-9E3B-486D-820E-8EAB311B601B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC4C33A-A50E-4E58-8D21-8D7FAB533AA3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5981,10 +5981,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2092" name="AutoShape 6">
+        <xdr:cNvPr id="2089" name="AutoShape 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{371FEE72-1CF7-4655-A756-302A697DD184}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1BC794C-887E-47F6-A629-EFD2515D84FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6035,10 +6035,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2093" name="AutoShape 4">
+        <xdr:cNvPr id="2090" name="AutoShape 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC592523-93AF-4BDB-84C5-805971853EBD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52B5200E-B4C3-4668-A1B9-BC942E23A56A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6089,10 +6089,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2094" name="AutoShape 2">
+        <xdr:cNvPr id="2091" name="AutoShape 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6189BCB4-FE88-4A24-8D4E-322A3626B446}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F5C12B0-F043-4D36-96F0-8A329F3E2609}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6148,10 +6148,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3075" name="_x0000_t202" hidden="1">
+        <xdr:cNvPr id="3074" name="_x0000_t202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3EDD78F-F81F-4F91-BF53-B472A01F67A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7556621B-40B2-4C91-891F-1E7CCE2D964F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6197,10 +6197,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3076" name="AutoShape 2">
+        <xdr:cNvPr id="3075" name="AutoShape 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B38A07F4-DA04-4555-91DB-1C6713848DD6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C78DE341-477E-42D0-A600-8981E2E20EE0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6259,7 +6259,7 @@
         <xdr:cNvPr id="4097" name="Imagem 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F561A33-97B1-4B5D-97BF-7B472FFF7312}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6341824D-7163-4803-A786-7B338F0D11C7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6649,7 +6649,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
@@ -6665,49 +6665,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20" x14ac:dyDescent="0.3">
-      <c r="B1" s="162" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="162"/>
-      <c r="H1" s="162"/>
-      <c r="I1" s="162"/>
-      <c r="J1" s="162"/>
-      <c r="K1" s="162"/>
-      <c r="L1" s="162"/>
+      <c r="B1" s="158" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
+      <c r="I1" s="158"/>
+      <c r="J1" s="158"/>
+      <c r="K1" s="158"/>
+      <c r="L1" s="158"/>
     </row>
     <row r="2" spans="1:12" ht="20" x14ac:dyDescent="0.4">
-      <c r="B2" s="163" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
+      <c r="B2" s="159" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="159"/>
+      <c r="J2" s="159"/>
+      <c r="K2" s="159"/>
+      <c r="L2" s="159"/>
     </row>
     <row r="3" spans="1:12" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="164" t="s">
+      <c r="B3" s="160" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="164"/>
-      <c r="D3" s="164"/>
-      <c r="E3" s="164"/>
-      <c r="F3" s="164"/>
-      <c r="G3" s="164"/>
-      <c r="H3" s="164"/>
-      <c r="I3" s="164"/>
-      <c r="J3" s="164"/>
-      <c r="K3" s="164"/>
-      <c r="L3" s="164"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="160"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="160"/>
+      <c r="K3" s="160"/>
+      <c r="L3" s="160"/>
     </row>
     <row r="4" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
@@ -6717,193 +6717,216 @@
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="165" t="s">
+      <c r="D4" s="161" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="165"/>
-      <c r="F4" s="165"/>
-      <c r="G4" s="165" t="s">
+      <c r="E4" s="161"/>
+      <c r="F4" s="161"/>
+      <c r="G4" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="165"/>
-      <c r="I4" s="165"/>
-      <c r="J4" s="165"/>
-      <c r="K4" s="165"/>
-      <c r="L4" s="165"/>
+      <c r="H4" s="161"/>
+      <c r="I4" s="161"/>
+      <c r="J4" s="161"/>
+      <c r="K4" s="161"/>
+      <c r="L4" s="161"/>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="166"/>
-      <c r="E5" s="166"/>
-      <c r="F5" s="166"/>
-      <c r="G5" s="166"/>
-      <c r="H5" s="166"/>
-      <c r="I5" s="166"/>
-      <c r="J5" s="166"/>
-      <c r="K5" s="166"/>
-      <c r="L5" s="166"/>
+      <c r="D5" s="157"/>
+      <c r="E5" s="157"/>
+      <c r="F5" s="157"/>
+      <c r="G5" s="157"/>
+      <c r="H5" s="157"/>
+      <c r="I5" s="157"/>
+      <c r="J5" s="157"/>
+      <c r="K5" s="157"/>
+      <c r="L5" s="157"/>
     </row>
     <row r="6" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="160"/>
-      <c r="E6" s="160"/>
-      <c r="F6" s="160"/>
-      <c r="G6" s="161"/>
-      <c r="H6" s="161"/>
-      <c r="I6" s="161"/>
-      <c r="J6" s="161"/>
-      <c r="K6" s="161"/>
-      <c r="L6" s="161"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
+      <c r="H6" s="163"/>
+      <c r="I6" s="163"/>
+      <c r="J6" s="163"/>
+      <c r="K6" s="163"/>
+      <c r="L6" s="163"/>
     </row>
     <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="157"/>
-      <c r="H7" s="157"/>
-      <c r="I7" s="157"/>
-      <c r="J7" s="157"/>
-      <c r="K7" s="157"/>
-      <c r="L7" s="157"/>
+      <c r="D7" s="164"/>
+      <c r="E7" s="164"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="165"/>
+      <c r="H7" s="165"/>
+      <c r="I7" s="165"/>
+      <c r="J7" s="165"/>
+      <c r="K7" s="165"/>
+      <c r="L7" s="165"/>
     </row>
     <row r="8" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="160"/>
-      <c r="E8" s="160"/>
-      <c r="F8" s="160"/>
-      <c r="G8" s="161"/>
-      <c r="H8" s="161"/>
-      <c r="I8" s="161"/>
-      <c r="J8" s="161"/>
-      <c r="K8" s="161"/>
-      <c r="L8" s="161"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
+      <c r="H8" s="163"/>
+      <c r="I8" s="163"/>
+      <c r="J8" s="163"/>
+      <c r="K8" s="163"/>
+      <c r="L8" s="163"/>
     </row>
     <row r="9" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="160"/>
-      <c r="E9" s="160"/>
-      <c r="F9" s="160"/>
-      <c r="G9" s="161"/>
-      <c r="H9" s="161"/>
-      <c r="I9" s="161"/>
-      <c r="J9" s="161"/>
-      <c r="K9" s="161"/>
-      <c r="L9" s="161"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="163"/>
+      <c r="H9" s="163"/>
+      <c r="I9" s="163"/>
+      <c r="J9" s="163"/>
+      <c r="K9" s="163"/>
+      <c r="L9" s="163"/>
     </row>
     <row r="10" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="157"/>
-      <c r="E10" s="157"/>
-      <c r="F10" s="157"/>
-      <c r="G10" s="157"/>
-      <c r="H10" s="157"/>
-      <c r="I10" s="157"/>
-      <c r="J10" s="157"/>
-      <c r="K10" s="157"/>
-      <c r="L10" s="157"/>
+      <c r="D10" s="165"/>
+      <c r="E10" s="165"/>
+      <c r="F10" s="165"/>
+      <c r="G10" s="165"/>
+      <c r="H10" s="165"/>
+      <c r="I10" s="165"/>
+      <c r="J10" s="165"/>
+      <c r="K10" s="165"/>
+      <c r="L10" s="165"/>
     </row>
     <row r="11" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="157"/>
-      <c r="E11" s="157"/>
-      <c r="F11" s="157"/>
-      <c r="G11" s="157"/>
-      <c r="H11" s="157"/>
-      <c r="I11" s="157"/>
-      <c r="J11" s="157"/>
-      <c r="K11" s="157"/>
-      <c r="L11" s="157"/>
+      <c r="D11" s="165"/>
+      <c r="E11" s="165"/>
+      <c r="F11" s="165"/>
+      <c r="G11" s="165"/>
+      <c r="H11" s="165"/>
+      <c r="I11" s="165"/>
+      <c r="J11" s="165"/>
+      <c r="K11" s="165"/>
+      <c r="L11" s="165"/>
     </row>
     <row r="12" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="158"/>
-      <c r="E12" s="158"/>
-      <c r="F12" s="158"/>
-      <c r="G12" s="157"/>
-      <c r="H12" s="157"/>
-      <c r="I12" s="157"/>
-      <c r="J12" s="157"/>
-      <c r="K12" s="157"/>
-      <c r="L12" s="157"/>
+      <c r="D12" s="164"/>
+      <c r="E12" s="164"/>
+      <c r="F12" s="164"/>
+      <c r="G12" s="165"/>
+      <c r="H12" s="165"/>
+      <c r="I12" s="165"/>
+      <c r="J12" s="165"/>
+      <c r="K12" s="165"/>
+      <c r="L12" s="165"/>
     </row>
     <row r="13" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="158"/>
-      <c r="E13" s="158"/>
-      <c r="F13" s="158"/>
-      <c r="G13" s="157"/>
-      <c r="H13" s="157"/>
-      <c r="I13" s="157"/>
-      <c r="J13" s="157"/>
-      <c r="K13" s="157"/>
-      <c r="L13" s="157"/>
+      <c r="D13" s="164"/>
+      <c r="E13" s="164"/>
+      <c r="F13" s="164"/>
+      <c r="G13" s="165"/>
+      <c r="H13" s="165"/>
+      <c r="I13" s="165"/>
+      <c r="J13" s="165"/>
+      <c r="K13" s="165"/>
+      <c r="L13" s="165"/>
     </row>
     <row r="14" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="158"/>
-      <c r="E14" s="158"/>
-      <c r="F14" s="158"/>
-      <c r="G14" s="157"/>
-      <c r="H14" s="157"/>
-      <c r="I14" s="157"/>
-      <c r="J14" s="157"/>
-      <c r="K14" s="157"/>
-      <c r="L14" s="157"/>
+      <c r="D14" s="164"/>
+      <c r="E14" s="164"/>
+      <c r="F14" s="164"/>
+      <c r="G14" s="165"/>
+      <c r="H14" s="165"/>
+      <c r="I14" s="165"/>
+      <c r="J14" s="165"/>
+      <c r="K14" s="165"/>
+      <c r="L14" s="165"/>
     </row>
     <row r="15" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="158"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="157"/>
-      <c r="H15" s="157"/>
-      <c r="I15" s="157"/>
-      <c r="J15" s="157"/>
-      <c r="K15" s="157"/>
-      <c r="L15" s="157"/>
+      <c r="D15" s="164"/>
+      <c r="E15" s="164"/>
+      <c r="F15" s="164"/>
+      <c r="G15" s="165"/>
+      <c r="H15" s="165"/>
+      <c r="I15" s="165"/>
+      <c r="J15" s="165"/>
+      <c r="K15" s="165"/>
+      <c r="L15" s="165"/>
     </row>
     <row r="16" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="D16" s="164"/>
+      <c r="E16" s="164"/>
+      <c r="F16" s="164"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
     </row>
     <row r="17" spans="2:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="B17" s="159" t="s">
+      <c r="B17" s="166" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="159"/>
-      <c r="D17" s="159"/>
-      <c r="E17" s="159"/>
-      <c r="F17" s="159"/>
-      <c r="G17" s="159"/>
-      <c r="H17" s="159"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="159"/>
-      <c r="K17" s="159"/>
-      <c r="L17" s="159"/>
+      <c r="C17" s="166"/>
+      <c r="D17" s="166"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="166"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="166"/>
+      <c r="L17" s="166"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="G16:L16"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:L12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="B17:L17"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:L14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="G15:L15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:L9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:L10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:L6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:L8"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:L5"/>
     <mergeCell ref="B1:L1"/>
@@ -6911,29 +6934,6 @@
     <mergeCell ref="B3:L3"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="G4:L4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:L6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:L8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:L9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:L10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="B17:L17"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:L14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:L15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:L16"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:L12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:L13"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6941,11 +6941,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D10" sqref="D10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6967,17 +6967,17 @@
       <c r="J1" s="11"/>
     </row>
     <row r="2" spans="2:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="186" t="s">
+      <c r="B2" s="169" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="186"/>
-      <c r="H2" s="186"/>
-      <c r="I2" s="186"/>
-      <c r="J2" s="186"/>
+      <c r="C2" s="169"/>
+      <c r="D2" s="169"/>
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+      <c r="G2" s="169"/>
+      <c r="H2" s="169"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
     </row>
     <row r="3" spans="2:10" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
@@ -7018,124 +7018,124 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="187" t="str">
+      <c r="B5" s="170" t="str">
         <f>IF(OR(ISBLANK(D13),D13=0),"Aguardando Aferição da Fábrica de Software",IF(OR(ISBLANK(D20),D20=0),"Aguardando Aferição da Fábrica de Métricas",IF(OR(AND(D24&gt;=0,D24&lt;=H3),AND(D24&lt;=0,D24&gt;=H4)),"Contagem Aprovada","Contagem em Divergência")))</f>
         <v>Aguardando Aferição da Fábrica de Software</v>
       </c>
-      <c r="C5" s="187"/>
-      <c r="D5" s="187"/>
-      <c r="E5" s="187"/>
-      <c r="F5" s="187"/>
-      <c r="G5" s="187"/>
-      <c r="H5" s="187"/>
-      <c r="I5" s="187"/>
-      <c r="J5" s="187"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="170"/>
+      <c r="H5" s="170"/>
+      <c r="I5" s="170"/>
+      <c r="J5" s="170"/>
     </row>
     <row r="6" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="168" t="s">
+      <c r="B6" s="171" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="168"/>
-      <c r="D6" s="168"/>
-      <c r="E6" s="168"/>
-      <c r="F6" s="168"/>
-      <c r="G6" s="168"/>
-      <c r="H6" s="168"/>
-      <c r="I6" s="168"/>
-      <c r="J6" s="168"/>
+      <c r="C6" s="171"/>
+      <c r="D6" s="171"/>
+      <c r="E6" s="171"/>
+      <c r="F6" s="171"/>
+      <c r="G6" s="171"/>
+      <c r="H6" s="171"/>
+      <c r="I6" s="171"/>
+      <c r="J6" s="171"/>
     </row>
     <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="174" t="s">
+      <c r="B7" s="167" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="174"/>
-      <c r="D7" s="184"/>
-      <c r="E7" s="184"/>
-      <c r="F7" s="184"/>
-      <c r="G7" s="184"/>
-      <c r="H7" s="184"/>
-      <c r="I7" s="184"/>
-      <c r="J7" s="184"/>
+      <c r="C7" s="167"/>
+      <c r="D7" s="172"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="172"/>
+      <c r="G7" s="172"/>
+      <c r="H7" s="172"/>
+      <c r="I7" s="172"/>
+      <c r="J7" s="172"/>
     </row>
     <row r="8" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="174" t="s">
+      <c r="B8" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="174"/>
-      <c r="D8" s="188"/>
-      <c r="E8" s="188"/>
-      <c r="F8" s="188"/>
-      <c r="G8" s="188"/>
-      <c r="H8" s="188"/>
-      <c r="I8" s="188"/>
-      <c r="J8" s="188"/>
+      <c r="C8" s="167"/>
+      <c r="D8" s="168"/>
+      <c r="E8" s="168"/>
+      <c r="F8" s="168"/>
+      <c r="G8" s="168"/>
+      <c r="H8" s="168"/>
+      <c r="I8" s="168"/>
+      <c r="J8" s="168"/>
     </row>
     <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="174" t="s">
+      <c r="B9" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="174"/>
-      <c r="D9" s="184"/>
-      <c r="E9" s="184"/>
-      <c r="F9" s="184"/>
-      <c r="G9" s="184"/>
-      <c r="H9" s="184"/>
-      <c r="I9" s="184"/>
-      <c r="J9" s="184"/>
+      <c r="C9" s="167"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="172"/>
+      <c r="G9" s="172"/>
+      <c r="H9" s="172"/>
+      <c r="I9" s="172"/>
+      <c r="J9" s="172"/>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="174" t="s">
+      <c r="B10" s="167" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="174"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="184"/>
-      <c r="F10" s="184"/>
-      <c r="G10" s="184"/>
-      <c r="H10" s="184"/>
-      <c r="I10" s="184"/>
-      <c r="J10" s="184"/>
+      <c r="C10" s="167"/>
+      <c r="D10" s="172"/>
+      <c r="E10" s="172"/>
+      <c r="F10" s="172"/>
+      <c r="G10" s="172"/>
+      <c r="H10" s="172"/>
+      <c r="I10" s="172"/>
+      <c r="J10" s="172"/>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="174" t="s">
+      <c r="B11" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="174"/>
-      <c r="D11" s="185"/>
-      <c r="E11" s="185"/>
-      <c r="F11" s="185"/>
-      <c r="G11" s="185"/>
-      <c r="H11" s="185"/>
-      <c r="I11" s="185"/>
-      <c r="J11" s="185"/>
+      <c r="C11" s="167"/>
+      <c r="D11" s="173"/>
+      <c r="E11" s="173"/>
+      <c r="F11" s="173"/>
+      <c r="G11" s="173"/>
+      <c r="H11" s="173"/>
+      <c r="I11" s="173"/>
+      <c r="J11" s="173"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="174" t="s">
+      <c r="B12" s="167" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="174"/>
-      <c r="D12" s="184"/>
-      <c r="E12" s="184"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="184"/>
-      <c r="I12" s="184"/>
-      <c r="J12" s="184"/>
+      <c r="C12" s="167"/>
+      <c r="D12" s="172"/>
+      <c r="E12" s="172"/>
+      <c r="F12" s="172"/>
+      <c r="G12" s="172"/>
+      <c r="H12" s="172"/>
+      <c r="I12" s="172"/>
+      <c r="J12" s="172"/>
     </row>
     <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="174" t="s">
+      <c r="B13" s="167" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="174"/>
+      <c r="C13" s="167"/>
       <c r="D13" s="16">
         <f>QuadroResumo!G10</f>
         <v>0</v>
       </c>
       <c r="E13" s="17"/>
-      <c r="F13" s="174" t="s">
+      <c r="F13" s="167" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="174"/>
+      <c r="G13" s="167"/>
       <c r="H13" s="16">
         <f>QuadroResumo!H10</f>
         <v>0</v>
@@ -7144,98 +7144,98 @@
       <c r="J13" s="19"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="181" t="s">
+      <c r="B14" s="174" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="181"/>
+      <c r="C14" s="174"/>
       <c r="D14" s="16">
         <f>SUMIF(Funções!D3:D202,"=RT1",Funções!Q3:Q202)+SUMIF(Funções!D3:D202,"=RT2",Funções!Q3:Q202)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="182"/>
-      <c r="F14" s="182"/>
-      <c r="G14" s="182"/>
-      <c r="H14" s="182"/>
-      <c r="I14" s="182"/>
+      <c r="E14" s="175"/>
+      <c r="F14" s="175"/>
+      <c r="G14" s="175"/>
+      <c r="H14" s="175"/>
+      <c r="I14" s="175"/>
       <c r="J14" s="20"/>
     </row>
     <row r="15" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="178"/>
-      <c r="C15" s="178"/>
-      <c r="D15" s="178"/>
-      <c r="E15" s="178"/>
-      <c r="F15" s="178"/>
-      <c r="G15" s="178"/>
-      <c r="H15" s="178"/>
-      <c r="I15" s="178"/>
-      <c r="J15" s="178"/>
+      <c r="B15" s="176"/>
+      <c r="C15" s="176"/>
+      <c r="D15" s="176"/>
+      <c r="E15" s="176"/>
+      <c r="F15" s="176"/>
+      <c r="G15" s="176"/>
+      <c r="H15" s="176"/>
+      <c r="I15" s="176"/>
+      <c r="J15" s="176"/>
     </row>
     <row r="16" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="168" t="s">
+      <c r="B16" s="171" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="168"/>
-      <c r="D16" s="168"/>
-      <c r="E16" s="168"/>
-      <c r="F16" s="168"/>
-      <c r="G16" s="168"/>
-      <c r="H16" s="168"/>
-      <c r="I16" s="168"/>
-      <c r="J16" s="168"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="171"/>
+      <c r="F16" s="171"/>
+      <c r="G16" s="171"/>
+      <c r="H16" s="171"/>
+      <c r="I16" s="171"/>
+      <c r="J16" s="171"/>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="174" t="s">
+      <c r="B17" s="167" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="174"/>
-      <c r="D17" s="183"/>
-      <c r="E17" s="183"/>
-      <c r="F17" s="183"/>
-      <c r="G17" s="183"/>
-      <c r="H17" s="183"/>
-      <c r="I17" s="183"/>
-      <c r="J17" s="183"/>
+      <c r="C17" s="167"/>
+      <c r="D17" s="177"/>
+      <c r="E17" s="177"/>
+      <c r="F17" s="177"/>
+      <c r="G17" s="177"/>
+      <c r="H17" s="177"/>
+      <c r="I17" s="177"/>
+      <c r="J17" s="177"/>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="174" t="s">
+      <c r="B18" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="174"/>
-      <c r="D18" s="183"/>
-      <c r="E18" s="183"/>
-      <c r="F18" s="183"/>
-      <c r="G18" s="183"/>
-      <c r="H18" s="183"/>
-      <c r="I18" s="183"/>
-      <c r="J18" s="183"/>
+      <c r="C18" s="167"/>
+      <c r="D18" s="177"/>
+      <c r="E18" s="177"/>
+      <c r="F18" s="177"/>
+      <c r="G18" s="177"/>
+      <c r="H18" s="177"/>
+      <c r="I18" s="177"/>
+      <c r="J18" s="177"/>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="174" t="s">
+      <c r="B19" s="167" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="174"/>
-      <c r="D19" s="180"/>
-      <c r="E19" s="180"/>
-      <c r="F19" s="180"/>
-      <c r="G19" s="180"/>
-      <c r="H19" s="180"/>
-      <c r="I19" s="180"/>
-      <c r="J19" s="180"/>
+      <c r="C19" s="167"/>
+      <c r="D19" s="178"/>
+      <c r="E19" s="178"/>
+      <c r="F19" s="178"/>
+      <c r="G19" s="178"/>
+      <c r="H19" s="178"/>
+      <c r="I19" s="178"/>
+      <c r="J19" s="178"/>
     </row>
     <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="174" t="s">
+      <c r="B20" s="167" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="174"/>
+      <c r="C20" s="167"/>
       <c r="D20" s="16">
         <f>QuadroResumo!G20</f>
         <v>0</v>
       </c>
       <c r="E20" s="17"/>
-      <c r="F20" s="174" t="s">
+      <c r="F20" s="167" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="174"/>
+      <c r="G20" s="167"/>
       <c r="H20" s="16">
         <f>QuadroResumo!H20</f>
         <v>0</v>
@@ -7244,50 +7244,50 @@
       <c r="J20" s="19"/>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="181" t="s">
+      <c r="B21" s="174" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="181"/>
+      <c r="C21" s="174"/>
       <c r="D21" s="16">
         <f>SUMIF(Funções!V3:V202,"=RT1",Funções!AG3:AG202)+SUMIF(Funções!V3:V202,"=RT2",Funções!AG3:AG202)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="182"/>
-      <c r="F21" s="182"/>
-      <c r="G21" s="182"/>
-      <c r="H21" s="182"/>
-      <c r="I21" s="182"/>
+      <c r="E21" s="175"/>
+      <c r="F21" s="175"/>
+      <c r="G21" s="175"/>
+      <c r="H21" s="175"/>
+      <c r="I21" s="175"/>
       <c r="J21" s="19"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="178"/>
-      <c r="C22" s="178"/>
-      <c r="D22" s="178"/>
-      <c r="E22" s="178"/>
-      <c r="F22" s="178"/>
-      <c r="G22" s="178"/>
-      <c r="H22" s="178"/>
-      <c r="I22" s="178"/>
-      <c r="J22" s="178"/>
+      <c r="B22" s="176"/>
+      <c r="C22" s="176"/>
+      <c r="D22" s="176"/>
+      <c r="E22" s="176"/>
+      <c r="F22" s="176"/>
+      <c r="G22" s="176"/>
+      <c r="H22" s="176"/>
+      <c r="I22" s="176"/>
+      <c r="J22" s="176"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="168" t="s">
+      <c r="B23" s="171" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="168"/>
-      <c r="D23" s="168"/>
-      <c r="E23" s="168"/>
-      <c r="F23" s="168"/>
-      <c r="G23" s="168"/>
-      <c r="H23" s="168"/>
-      <c r="I23" s="168"/>
-      <c r="J23" s="168"/>
+      <c r="C23" s="171"/>
+      <c r="D23" s="171"/>
+      <c r="E23" s="171"/>
+      <c r="F23" s="171"/>
+      <c r="G23" s="171"/>
+      <c r="H23" s="171"/>
+      <c r="I23" s="171"/>
+      <c r="J23" s="171"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="174" t="s">
+      <c r="B24" s="167" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="174"/>
+      <c r="C24" s="167"/>
       <c r="D24" s="21">
         <f>IFERROR(ROUND((D20-D13)/D13,2),0)</f>
         <v>0</v>
@@ -7311,15 +7311,15 @@
       <c r="J25" s="22"/>
     </row>
     <row r="26" spans="2:10" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="174" t="s">
+      <c r="B26" s="167" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="174"/>
-      <c r="D26" s="176">
+      <c r="C26" s="167"/>
+      <c r="D26" s="180">
         <v>19809</v>
       </c>
-      <c r="E26" s="176"/>
-      <c r="F26" s="176"/>
+      <c r="E26" s="180"/>
+      <c r="F26" s="180"/>
       <c r="G26" s="23" t="s">
         <v>27</v>
       </c>
@@ -7333,17 +7333,17 @@
       </c>
     </row>
     <row r="27" spans="2:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="174" t="s">
+      <c r="B27" s="167" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="174"/>
-      <c r="D27" s="176" t="s">
+      <c r="C27" s="167"/>
+      <c r="D27" s="180" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="176"/>
-      <c r="F27" s="176"/>
-      <c r="G27" s="176"/>
-      <c r="H27" s="176"/>
+      <c r="E27" s="180"/>
+      <c r="F27" s="180"/>
+      <c r="G27" s="180"/>
+      <c r="H27" s="180"/>
       <c r="I27" s="23" t="s">
         <v>4</v>
       </c>
@@ -7352,28 +7352,28 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="174" t="s">
+      <c r="B28" s="167" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="174"/>
-      <c r="D28" s="176"/>
-      <c r="E28" s="176"/>
-      <c r="F28" s="176"/>
-      <c r="G28" s="176"/>
-      <c r="H28" s="176"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="180"/>
+      <c r="E28" s="180"/>
+      <c r="F28" s="180"/>
+      <c r="G28" s="180"/>
+      <c r="H28" s="180"/>
       <c r="I28" s="23" t="s">
         <v>4</v>
       </c>
       <c r="J28" s="26"/>
     </row>
     <row r="29" spans="2:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="177" t="s">
+      <c r="B29" s="181" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="174" t="s">
+      <c r="C29" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="174"/>
+      <c r="D29" s="167"/>
       <c r="E29" s="27"/>
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
@@ -7382,11 +7382,11 @@
       <c r="J29" s="28"/>
     </row>
     <row r="30" spans="2:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="177"/>
-      <c r="C30" s="174" t="s">
+      <c r="B30" s="181"/>
+      <c r="C30" s="167" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="174"/>
+      <c r="D30" s="167"/>
       <c r="E30" s="27"/>
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
@@ -7399,11 +7399,11 @@
       </c>
     </row>
     <row r="31" spans="2:10" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="177"/>
-      <c r="C31" s="174" t="s">
+      <c r="B31" s="181"/>
+      <c r="C31" s="167" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="174"/>
+      <c r="D31" s="167"/>
       <c r="E31" s="27"/>
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
@@ -7417,11 +7417,11 @@
       </c>
     </row>
     <row r="32" spans="2:10" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="177"/>
-      <c r="C32" s="174" t="s">
+      <c r="B32" s="181"/>
+      <c r="C32" s="167" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="174"/>
+      <c r="D32" s="167"/>
       <c r="E32" s="27"/>
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
@@ -7435,11 +7435,11 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="177"/>
-      <c r="C33" s="174" t="s">
+      <c r="B33" s="181"/>
+      <c r="C33" s="167" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="174"/>
+      <c r="D33" s="167"/>
       <c r="E33" s="27" t="s">
         <v>42</v>
       </c>
@@ -7455,11 +7455,11 @@
       </c>
     </row>
     <row r="34" spans="2:10" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="177"/>
-      <c r="C34" s="174" t="s">
+      <c r="B34" s="181"/>
+      <c r="C34" s="167" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="174"/>
+      <c r="D34" s="167"/>
       <c r="E34" s="27"/>
       <c r="F34" s="28"/>
       <c r="G34" s="28"/>
@@ -7473,11 +7473,11 @@
       </c>
     </row>
     <row r="35" spans="2:10" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="177"/>
-      <c r="C35" s="174" t="s">
+      <c r="B35" s="181"/>
+      <c r="C35" s="167" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="174"/>
+      <c r="D35" s="167"/>
       <c r="E35" s="27"/>
       <c r="F35" s="28"/>
       <c r="G35" s="28"/>
@@ -7491,11 +7491,11 @@
       </c>
     </row>
     <row r="36" spans="2:10" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="177"/>
-      <c r="C36" s="174" t="s">
+      <c r="B36" s="181"/>
+      <c r="C36" s="167" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="174"/>
+      <c r="D36" s="167"/>
       <c r="E36" s="27"/>
       <c r="F36" s="33" t="s">
         <v>49</v>
@@ -7506,293 +7506,282 @@
       <c r="J36" s="28"/>
     </row>
     <row r="37" spans="2:10" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="175" t="str">
+      <c r="B37" s="182" t="str">
         <f>CONCATENATE(B16," = ",D20," PF")</f>
         <v>Contagem Fábrica de Métricas = 0 PF</v>
       </c>
-      <c r="C37" s="175"/>
-      <c r="D37" s="175"/>
-      <c r="E37" s="175"/>
-      <c r="F37" s="175"/>
-      <c r="G37" s="175"/>
-      <c r="H37" s="175"/>
-      <c r="I37" s="175"/>
-      <c r="J37" s="175"/>
+      <c r="C37" s="182"/>
+      <c r="D37" s="182"/>
+      <c r="E37" s="182"/>
+      <c r="F37" s="182"/>
+      <c r="G37" s="182"/>
+      <c r="H37" s="182"/>
+      <c r="I37" s="182"/>
+      <c r="J37" s="182"/>
     </row>
     <row r="38" spans="2:10" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="175" t="str">
+      <c r="B38" s="182" t="str">
         <f>CONCATENATE(E20,":",H20," PF")</f>
         <v>:0 PF</v>
       </c>
-      <c r="C38" s="175"/>
-      <c r="D38" s="175"/>
-      <c r="E38" s="175"/>
-      <c r="F38" s="175"/>
-      <c r="G38" s="175"/>
-      <c r="H38" s="175"/>
-      <c r="I38" s="175"/>
-      <c r="J38" s="175"/>
+      <c r="C38" s="182"/>
+      <c r="D38" s="182"/>
+      <c r="E38" s="182"/>
+      <c r="F38" s="182"/>
+      <c r="G38" s="182"/>
+      <c r="H38" s="182"/>
+      <c r="I38" s="182"/>
+      <c r="J38" s="182"/>
     </row>
     <row r="39" spans="2:10" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="175" t="str">
+      <c r="B39" s="182" t="str">
         <f>CONCATENATE(B24,":",D24*100,"%")</f>
         <v xml:space="preserve">    % de Divergência:0%</v>
       </c>
-      <c r="C39" s="175"/>
-      <c r="D39" s="175"/>
-      <c r="E39" s="175"/>
-      <c r="F39" s="175"/>
-      <c r="G39" s="175"/>
-      <c r="H39" s="175"/>
-      <c r="I39" s="175"/>
-      <c r="J39" s="175"/>
+      <c r="C39" s="182"/>
+      <c r="D39" s="182"/>
+      <c r="E39" s="182"/>
+      <c r="F39" s="182"/>
+      <c r="G39" s="182"/>
+      <c r="H39" s="182"/>
+      <c r="I39" s="182"/>
+      <c r="J39" s="182"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B40" s="173"/>
-      <c r="C40" s="173"/>
-      <c r="D40" s="173"/>
-      <c r="E40" s="173"/>
-      <c r="F40" s="173"/>
-      <c r="G40" s="173"/>
-      <c r="H40" s="173"/>
-      <c r="I40" s="173"/>
+      <c r="B40" s="183"/>
+      <c r="C40" s="183"/>
+      <c r="D40" s="183"/>
+      <c r="E40" s="183"/>
+      <c r="F40" s="183"/>
+      <c r="G40" s="183"/>
+      <c r="H40" s="183"/>
+      <c r="I40" s="183"/>
       <c r="J40" s="35"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B41" s="168" t="s">
+      <c r="B41" s="171" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="168"/>
-      <c r="D41" s="168"/>
-      <c r="E41" s="168"/>
-      <c r="F41" s="168"/>
-      <c r="G41" s="168"/>
-      <c r="H41" s="168"/>
-      <c r="I41" s="168"/>
-      <c r="J41" s="168"/>
+      <c r="C41" s="171"/>
+      <c r="D41" s="171"/>
+      <c r="E41" s="171"/>
+      <c r="F41" s="171"/>
+      <c r="G41" s="171"/>
+      <c r="H41" s="171"/>
+      <c r="I41" s="171"/>
+      <c r="J41" s="171"/>
     </row>
     <row r="42" spans="2:10" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="167"/>
-      <c r="C42" s="167"/>
-      <c r="D42" s="167"/>
-      <c r="E42" s="167"/>
-      <c r="F42" s="167"/>
-      <c r="G42" s="167"/>
-      <c r="H42" s="167"/>
-      <c r="I42" s="167"/>
+      <c r="B42" s="184"/>
+      <c r="C42" s="184"/>
+      <c r="D42" s="184"/>
+      <c r="E42" s="184"/>
+      <c r="F42" s="184"/>
+      <c r="G42" s="184"/>
+      <c r="H42" s="184"/>
+      <c r="I42" s="184"/>
       <c r="J42" s="36"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B43" s="168" t="s">
+      <c r="B43" s="171" t="s">
         <v>51</v>
       </c>
-      <c r="C43" s="168"/>
-      <c r="D43" s="168"/>
-      <c r="E43" s="168"/>
-      <c r="F43" s="168"/>
-      <c r="G43" s="168"/>
-      <c r="H43" s="168"/>
-      <c r="I43" s="168"/>
-      <c r="J43" s="168"/>
+      <c r="C43" s="171"/>
+      <c r="D43" s="171"/>
+      <c r="E43" s="171"/>
+      <c r="F43" s="171"/>
+      <c r="G43" s="171"/>
+      <c r="H43" s="171"/>
+      <c r="I43" s="171"/>
+      <c r="J43" s="171"/>
     </row>
     <row r="44" spans="2:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="167"/>
-      <c r="C44" s="167"/>
-      <c r="D44" s="167"/>
-      <c r="E44" s="167"/>
-      <c r="F44" s="167"/>
-      <c r="G44" s="167"/>
-      <c r="H44" s="167"/>
-      <c r="I44" s="167"/>
+      <c r="B44" s="184"/>
+      <c r="C44" s="184"/>
+      <c r="D44" s="184"/>
+      <c r="E44" s="184"/>
+      <c r="F44" s="184"/>
+      <c r="G44" s="184"/>
+      <c r="H44" s="184"/>
+      <c r="I44" s="184"/>
       <c r="J44" s="37"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B45" s="168" t="s">
+      <c r="B45" s="171" t="s">
         <v>52</v>
       </c>
-      <c r="C45" s="168"/>
-      <c r="D45" s="168"/>
-      <c r="E45" s="168"/>
-      <c r="F45" s="168"/>
-      <c r="G45" s="168"/>
-      <c r="H45" s="168"/>
-      <c r="I45" s="168"/>
-      <c r="J45" s="168"/>
+      <c r="C45" s="171"/>
+      <c r="D45" s="171"/>
+      <c r="E45" s="171"/>
+      <c r="F45" s="171"/>
+      <c r="G45" s="171"/>
+      <c r="H45" s="171"/>
+      <c r="I45" s="171"/>
+      <c r="J45" s="171"/>
     </row>
     <row r="46" spans="2:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="167"/>
-      <c r="C46" s="167"/>
-      <c r="D46" s="167"/>
-      <c r="E46" s="167"/>
-      <c r="F46" s="167"/>
-      <c r="G46" s="167"/>
-      <c r="H46" s="167"/>
-      <c r="I46" s="167"/>
+      <c r="B46" s="184"/>
+      <c r="C46" s="184"/>
+      <c r="D46" s="184"/>
+      <c r="E46" s="184"/>
+      <c r="F46" s="184"/>
+      <c r="G46" s="184"/>
+      <c r="H46" s="184"/>
+      <c r="I46" s="184"/>
       <c r="J46" s="36"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B47" s="168" t="s">
+      <c r="B47" s="171" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="168"/>
-      <c r="D47" s="168"/>
-      <c r="E47" s="168"/>
-      <c r="F47" s="168"/>
-      <c r="G47" s="168"/>
-      <c r="H47" s="168"/>
-      <c r="I47" s="168"/>
-      <c r="J47" s="168"/>
+      <c r="C47" s="171"/>
+      <c r="D47" s="171"/>
+      <c r="E47" s="171"/>
+      <c r="F47" s="171"/>
+      <c r="G47" s="171"/>
+      <c r="H47" s="171"/>
+      <c r="I47" s="171"/>
+      <c r="J47" s="171"/>
     </row>
     <row r="48" spans="2:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="167"/>
-      <c r="C48" s="167"/>
-      <c r="D48" s="167"/>
-      <c r="E48" s="167"/>
-      <c r="F48" s="167"/>
-      <c r="G48" s="167"/>
-      <c r="H48" s="167"/>
-      <c r="I48" s="167"/>
+      <c r="B48" s="184"/>
+      <c r="C48" s="184"/>
+      <c r="D48" s="184"/>
+      <c r="E48" s="184"/>
+      <c r="F48" s="184"/>
+      <c r="G48" s="184"/>
+      <c r="H48" s="184"/>
+      <c r="I48" s="184"/>
       <c r="J48" s="36"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B49" s="168" t="s">
+      <c r="B49" s="171" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="168"/>
-      <c r="D49" s="168"/>
-      <c r="E49" s="168"/>
-      <c r="F49" s="168"/>
-      <c r="G49" s="168"/>
-      <c r="H49" s="168"/>
-      <c r="I49" s="168"/>
-      <c r="J49" s="168"/>
+      <c r="C49" s="171"/>
+      <c r="D49" s="171"/>
+      <c r="E49" s="171"/>
+      <c r="F49" s="171"/>
+      <c r="G49" s="171"/>
+      <c r="H49" s="171"/>
+      <c r="I49" s="171"/>
+      <c r="J49" s="171"/>
     </row>
     <row r="50" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="170" t="s">
+      <c r="B50" s="185" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="170"/>
-      <c r="D50" s="171"/>
-      <c r="E50" s="171"/>
-      <c r="F50" s="171"/>
-      <c r="G50" s="171"/>
-      <c r="H50" s="171"/>
-      <c r="I50" s="171"/>
-      <c r="J50" s="171"/>
+      <c r="C50" s="185"/>
+      <c r="D50" s="186"/>
+      <c r="E50" s="186"/>
+      <c r="F50" s="186"/>
+      <c r="G50" s="186"/>
+      <c r="H50" s="186"/>
+      <c r="I50" s="186"/>
+      <c r="J50" s="186"/>
     </row>
     <row r="51" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="170" t="s">
+      <c r="B51" s="185" t="s">
         <v>56</v>
       </c>
-      <c r="C51" s="170"/>
-      <c r="D51" s="171"/>
-      <c r="E51" s="171"/>
-      <c r="F51" s="171"/>
-      <c r="G51" s="171"/>
-      <c r="H51" s="171"/>
-      <c r="I51" s="171"/>
-      <c r="J51" s="171"/>
+      <c r="C51" s="185"/>
+      <c r="D51" s="186"/>
+      <c r="E51" s="186"/>
+      <c r="F51" s="186"/>
+      <c r="G51" s="186"/>
+      <c r="H51" s="186"/>
+      <c r="I51" s="186"/>
+      <c r="J51" s="186"/>
     </row>
     <row r="52" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="170" t="s">
+      <c r="B52" s="185" t="s">
         <v>57</v>
       </c>
-      <c r="C52" s="170"/>
-      <c r="D52" s="172"/>
-      <c r="E52" s="172"/>
-      <c r="F52" s="172"/>
-      <c r="G52" s="172"/>
-      <c r="H52" s="172"/>
-      <c r="I52" s="172"/>
-      <c r="J52" s="172"/>
+      <c r="C52" s="185"/>
+      <c r="D52" s="188"/>
+      <c r="E52" s="188"/>
+      <c r="F52" s="188"/>
+      <c r="G52" s="188"/>
+      <c r="H52" s="188"/>
+      <c r="I52" s="188"/>
+      <c r="J52" s="188"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B53" s="168" t="s">
+      <c r="B53" s="171" t="s">
         <v>58</v>
       </c>
-      <c r="C53" s="168"/>
-      <c r="D53" s="168"/>
-      <c r="E53" s="168"/>
-      <c r="F53" s="168"/>
-      <c r="G53" s="168"/>
-      <c r="H53" s="168"/>
-      <c r="I53" s="168"/>
-      <c r="J53" s="168"/>
+      <c r="C53" s="171"/>
+      <c r="D53" s="171"/>
+      <c r="E53" s="171"/>
+      <c r="F53" s="171"/>
+      <c r="G53" s="171"/>
+      <c r="H53" s="171"/>
+      <c r="I53" s="171"/>
+      <c r="J53" s="171"/>
     </row>
     <row r="54" spans="2:10" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="167"/>
-      <c r="C54" s="167"/>
-      <c r="D54" s="167"/>
-      <c r="E54" s="167"/>
-      <c r="F54" s="167"/>
-      <c r="G54" s="167"/>
-      <c r="H54" s="167"/>
-      <c r="I54" s="167"/>
+      <c r="B54" s="184"/>
+      <c r="C54" s="184"/>
+      <c r="D54" s="184"/>
+      <c r="E54" s="184"/>
+      <c r="F54" s="184"/>
+      <c r="G54" s="184"/>
+      <c r="H54" s="184"/>
+      <c r="I54" s="184"/>
       <c r="J54" s="36"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B55" s="168" t="s">
+      <c r="B55" s="171" t="s">
         <v>59</v>
       </c>
-      <c r="C55" s="168"/>
-      <c r="D55" s="168"/>
-      <c r="E55" s="168"/>
-      <c r="F55" s="168"/>
-      <c r="G55" s="168"/>
-      <c r="H55" s="168"/>
-      <c r="I55" s="168"/>
-      <c r="J55" s="168"/>
+      <c r="C55" s="171"/>
+      <c r="D55" s="171"/>
+      <c r="E55" s="171"/>
+      <c r="F55" s="171"/>
+      <c r="G55" s="171"/>
+      <c r="H55" s="171"/>
+      <c r="I55" s="171"/>
+      <c r="J55" s="171"/>
     </row>
     <row r="56" spans="2:10" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="169"/>
-      <c r="C56" s="169"/>
-      <c r="D56" s="169"/>
-      <c r="E56" s="169"/>
-      <c r="F56" s="169"/>
-      <c r="G56" s="169"/>
-      <c r="H56" s="169"/>
-      <c r="I56" s="169"/>
-      <c r="J56" s="169"/>
+      <c r="B56" s="187"/>
+      <c r="C56" s="187"/>
+      <c r="D56" s="187"/>
+      <c r="E56" s="187"/>
+      <c r="F56" s="187"/>
+      <c r="G56" s="187"/>
+      <c r="H56" s="187"/>
+      <c r="I56" s="187"/>
+      <c r="J56" s="187"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:J12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:J18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:J50"/>
+    <mergeCell ref="B54:I54"/>
+    <mergeCell ref="B55:J55"/>
+    <mergeCell ref="B56:J56"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:J51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:J52"/>
+    <mergeCell ref="B53:J53"/>
+    <mergeCell ref="B43:J43"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B46:I46"/>
+    <mergeCell ref="B47:J47"/>
+    <mergeCell ref="B48:I48"/>
+    <mergeCell ref="B49:J49"/>
+    <mergeCell ref="B45:J45"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="B38:J38"/>
+    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="B41:J41"/>
+    <mergeCell ref="B42:I42"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:H27"/>
     <mergeCell ref="B28:C28"/>
@@ -7803,32 +7792,43 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C33:D33"/>
-    <mergeCell ref="B45:J45"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="B38:J38"/>
-    <mergeCell ref="B39:J39"/>
-    <mergeCell ref="B40:I40"/>
-    <mergeCell ref="B41:J41"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="B43:J43"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="B46:I46"/>
-    <mergeCell ref="B47:J47"/>
-    <mergeCell ref="B48:I48"/>
-    <mergeCell ref="B49:J49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:J50"/>
-    <mergeCell ref="B54:I54"/>
-    <mergeCell ref="B55:J55"/>
-    <mergeCell ref="B56:J56"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:J51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:J52"/>
-    <mergeCell ref="B53:J53"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:J18"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:J12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:J7"/>
   </mergeCells>
   <conditionalFormatting sqref="B5">
     <cfRule type="expression" dxfId="268" priority="2">
@@ -7839,7 +7839,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D12:J12" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D12:J12">
       <formula1>"Contagem Estimada,Contagem Detalhada"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7850,7 +7850,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IQ31"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
@@ -8374,11 +8374,11 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I3:I15" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I3:I15">
       <formula1>"OK,NOK"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A3:A15" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A3:A15">
       <formula1>ListaCTIS</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8391,7 +8391,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK371"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="85" workbookViewId="0">
@@ -27338,13 +27338,13 @@
   </mergeCells>
   <conditionalFormatting sqref="Z4:AB4 Z3:AG3 Y5:AB16 T6:T12 S4:S203 AJ102:AM202 AC102:AH102 C3:E3 D102:R102 B203:B371 G3 I3:Q3 S3:T3 AI3:AI203 I98:Q99 G100:Q101 G92:Q97 D106:R202 I103:Q105 D93:H95 I89:Q91 G96:H101 AC4:AG101 AC104:AH202 AC103:AG103 Y30:AB101 T92:T202 T17:T88 AJ98:AJ101 AL3:AM101 C4:Q19 D20:Q88 D92:E101 C20:C202 V17:AB29 V102:AB202">
     <cfRule type="expression" dxfId="266" priority="2">
-      <formula>ISBLANK($T1048380)</formula>
+      <formula>ISBLANK(#REF!)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="265" priority="3">
-      <formula>$T1048380="NOK"</formula>
+      <formula>#REF!="NOK"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="264" priority="4">
-      <formula>$K1048380&lt;&gt;$AA1048380</formula>
+      <formula>#REF!&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3:Y4">
@@ -28316,23 +28316,23 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C3:C203 U3:U203" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C3:C203 U3:U203">
       <formula1>ListaTipos</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T3:T203" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T3:T203">
       <formula1>"OK,NOK"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D3:D202 V3:V202" xr:uid="{00000000-0002-0000-0300-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D3:D202 V3:V202">
       <formula1>ListaCTIS</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" sqref="A10:A202 B617:B1203" xr:uid="{00000000-0002-0000-0300-000003000000}">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" sqref="A10:A202 B617:B1203">
       <formula1>Lista_Estorias</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A3:A9" xr:uid="{00000000-0002-0000-0300-000004000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A3:A9">
       <formula1>Lista_Estorias</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -28345,7 +28345,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L20"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
@@ -28935,7 +28935,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="90" workbookViewId="0">
@@ -29626,12 +29626,12 @@
       <c r="F39" s="139"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E37" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
+  <autoFilter ref="A2:E37"/>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E37" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E37">
       <formula1>"PC,PF,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -29644,7 +29644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C99"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
@@ -30352,7 +30352,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
@@ -30539,7 +30539,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:D4"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">

</xml_diff>